<commit_message>
`ZI`: image processing functions
For now it includes `imfill` and `bwlabeln`
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="548">
   <si>
     <t>Normal function</t>
   </si>
@@ -1662,6 +1662,9 @@
   </si>
   <si>
     <t>sound, soundsc, audiowrite</t>
+  </si>
+  <si>
+    <t>image processing functions</t>
   </si>
 </sst>
 </file>
@@ -2296,8 +2299,8 @@
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F98" sqref="B3:F98"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" customHeight="1"/>
@@ -3005,7 +3008,9 @@
       <c r="E45" s="28" t="s">
         <v>528</v>
       </c>
-      <c r="F45" s="46"/>
+      <c r="F45" s="52" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
       <c r="B46" s="27" t="s">

</xml_diff>

<commit_message>
Added function `YQ` (`rat`: rational approximation)
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="548">
   <si>
     <t>Normal function</t>
   </si>
@@ -2300,7 +2300,7 @@
   <dimension ref="A1:L302"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" customHeight="1"/>
@@ -3127,7 +3127,9 @@
       <c r="D53" s="28" t="s">
         <v>384</v>
       </c>
-      <c r="E53" s="29"/>
+      <c r="E53" s="9" t="s">
+        <v>336</v>
+      </c>
       <c r="F53" s="28" t="s">
         <v>522</v>
       </c>

</xml_diff>

<commit_message>
Defined "do twice" loop
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="549">
   <si>
     <t>Normal function</t>
   </si>
@@ -1665,6 +1665,9 @@
   </si>
   <si>
     <t>image processing functions</t>
+  </si>
+  <si>
+    <t>do twice</t>
   </si>
 </sst>
 </file>
@@ -1855,7 +1858,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1987,6 +1990,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2299,8 +2305,8 @@
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" customHeight="1"/>
@@ -2560,7 +2566,9 @@
       <c r="B16" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="46"/>
+      <c r="C16" s="53" t="s">
+        <v>548</v>
+      </c>
       <c r="D16" s="28" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Function `YF: skipping / non-skipping
`YF`: With two outputs, primes that are not factors are skipped,
together with thier (zero) exponents. If the input contains at least a
negative entry the behaviour is changed: primes are skipped if one
output, and are not skipped if two outputs.
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1589,9 +1589,6 @@
     <t>nonzeros / remove whitespace</t>
   </si>
   <si>
-    <t>polyval / roots / polyfit</t>
-  </si>
-  <si>
     <t>gammaln / betaln</t>
   </si>
   <si>
@@ -1668,6 +1665,9 @@
   </si>
   <si>
     <t>do twice</t>
+  </si>
+  <si>
+    <t>polyval / roots / polyfit / inpolygon</t>
   </si>
 </sst>
 </file>
@@ -2305,8 +2305,8 @@
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" customHeight="1"/>
@@ -2426,7 +2426,7 @@
         <v>517</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>263</v>
@@ -2567,7 +2567,7 @@
         <v>103</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>47</v>
@@ -2777,7 +2777,7 @@
         <v>170</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>213</v>
@@ -2935,7 +2935,7 @@
         <v>128</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D40" s="28" t="s">
         <v>460</v>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="D42" s="38"/>
       <c r="E42" s="28" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F42" s="38"/>
     </row>
@@ -3014,10 +3014,10 @@
         <v>249</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F45" s="52" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
@@ -3082,7 +3082,7 @@
         <v>206</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>203</v>
@@ -3138,8 +3138,8 @@
       <c r="E53" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="F53" s="28" t="s">
-        <v>522</v>
+      <c r="F53" s="52" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="12" customHeight="1">
@@ -3150,13 +3150,13 @@
         <v>41</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>40</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="12" customHeight="1">
@@ -3194,7 +3194,7 @@
         <v>43</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D57" s="28" t="s">
         <v>142</v>
@@ -3292,7 +3292,7 @@
         <v>205</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="12" customHeight="1">
@@ -3322,7 +3322,7 @@
         <v>236</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="12" customHeight="1">
@@ -3364,7 +3364,7 @@
         <v>492</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F69" s="28" t="s">
         <v>516</v>
@@ -3458,10 +3458,10 @@
         <v>73</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="12" customHeight="1">
@@ -3510,7 +3510,7 @@
         <v>136</v>
       </c>
       <c r="F78" s="52" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="12" customHeight="1">
@@ -3536,7 +3536,7 @@
         <v>289</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E80" s="28" t="s">
         <v>265</v>
@@ -3567,13 +3567,13 @@
         <v>66</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D82" s="28" t="s">
+        <v>525</v>
+      </c>
+      <c r="E82" s="28" t="s">
         <v>526</v>
-      </c>
-      <c r="E82" s="28" t="s">
-        <v>527</v>
       </c>
       <c r="F82" s="46"/>
     </row>
@@ -3582,7 +3582,7 @@
         <v>78</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>76</v>
@@ -3659,7 +3659,7 @@
         <v>64</v>
       </c>
       <c r="F87" s="28" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="12" customHeight="1">
@@ -3699,10 +3699,10 @@
       </c>
       <c r="D90" s="46"/>
       <c r="E90" s="28" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F90" s="52" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="12" customHeight="1">
@@ -3798,7 +3798,7 @@
         <v>182</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D97" s="46"/>
       <c r="E97" s="46"/>

</xml_diff>

<commit_message>
`Zv` with two inputs
`Zv` with two inputs: symmetrize array along specified dimension
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1646,9 +1646,6 @@
     <t>clamp (limit to a range)</t>
   </si>
   <si>
-    <t>deblank / symmetric range</t>
-  </si>
-  <si>
     <t>colon (range)</t>
   </si>
   <si>
@@ -1668,6 +1665,9 @@
   </si>
   <si>
     <t>polyval / roots / polyfit / inpolygon</t>
+  </si>
+  <si>
+    <t>symmetric range / array / deblank</t>
   </si>
 </sst>
 </file>
@@ -2305,8 +2305,8 @@
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" customHeight="1"/>
@@ -2426,7 +2426,7 @@
         <v>517</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>263</v>
@@ -2567,7 +2567,7 @@
         <v>103</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>47</v>
@@ -2777,7 +2777,7 @@
         <v>170</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>213</v>
@@ -3017,7 +3017,7 @@
         <v>527</v>
       </c>
       <c r="F45" s="52" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
@@ -3139,7 +3139,7 @@
         <v>336</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="12" customHeight="1">
@@ -3292,7 +3292,7 @@
         <v>205</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="12" customHeight="1">
@@ -3510,7 +3510,7 @@
         <v>136</v>
       </c>
       <c r="F78" s="52" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="12" customHeight="1">
@@ -3702,7 +3702,7 @@
         <v>531</v>
       </c>
       <c r="F90" s="52" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="12" customHeight="1">

</xml_diff>

<commit_message>
`_` with uint8 input normalizes it
by converting to double and dividing by 255
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1238,9 +1238,6 @@
     <t>phi</t>
   </si>
   <si>
-    <t>unary minus</t>
-  </si>
-  <si>
     <t>BinMethod</t>
   </si>
   <si>
@@ -1668,6 +1665,9 @@
   </si>
   <si>
     <t>symmetric range / array / deblank</t>
+  </si>
+  <si>
+    <t>unary minus / normalize uint8</t>
   </si>
 </sst>
 </file>
@@ -2305,8 +2305,8 @@
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F91" sqref="F91"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F98" sqref="B3:F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" customHeight="1"/>
@@ -2385,7 +2385,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>92</v>
@@ -2408,10 +2408,10 @@
         <v>16</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -2423,10 +2423,10 @@
         <v>189</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>263</v>
@@ -2469,13 +2469,13 @@
         <v>37</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>150</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F10" s="28" t="s">
         <v>217</v>
@@ -2490,10 +2490,10 @@
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="28" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="12" customHeight="1">
@@ -2501,16 +2501,16 @@
         <v>109</v>
       </c>
       <c r="C12" s="37" t="s">
+        <v>495</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>493</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>496</v>
       </c>
-      <c r="D12" s="37" t="s">
-        <v>494</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>497</v>
-      </c>
       <c r="F12" s="37" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12" customHeight="1">
@@ -2518,16 +2518,16 @@
         <v>110</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12" customHeight="1">
@@ -2559,7 +2559,7 @@
         <v>191</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12" customHeight="1">
@@ -2567,7 +2567,7 @@
         <v>103</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>47</v>
@@ -2777,7 +2777,7 @@
         <v>170</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>213</v>
@@ -2858,7 +2858,7 @@
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F35" s="28" t="s">
         <v>98</v>
@@ -2872,7 +2872,7 @@
         <v>261</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E36" s="28" t="s">
         <v>87</v>
@@ -2889,7 +2889,7 @@
         <v>7</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E37" s="28" t="s">
         <v>309</v>
@@ -2903,7 +2903,7 @@
         <v>171</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D38" s="28" t="s">
         <v>252</v>
@@ -2924,10 +2924,10 @@
         <v>122</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="12" customHeight="1">
@@ -2935,13 +2935,13 @@
         <v>128</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F40" s="28" t="s">
         <v>18</v>
@@ -2952,10 +2952,10 @@
         <v>172</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="46"/>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="D42" s="38"/>
       <c r="E42" s="28" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F42" s="38"/>
     </row>
@@ -2978,16 +2978,16 @@
         <v>138</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D43" s="28" t="s">
         <v>100</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F43" s="36" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="12" customHeight="1">
@@ -3014,10 +3014,10 @@
         <v>249</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F45" s="52" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
@@ -3051,13 +3051,13 @@
         <v>42</v>
       </c>
       <c r="C48" s="40" t="s">
+        <v>478</v>
+      </c>
+      <c r="D48" s="40" t="s">
         <v>479</v>
       </c>
-      <c r="D48" s="40" t="s">
-        <v>480</v>
-      </c>
       <c r="E48" s="28" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F48" s="46"/>
     </row>
@@ -3066,10 +3066,10 @@
         <v>11</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E49" s="29"/>
       <c r="F49" s="29"/>
@@ -3082,7 +3082,7 @@
         <v>206</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>203</v>
@@ -3116,7 +3116,7 @@
         <v>72</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>402</v>
@@ -3130,7 +3130,7 @@
         <v>121</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D53" s="28" t="s">
         <v>384</v>
@@ -3139,7 +3139,7 @@
         <v>336</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="12" customHeight="1">
@@ -3150,13 +3150,13 @@
         <v>41</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>40</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="12" customHeight="1">
@@ -3173,7 +3173,7 @@
         <v>196</v>
       </c>
       <c r="F55" s="28" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="12" customHeight="1">
@@ -3194,7 +3194,7 @@
         <v>43</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D57" s="28" t="s">
         <v>142</v>
@@ -3218,7 +3218,7 @@
         <v>146</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -3292,7 +3292,7 @@
         <v>205</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="12" customHeight="1">
@@ -3322,7 +3322,7 @@
         <v>236</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="12" customHeight="1">
@@ -3330,7 +3330,7 @@
         <v>93</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>405</v>
+        <v>548</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
@@ -3341,10 +3341,10 @@
         <v>106</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E68" s="28" t="s">
         <v>234</v>
@@ -3361,13 +3361,13 @@
         <v>5</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="12" customHeight="1">
@@ -3388,7 +3388,7 @@
         <v>75</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D71" s="28" t="s">
         <v>3</v>
@@ -3408,7 +3408,7 @@
         <v>126</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E72" s="28" t="s">
         <v>246</v>
@@ -3422,7 +3422,7 @@
         <v>179</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="29"/>
@@ -3452,16 +3452,16 @@
         <v>131</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D75" s="28" t="s">
         <v>73</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="12" customHeight="1">
@@ -3492,7 +3492,7 @@
         <v>233</v>
       </c>
       <c r="E77" s="28" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F77" s="46"/>
     </row>
@@ -3510,7 +3510,7 @@
         <v>136</v>
       </c>
       <c r="F78" s="52" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="12" customHeight="1">
@@ -3518,13 +3518,13 @@
         <v>119</v>
       </c>
       <c r="C79" s="28" t="s">
+        <v>501</v>
+      </c>
+      <c r="D79" s="28" t="s">
         <v>502</v>
       </c>
-      <c r="D79" s="28" t="s">
-        <v>503</v>
-      </c>
       <c r="E79" s="28" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F79" s="46"/>
     </row>
@@ -3536,7 +3536,7 @@
         <v>289</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E80" s="28" t="s">
         <v>265</v>
@@ -3567,13 +3567,13 @@
         <v>66</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D82" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="E82" s="28" t="s">
         <v>525</v>
-      </c>
-      <c r="E82" s="28" t="s">
-        <v>526</v>
       </c>
       <c r="F82" s="46"/>
     </row>
@@ -3582,13 +3582,13 @@
         <v>78</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E83" s="28" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F83" s="28" t="s">
         <v>154</v>
@@ -3602,13 +3602,13 @@
         <v>63</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E84" s="28" t="s">
         <v>65</v>
       </c>
       <c r="F84" s="28" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="85" spans="2:6" ht="12" customHeight="1">
@@ -3616,13 +3616,13 @@
         <v>120</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D85" s="28" t="s">
         <v>390</v>
       </c>
       <c r="E85" s="28" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F85" s="28" t="s">
         <v>88</v>
@@ -3653,13 +3653,13 @@
         <v>60</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E87" s="28" t="s">
         <v>64</v>
       </c>
       <c r="F87" s="28" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="12" customHeight="1">
@@ -3667,7 +3667,7 @@
         <v>129</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D88" s="46"/>
       <c r="E88" s="46"/>
@@ -3699,10 +3699,10 @@
       </c>
       <c r="D90" s="46"/>
       <c r="E90" s="28" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F90" s="52" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="12" customHeight="1">
@@ -3734,7 +3734,7 @@
         <v>147</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D93" s="28" t="s">
         <v>61</v>
@@ -3754,7 +3754,7 @@
         <v>62</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E94" s="29"/>
       <c r="F94" s="29"/>
@@ -3781,13 +3781,13 @@
         <v>38</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D96" s="28" t="s">
         <v>148</v>
       </c>
       <c r="E96" s="36" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F96" s="28" t="s">
         <v>220</v>
@@ -3798,12 +3798,12 @@
         <v>182</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D97" s="46"/>
       <c r="E97" s="46"/>
       <c r="F97" s="28" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="98" spans="2:6" ht="12" customHeight="1">
@@ -4589,7 +4589,7 @@
     </row>
     <row r="43" spans="1:11" s="48" customFormat="1">
       <c r="A43" s="48" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B43" s="48" t="s">
         <v>4</v>
@@ -4600,7 +4600,7 @@
     </row>
     <row r="44" spans="1:11" s="48" customFormat="1">
       <c r="A44" s="48" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B44" s="48" t="s">
         <v>4</v>
@@ -4611,7 +4611,7 @@
     </row>
     <row r="45" spans="1:11" s="48" customFormat="1">
       <c r="A45" s="48" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B45" s="48" t="s">
         <v>4</v>
@@ -4622,7 +4622,7 @@
     </row>
     <row r="46" spans="1:11" s="48" customFormat="1">
       <c r="A46" s="48" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B46" s="48" t="s">
         <v>4</v>
@@ -4633,7 +4633,7 @@
     </row>
     <row r="47" spans="1:11" s="48" customFormat="1">
       <c r="A47" s="48" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B47" s="48" t="s">
         <v>4</v>
@@ -4644,7 +4644,7 @@
     </row>
     <row r="48" spans="1:11" s="48" customFormat="1">
       <c r="A48" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B48" s="48" t="s">
         <v>4</v>
@@ -5031,7 +5031,7 @@
     </row>
     <row r="78" spans="1:11" s="48" customFormat="1">
       <c r="A78" s="48" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B78" s="48" t="s">
         <v>113</v>
@@ -5330,7 +5330,7 @@
     </row>
     <row r="97" spans="1:5" s="48" customFormat="1">
       <c r="A97" s="48" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B97" s="48" t="s">
         <v>143</v>
@@ -5391,7 +5391,7 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C102" s="48" t="s">
         <v>287</v>
@@ -5399,7 +5399,7 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C103" s="48" t="s">
         <v>287</v>
@@ -5407,7 +5407,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C104" s="48" t="s">
         <v>287</v>
@@ -5415,7 +5415,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C105" s="48" t="s">
         <v>287</v>
@@ -5423,7 +5423,7 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C106" s="48" t="s">
         <v>287</v>
@@ -5431,7 +5431,7 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C107" s="48" t="s">
         <v>287</v>
@@ -5439,7 +5439,7 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C108" s="48" t="s">
         <v>287</v>
@@ -5447,183 +5447,183 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B109" t="s">
         <v>143</v>
       </c>
       <c r="C109" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B110" t="s">
         <v>143</v>
       </c>
       <c r="C110" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B111" t="s">
         <v>143</v>
       </c>
       <c r="C111" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B112" t="s">
         <v>143</v>
       </c>
       <c r="C112" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B113" t="s">
         <v>143</v>
       </c>
       <c r="C113" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B114" t="s">
         <v>143</v>
       </c>
       <c r="C114" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B115" t="s">
         <v>143</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B116" t="s">
         <v>143</v>
       </c>
       <c r="C116" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B117" t="s">
         <v>144</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B118" t="s">
         <v>144</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B119" t="s">
         <v>144</v>
       </c>
       <c r="C119" s="48" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B120" t="s">
         <v>144</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B121" t="s">
         <v>144</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B122" t="s">
         <v>144</v>
       </c>
       <c r="C122" s="48" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B123" t="s">
         <v>144</v>
       </c>
       <c r="C123" s="48" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B124" t="s">
         <v>144</v>
       </c>
       <c r="C124" s="48" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B125" t="s">
         <v>144</v>
@@ -5634,194 +5634,194 @@
     </row>
     <row r="126" spans="1:3" s="48" customFormat="1">
       <c r="A126" s="48" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B126" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C126" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="127" spans="1:3" s="48" customFormat="1">
       <c r="A127" s="48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B127" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C127" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="128" spans="1:3" s="48" customFormat="1">
       <c r="A128" s="48" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B128" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C128" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="129" spans="1:3" s="48" customFormat="1">
       <c r="A129" s="48" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B129" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C129" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="130" spans="1:3" s="48" customFormat="1">
       <c r="A130" s="48" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B130" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C130" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="131" spans="1:3" s="48" customFormat="1">
       <c r="A131" s="48" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B131" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C131" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="132" spans="1:3" s="48" customFormat="1">
       <c r="A132" s="48" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B132" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C132" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="133" spans="1:3" s="48" customFormat="1">
       <c r="A133" s="48" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B133" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C133" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="134" spans="1:3" s="48" customFormat="1">
       <c r="A134" s="48" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B134" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C134" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="135" spans="1:3" s="48" customFormat="1">
       <c r="A135" s="48" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B135" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C135" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="136" spans="1:3" s="48" customFormat="1">
       <c r="A136" s="48" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B136" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C136" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="137" spans="1:3" s="48" customFormat="1">
       <c r="A137" s="48" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B137" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C137" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="138" spans="1:3" s="48" customFormat="1">
       <c r="A138" s="48" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B138" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C138" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="139" spans="1:3" s="48" customFormat="1">
       <c r="A139" s="48" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B139" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C139" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="140" spans="1:3" s="48" customFormat="1">
       <c r="A140" s="48" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B140" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C140" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="141" spans="1:3" s="48" customFormat="1">
       <c r="A141" s="48" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B141" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C141" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="142" spans="1:3" s="48" customFormat="1">
       <c r="A142" s="48" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B142" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C142" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="48" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B143" s="48" t="s">
         <v>132</v>
@@ -5829,7 +5829,7 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="48" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B144" s="48" t="s">
         <v>180</v>

</xml_diff>

<commit_message>
Removed `XC` (`histcounts`) and its associated predefined literals (`X7`)
The reasons, as stated in the doc, are as follows. `histc`.  would be a
little redundant; compare histc(x,unique(x)) with 8\#u or SY'; or
compare histc(x,y) with !=s. Besides, MATLAB's histc is deprecated and
replaced by histcounts. The latter works differently; and I preferred
the old histc behaviour: given x = [10 20 30 20 30],
histcounts(x,unique(x)) gives [1 4] whereas histc(x,unique(x)) gives [1
2 2].
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="549">
   <si>
     <t>Normal function</t>
   </si>
@@ -2920,9 +2920,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="46"/>
-      <c r="D39" s="28" t="s">
-        <v>122</v>
-      </c>
+      <c r="D39" s="46"/>
       <c r="E39" s="28" t="s">
         <v>472</v>
       </c>

</xml_diff>

<commit_message>
`YG` can now handle colormaps of type `logical`
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -806,9 +806,6 @@
     <t>separator</t>
   </si>
   <si>
-    <t>push "for" value / "while" index</t>
-  </si>
-  <si>
     <t>fopen, fread, fclose</t>
   </si>
   <si>
@@ -1544,9 +1541,6 @@
     <t>closest values</t>
   </si>
   <si>
-    <t>push "for" index</t>
-  </si>
-  <si>
     <t>conv2(…, 'same')</t>
   </si>
   <si>
@@ -1668,6 +1662,12 @@
   </si>
   <si>
     <t>unary minus / normalize uint8</t>
+  </si>
+  <si>
+    <t>"for" / "do twice" value / "while" index</t>
+  </si>
+  <si>
+    <t>"for" index</t>
   </si>
 </sst>
 </file>
@@ -2385,7 +2385,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>92</v>
@@ -2408,10 +2408,10 @@
         <v>16</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -2423,13 +2423,13 @@
         <v>189</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="12" customHeight="1">
@@ -2441,10 +2441,10 @@
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="12" customHeight="1">
@@ -2458,7 +2458,7 @@
         <v>223</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F9" s="34" t="s">
         <v>222</v>
@@ -2469,13 +2469,13 @@
         <v>37</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>150</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F10" s="28" t="s">
         <v>217</v>
@@ -2486,14 +2486,14 @@
         <v>159</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="28" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="12" customHeight="1">
@@ -2501,16 +2501,16 @@
         <v>109</v>
       </c>
       <c r="C12" s="37" t="s">
+        <v>494</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>492</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>495</v>
       </c>
-      <c r="D12" s="37" t="s">
-        <v>493</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>496</v>
-      </c>
       <c r="F12" s="37" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12" customHeight="1">
@@ -2518,16 +2518,16 @@
         <v>110</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12" customHeight="1">
@@ -2559,7 +2559,7 @@
         <v>191</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12" customHeight="1">
@@ -2567,7 +2567,7 @@
         <v>103</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>47</v>
@@ -2636,10 +2636,10 @@
         <v>185</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F20" s="39"/>
     </row>
@@ -2651,10 +2651,10 @@
         <v>185</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F21" s="39"/>
     </row>
@@ -2666,10 +2666,10 @@
         <v>185</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F22" s="39"/>
     </row>
@@ -2681,10 +2681,10 @@
         <v>185</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F23" s="39"/>
     </row>
@@ -2696,10 +2696,10 @@
         <v>185</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F24" s="39"/>
     </row>
@@ -2711,10 +2711,10 @@
         <v>185</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F25" s="39"/>
     </row>
@@ -2726,10 +2726,10 @@
         <v>185</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F26" s="39"/>
     </row>
@@ -2741,7 +2741,7 @@
         <v>185</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E27" s="39"/>
       <c r="F27" s="39"/>
@@ -2754,7 +2754,7 @@
         <v>185</v>
       </c>
       <c r="D28" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E28" s="39"/>
       <c r="F28" s="39"/>
@@ -2767,7 +2767,7 @@
         <v>185</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="39"/>
@@ -2777,7 +2777,7 @@
         <v>170</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>213</v>
@@ -2858,7 +2858,7 @@
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="28" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F35" s="28" t="s">
         <v>98</v>
@@ -2868,11 +2868,11 @@
       <c r="B36" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="31" t="s">
-        <v>261</v>
-      </c>
-      <c r="D36" s="31" t="s">
-        <v>507</v>
+      <c r="C36" s="53" t="s">
+        <v>547</v>
+      </c>
+      <c r="D36" s="53" t="s">
+        <v>548</v>
       </c>
       <c r="E36" s="28" t="s">
         <v>87</v>
@@ -2889,13 +2889,13 @@
         <v>7</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E37" s="28" t="s">
+        <v>308</v>
+      </c>
+      <c r="F37" s="28" t="s">
         <v>309</v>
-      </c>
-      <c r="F37" s="28" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="12" customHeight="1">
@@ -2903,16 +2903,16 @@
         <v>171</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D38" s="28" t="s">
         <v>252</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="12" customHeight="1">
@@ -2922,10 +2922,10 @@
       <c r="C39" s="46"/>
       <c r="D39" s="46"/>
       <c r="E39" s="28" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="12" customHeight="1">
@@ -2933,13 +2933,13 @@
         <v>128</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F40" s="28" t="s">
         <v>18</v>
@@ -2950,10 +2950,10 @@
         <v>172</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="46"/>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="D42" s="38"/>
       <c r="E42" s="28" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F42" s="38"/>
     </row>
@@ -2976,16 +2976,16 @@
         <v>138</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D43" s="28" t="s">
         <v>100</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F43" s="36" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="12" customHeight="1">
@@ -2993,7 +2993,7 @@
         <v>125</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D44" s="40" t="s">
         <v>250</v>
@@ -3006,16 +3006,16 @@
         <v>97</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D45" s="40" t="s">
         <v>249</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F45" s="52" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
@@ -3023,7 +3023,7 @@
         <v>134</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D46" s="40" t="s">
         <v>248</v>
@@ -3036,7 +3036,7 @@
         <v>143</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D47" s="40" t="s">
         <v>247</v>
@@ -3049,13 +3049,13 @@
         <v>42</v>
       </c>
       <c r="C48" s="40" t="s">
+        <v>477</v>
+      </c>
+      <c r="D48" s="40" t="s">
         <v>478</v>
       </c>
-      <c r="D48" s="40" t="s">
-        <v>479</v>
-      </c>
       <c r="E48" s="28" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F48" s="46"/>
     </row>
@@ -3064,10 +3064,10 @@
         <v>11</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E49" s="29"/>
       <c r="F49" s="29"/>
@@ -3080,7 +3080,7 @@
         <v>206</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>203</v>
@@ -3094,7 +3094,7 @@
         <v>132</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D51" s="28" t="s">
         <v>210</v>
@@ -3114,10 +3114,10 @@
         <v>72</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F52" s="28" t="s">
         <v>244</v>
@@ -3128,16 +3128,16 @@
         <v>121</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="12" customHeight="1">
@@ -3148,13 +3148,13 @@
         <v>41</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>40</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="12" customHeight="1">
@@ -3171,7 +3171,7 @@
         <v>196</v>
       </c>
       <c r="F55" s="28" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="12" customHeight="1">
@@ -3192,7 +3192,7 @@
         <v>43</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D57" s="28" t="s">
         <v>142</v>
@@ -3216,7 +3216,7 @@
         <v>146</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -3268,7 +3268,7 @@
         <v>176</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D63" s="36" t="s">
         <v>13</v>
@@ -3290,7 +3290,7 @@
         <v>205</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="12" customHeight="1">
@@ -3320,7 +3320,7 @@
         <v>236</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="12" customHeight="1">
@@ -3328,7 +3328,7 @@
         <v>93</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
@@ -3339,10 +3339,10 @@
         <v>106</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E68" s="28" t="s">
         <v>234</v>
@@ -3359,13 +3359,13 @@
         <v>5</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="12" customHeight="1">
@@ -3386,7 +3386,7 @@
         <v>75</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D71" s="28" t="s">
         <v>3</v>
@@ -3406,13 +3406,13 @@
         <v>126</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E72" s="28" t="s">
         <v>246</v>
       </c>
       <c r="F72" s="28" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="12" customHeight="1">
@@ -3420,7 +3420,7 @@
         <v>179</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="29"/>
@@ -3450,16 +3450,16 @@
         <v>131</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D75" s="28" t="s">
         <v>73</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="12" customHeight="1">
@@ -3470,7 +3470,7 @@
         <v>201</v>
       </c>
       <c r="D76" s="34" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E76" s="28" t="s">
         <v>239</v>
@@ -3490,7 +3490,7 @@
         <v>233</v>
       </c>
       <c r="E77" s="28" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F77" s="46"/>
     </row>
@@ -3508,7 +3508,7 @@
         <v>136</v>
       </c>
       <c r="F78" s="52" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="12" customHeight="1">
@@ -3516,13 +3516,13 @@
         <v>119</v>
       </c>
       <c r="C79" s="28" t="s">
+        <v>500</v>
+      </c>
+      <c r="D79" s="28" t="s">
         <v>501</v>
       </c>
-      <c r="D79" s="28" t="s">
-        <v>502</v>
-      </c>
       <c r="E79" s="28" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F79" s="46"/>
     </row>
@@ -3531,13 +3531,13 @@
         <v>111</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E80" s="28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F80" s="28" t="s">
         <v>198</v>
@@ -3551,13 +3551,13 @@
         <v>127</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E81" s="28" t="s">
         <v>228</v>
       </c>
       <c r="F81" s="28" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="82" spans="2:6" ht="12" customHeight="1">
@@ -3565,13 +3565,13 @@
         <v>66</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D82" s="28" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E82" s="28" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F82" s="46"/>
     </row>
@@ -3580,13 +3580,13 @@
         <v>78</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E83" s="28" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="F83" s="28" t="s">
         <v>154</v>
@@ -3600,13 +3600,13 @@
         <v>63</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E84" s="28" t="s">
         <v>65</v>
       </c>
       <c r="F84" s="28" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="85" spans="2:6" ht="12" customHeight="1">
@@ -3614,13 +3614,13 @@
         <v>120</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E85" s="28" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F85" s="28" t="s">
         <v>88</v>
@@ -3651,13 +3651,13 @@
         <v>60</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E87" s="28" t="s">
         <v>64</v>
       </c>
       <c r="F87" s="28" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="12" customHeight="1">
@@ -3665,7 +3665,7 @@
         <v>129</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D88" s="46"/>
       <c r="E88" s="46"/>
@@ -3697,10 +3697,10 @@
       </c>
       <c r="D90" s="46"/>
       <c r="E90" s="28" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F90" s="52" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="12" customHeight="1">
@@ -3732,7 +3732,7 @@
         <v>147</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D93" s="28" t="s">
         <v>61</v>
@@ -3752,7 +3752,7 @@
         <v>62</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E94" s="29"/>
       <c r="F94" s="29"/>
@@ -3762,7 +3762,7 @@
         <v>181</v>
       </c>
       <c r="C95" s="35" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D95" s="36" t="s">
         <v>140</v>
@@ -3779,13 +3779,13 @@
         <v>38</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D96" s="28" t="s">
         <v>148</v>
       </c>
       <c r="E96" s="36" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F96" s="28" t="s">
         <v>220</v>
@@ -3796,12 +3796,12 @@
         <v>182</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D97" s="46"/>
       <c r="E97" s="46"/>
       <c r="F97" s="28" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="98" spans="2:6" ht="12" customHeight="1">
@@ -3879,10 +3879,10 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="45" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="50" customFormat="1">
@@ -3898,7 +3898,7 @@
     </row>
     <row r="3" spans="1:11" s="48" customFormat="1">
       <c r="A3" s="48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>8</v>
@@ -3909,7 +3909,7 @@
     </row>
     <row r="4" spans="1:11" s="48" customFormat="1">
       <c r="A4" s="48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>8</v>
@@ -3926,13 +3926,13 @@
         <v>171</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F5" s="48" t="s">
         <v>222</v>
@@ -3952,7 +3952,7 @@
     </row>
     <row r="6" spans="1:11" s="48" customFormat="1">
       <c r="A6" s="48" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B6" s="48" t="s">
         <v>8</v>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="7" spans="1:11" s="48" customFormat="1">
       <c r="A7" s="48" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B7" s="48" t="s">
         <v>8</v>
@@ -3974,7 +3974,7 @@
     </row>
     <row r="8" spans="1:11" s="48" customFormat="1">
       <c r="A8" s="48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B8" s="48" t="s">
         <v>8</v>
@@ -3985,7 +3985,7 @@
     </row>
     <row r="9" spans="1:11" s="48" customFormat="1">
       <c r="A9" s="48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B9" s="48" t="s">
         <v>8</v>
@@ -3996,7 +3996,7 @@
     </row>
     <row r="10" spans="1:11" s="48" customFormat="1">
       <c r="A10" s="48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B10" s="48" t="s">
         <v>8</v>
@@ -4007,7 +4007,7 @@
     </row>
     <row r="11" spans="1:11" s="48" customFormat="1">
       <c r="A11" s="48" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B11" s="48" t="s">
         <v>8</v>
@@ -4018,7 +4018,7 @@
     </row>
     <row r="12" spans="1:11" s="48" customFormat="1">
       <c r="A12" s="48" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B12" s="48" t="s">
         <v>8</v>
@@ -4029,7 +4029,7 @@
     </row>
     <row r="13" spans="1:11" s="48" customFormat="1">
       <c r="A13" s="48" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B13" s="48" t="s">
         <v>8</v>
@@ -4043,7 +4043,7 @@
     </row>
     <row r="14" spans="1:11" s="48" customFormat="1">
       <c r="A14" s="48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B14" s="48" t="s">
         <v>8</v>
@@ -4054,7 +4054,7 @@
     </row>
     <row r="15" spans="1:11" s="48" customFormat="1">
       <c r="A15" s="48" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B15" s="48" t="s">
         <v>8</v>
@@ -4065,7 +4065,7 @@
     </row>
     <row r="16" spans="1:11" s="48" customFormat="1">
       <c r="A16" s="48" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B16" s="48" t="s">
         <v>8</v>
@@ -4082,7 +4082,7 @@
         <v>171</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D17" s="48" t="s">
         <v>222</v>
@@ -4090,18 +4090,18 @@
     </row>
     <row r="18" spans="1:11" s="48" customFormat="1">
       <c r="A18" s="48" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B18" s="48" t="s">
         <v>116</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="48" customFormat="1">
       <c r="A19" s="48" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B19" s="48" t="s">
         <v>116</v>
@@ -4121,13 +4121,13 @@
     </row>
     <row r="20" spans="1:11" s="48" customFormat="1">
       <c r="A20" s="48" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B20" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D20" s="48" t="s">
         <v>222</v>
@@ -4153,13 +4153,13 @@
     </row>
     <row r="21" spans="1:11" s="48" customFormat="1">
       <c r="A21" s="48" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B21" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D21" s="48" t="s">
         <v>222</v>
@@ -4191,7 +4191,7 @@
         <v>171</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D22" s="48" t="s">
         <v>222</v>
@@ -4217,13 +4217,13 @@
     </row>
     <row r="23" spans="1:11" s="48" customFormat="1">
       <c r="A23" s="48" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B23" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D23" s="48" t="s">
         <v>222</v>
@@ -4249,16 +4249,16 @@
     </row>
     <row r="24" spans="1:11" s="48" customFormat="1">
       <c r="A24" s="48" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B24" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E24" s="48" t="s">
         <v>223</v>
@@ -4284,7 +4284,7 @@
         <v>171</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D25" s="48" t="s">
         <v>222</v>
@@ -4295,7 +4295,7 @@
     </row>
     <row r="26" spans="1:11" s="48" customFormat="1">
       <c r="A26" s="48" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B26" s="48" t="s">
         <v>171</v>
@@ -4309,7 +4309,7 @@
     </row>
     <row r="27" spans="1:11" s="48" customFormat="1">
       <c r="A27" s="48" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B27" s="48" t="s">
         <v>116</v>
@@ -4329,7 +4329,7 @@
     </row>
     <row r="28" spans="1:11" s="48" customFormat="1">
       <c r="A28" s="48" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B28" s="48" t="s">
         <v>116</v>
@@ -4340,7 +4340,7 @@
     </row>
     <row r="29" spans="1:11" s="48" customFormat="1">
       <c r="A29" s="48" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B29" s="48" t="s">
         <v>171</v>
@@ -4357,13 +4357,13 @@
     </row>
     <row r="30" spans="1:11" s="48" customFormat="1">
       <c r="A30" s="48" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B30" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D30" s="48" t="s">
         <v>222</v>
@@ -4389,13 +4389,13 @@
     </row>
     <row r="31" spans="1:11" s="48" customFormat="1">
       <c r="A31" s="48" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B31" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D31" s="48" t="s">
         <v>222</v>
@@ -4421,13 +4421,13 @@
     </row>
     <row r="32" spans="1:11" s="48" customFormat="1">
       <c r="A32" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B32" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C32" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D32" s="48" t="s">
         <v>222</v>
@@ -4448,7 +4448,7 @@
         <v>221</v>
       </c>
       <c r="J32" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K32" s="48" t="s">
         <v>27</v>
@@ -4456,13 +4456,13 @@
     </row>
     <row r="33" spans="1:11" s="48" customFormat="1">
       <c r="A33" s="48" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B33" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C33" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D33" s="48" t="s">
         <v>222</v>
@@ -4488,7 +4488,7 @@
     </row>
     <row r="34" spans="1:11" s="48" customFormat="1">
       <c r="A34" s="48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B34" s="48" t="s">
         <v>4</v>
@@ -4499,7 +4499,7 @@
     </row>
     <row r="35" spans="1:11" s="48" customFormat="1">
       <c r="A35" s="48" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B35" s="48" t="s">
         <v>4</v>
@@ -4510,7 +4510,7 @@
     </row>
     <row r="36" spans="1:11" s="48" customFormat="1">
       <c r="A36" s="48" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B36" s="48" t="s">
         <v>4</v>
@@ -4521,7 +4521,7 @@
     </row>
     <row r="37" spans="1:11" s="48" customFormat="1">
       <c r="A37" s="48" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B37" s="48" t="s">
         <v>4</v>
@@ -4532,7 +4532,7 @@
     </row>
     <row r="38" spans="1:11" s="48" customFormat="1">
       <c r="A38" s="48" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B38" s="48" t="s">
         <v>4</v>
@@ -4543,7 +4543,7 @@
     </row>
     <row r="39" spans="1:11" s="48" customFormat="1">
       <c r="A39" s="48" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B39" s="48" t="s">
         <v>4</v>
@@ -4554,7 +4554,7 @@
     </row>
     <row r="40" spans="1:11" s="48" customFormat="1">
       <c r="A40" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B40" s="48" t="s">
         <v>4</v>
@@ -4565,7 +4565,7 @@
     </row>
     <row r="41" spans="1:11" s="48" customFormat="1">
       <c r="A41" s="48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B41" s="48" t="s">
         <v>4</v>
@@ -4576,7 +4576,7 @@
     </row>
     <row r="42" spans="1:11" s="48" customFormat="1">
       <c r="A42" s="48" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B42" s="48" t="s">
         <v>4</v>
@@ -4587,7 +4587,7 @@
     </row>
     <row r="43" spans="1:11" s="48" customFormat="1">
       <c r="A43" s="48" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B43" s="48" t="s">
         <v>4</v>
@@ -4598,7 +4598,7 @@
     </row>
     <row r="44" spans="1:11" s="48" customFormat="1">
       <c r="A44" s="48" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B44" s="48" t="s">
         <v>4</v>
@@ -4609,7 +4609,7 @@
     </row>
     <row r="45" spans="1:11" s="48" customFormat="1">
       <c r="A45" s="48" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B45" s="48" t="s">
         <v>4</v>
@@ -4620,7 +4620,7 @@
     </row>
     <row r="46" spans="1:11" s="48" customFormat="1">
       <c r="A46" s="48" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B46" s="48" t="s">
         <v>4</v>
@@ -4631,7 +4631,7 @@
     </row>
     <row r="47" spans="1:11" s="48" customFormat="1">
       <c r="A47" s="48" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B47" s="48" t="s">
         <v>4</v>
@@ -4642,7 +4642,7 @@
     </row>
     <row r="48" spans="1:11" s="48" customFormat="1">
       <c r="A48" s="48" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B48" s="48" t="s">
         <v>4</v>
@@ -4664,7 +4664,7 @@
     </row>
     <row r="50" spans="1:11" s="48" customFormat="1">
       <c r="A50" s="48" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B50" s="48" t="s">
         <v>128</v>
@@ -4678,7 +4678,7 @@
     </row>
     <row r="51" spans="1:11" s="48" customFormat="1">
       <c r="A51" s="48" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B51" s="48" t="s">
         <v>19</v>
@@ -4689,7 +4689,7 @@
     </row>
     <row r="52" spans="1:11" s="48" customFormat="1">
       <c r="A52" s="48" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B52" s="48" t="s">
         <v>128</v>
@@ -4703,7 +4703,7 @@
     </row>
     <row r="53" spans="1:11" s="48" customFormat="1">
       <c r="A53" s="48" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B53" s="48" t="s">
         <v>128</v>
@@ -4714,7 +4714,7 @@
     </row>
     <row r="54" spans="1:11" s="48" customFormat="1">
       <c r="A54" s="48" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B54" s="48" t="s">
         <v>128</v>
@@ -4723,7 +4723,7 @@
         <v>90</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K54" s="48" t="s">
         <v>27</v>
@@ -4731,7 +4731,7 @@
     </row>
     <row r="55" spans="1:11" s="48" customFormat="1">
       <c r="A55" s="48" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B55" s="48" t="s">
         <v>19</v>
@@ -4742,7 +4742,7 @@
     </row>
     <row r="56" spans="1:11" s="48" customFormat="1">
       <c r="A56" s="48" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B56" s="48" t="s">
         <v>128</v>
@@ -4756,7 +4756,7 @@
     </row>
     <row r="57" spans="1:11" s="48" customFormat="1">
       <c r="A57" s="48" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B57" s="48" t="s">
         <v>128</v>
@@ -4770,7 +4770,7 @@
     </row>
     <row r="58" spans="1:11" s="48" customFormat="1">
       <c r="A58" s="48" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B58" s="48" t="s">
         <v>128</v>
@@ -4781,7 +4781,7 @@
     </row>
     <row r="59" spans="1:11" s="48" customFormat="1">
       <c r="A59" s="48" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B59" s="48" t="s">
         <v>128</v>
@@ -4792,7 +4792,7 @@
     </row>
     <row r="60" spans="1:11" s="48" customFormat="1">
       <c r="A60" s="48" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B60" s="48" t="s">
         <v>172</v>
@@ -4806,7 +4806,7 @@
     </row>
     <row r="61" spans="1:11" s="48" customFormat="1">
       <c r="A61" s="48" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B61" s="48" t="s">
         <v>172</v>
@@ -4817,7 +4817,7 @@
     </row>
     <row r="62" spans="1:11" s="48" customFormat="1">
       <c r="A62" s="48" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B62" s="48" t="s">
         <v>172</v>
@@ -4828,7 +4828,7 @@
     </row>
     <row r="63" spans="1:11" s="48" customFormat="1">
       <c r="A63" s="48" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B63" s="48" t="s">
         <v>172</v>
@@ -4842,18 +4842,18 @@
     </row>
     <row r="64" spans="1:11" s="48" customFormat="1">
       <c r="A64" s="48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B64" s="48" t="s">
         <v>172</v>
       </c>
       <c r="C64" s="48" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="65" spans="1:11" s="48" customFormat="1">
       <c r="A65" s="48" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B65" s="48" t="s">
         <v>172</v>
@@ -4864,18 +4864,18 @@
     </row>
     <row r="66" spans="1:11" s="48" customFormat="1">
       <c r="A66" s="48" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B66" s="48" t="s">
         <v>172</v>
       </c>
       <c r="C66" s="48" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="48" customFormat="1">
       <c r="A67" s="48" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B67" s="48" t="s">
         <v>113</v>
@@ -4889,7 +4889,7 @@
     </row>
     <row r="68" spans="1:11" s="48" customFormat="1">
       <c r="A68" s="48" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B68" s="48" t="s">
         <v>113</v>
@@ -4903,7 +4903,7 @@
     </row>
     <row r="69" spans="1:11" s="48" customFormat="1">
       <c r="A69" s="48" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B69" s="48" t="s">
         <v>113</v>
@@ -4917,7 +4917,7 @@
     </row>
     <row r="70" spans="1:11" s="48" customFormat="1">
       <c r="A70" s="48" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B70" s="48" t="s">
         <v>113</v>
@@ -4931,13 +4931,13 @@
     </row>
     <row r="71" spans="1:11" s="48" customFormat="1">
       <c r="A71" s="48" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B71" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C71" s="48" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D71" s="48" t="s">
         <v>244</v>
@@ -4945,7 +4945,7 @@
     </row>
     <row r="72" spans="1:11" s="48" customFormat="1">
       <c r="A72" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B72" s="48" t="s">
         <v>15</v>
@@ -4956,7 +4956,7 @@
     </row>
     <row r="73" spans="1:11" s="48" customFormat="1">
       <c r="A73" s="48" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B73" s="48" t="s">
         <v>113</v>
@@ -4973,7 +4973,7 @@
     </row>
     <row r="74" spans="1:11" s="48" customFormat="1">
       <c r="A74" s="48" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B74" s="48" t="s">
         <v>113</v>
@@ -4987,7 +4987,7 @@
     </row>
     <row r="75" spans="1:11" s="48" customFormat="1">
       <c r="A75" s="48" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B75" s="48" t="s">
         <v>113</v>
@@ -5001,7 +5001,7 @@
     </row>
     <row r="76" spans="1:11" s="48" customFormat="1">
       <c r="A76" s="48" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B76" s="48" t="s">
         <v>113</v>
@@ -5015,7 +5015,7 @@
     </row>
     <row r="77" spans="1:11" s="48" customFormat="1">
       <c r="A77" s="48" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B77" s="48" t="s">
         <v>113</v>
@@ -5029,7 +5029,7 @@
     </row>
     <row r="78" spans="1:11" s="48" customFormat="1">
       <c r="A78" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B78" s="48" t="s">
         <v>113</v>
@@ -5040,7 +5040,7 @@
     </row>
     <row r="79" spans="1:11" s="48" customFormat="1">
       <c r="A79" s="48" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B79" s="48" t="s">
         <v>113</v>
@@ -5051,7 +5051,7 @@
     </row>
     <row r="80" spans="1:11" s="48" customFormat="1">
       <c r="A80" s="48" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B80" s="48" t="s">
         <v>113</v>
@@ -5065,13 +5065,13 @@
     </row>
     <row r="81" spans="1:11" s="48" customFormat="1">
       <c r="A81" s="48" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B81" s="48" t="s">
         <v>138</v>
       </c>
       <c r="C81" s="48" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D81" s="48" t="s">
         <v>86</v>
@@ -5082,24 +5082,24 @@
     </row>
     <row r="82" spans="1:11" s="48" customFormat="1">
       <c r="A82" s="48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B82" s="48" t="s">
         <v>131</v>
       </c>
       <c r="C82" s="48" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D82" s="48" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E82" s="48" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="83" spans="1:11" s="48" customFormat="1">
       <c r="A83" s="49" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B83" s="48" t="s">
         <v>138</v>
@@ -5111,27 +5111,27 @@
         <v>86</v>
       </c>
       <c r="K83" s="48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="84" spans="1:11" s="48" customFormat="1">
       <c r="A84" s="48" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B84" s="48" t="s">
         <v>138</v>
       </c>
       <c r="C84" s="48" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D84" s="48" t="s">
+        <v>298</v>
+      </c>
+      <c r="E84" s="48" t="s">
         <v>299</v>
       </c>
-      <c r="E84" s="48" t="s">
-        <v>300</v>
-      </c>
       <c r="F84" s="48" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G84" s="48" t="s">
         <v>155</v>
@@ -5139,7 +5139,7 @@
     </row>
     <row r="85" spans="1:11" s="48" customFormat="1">
       <c r="A85" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B85" s="48" t="s">
         <v>131</v>
@@ -5159,13 +5159,13 @@
     </row>
     <row r="86" spans="1:11" s="48" customFormat="1">
       <c r="A86" s="48" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B86" s="48" t="s">
         <v>138</v>
       </c>
       <c r="C86" s="48" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D86" s="48" t="s">
         <v>150</v>
@@ -5174,18 +5174,18 @@
         <v>149</v>
       </c>
       <c r="F86" s="48" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G86" s="48" t="s">
         <v>155</v>
       </c>
       <c r="K86" s="48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="87" spans="1:11" s="48" customFormat="1">
       <c r="A87" s="48" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B87" s="48" t="s">
         <v>138</v>
@@ -5203,12 +5203,12 @@
         <v>155</v>
       </c>
       <c r="K87" s="48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="88" spans="1:11" s="48" customFormat="1">
       <c r="A88" s="49" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B88" s="48" t="s">
         <v>138</v>
@@ -5226,12 +5226,12 @@
         <v>155</v>
       </c>
       <c r="K88" s="48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="89" spans="1:11" s="47" customFormat="1">
       <c r="A89" s="47" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B89" s="47" t="s">
         <v>125</v>
@@ -5248,7 +5248,7 @@
     </row>
     <row r="90" spans="1:11" s="48" customFormat="1">
       <c r="A90" s="48" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B90" s="48" t="s">
         <v>97</v>
@@ -5262,12 +5262,12 @@
         <v>134</v>
       </c>
       <c r="C91" s="48" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="92" spans="1:11" s="48" customFormat="1">
       <c r="A92" s="48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B92" s="48" t="s">
         <v>134</v>
@@ -5281,7 +5281,7 @@
     </row>
     <row r="93" spans="1:11" s="48" customFormat="1">
       <c r="A93" s="49" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B93" s="48" t="s">
         <v>134</v>
@@ -5290,12 +5290,12 @@
         <v>133</v>
       </c>
       <c r="K93" s="48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="94" spans="1:11" s="48" customFormat="1">
       <c r="A94" s="48" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B94" s="48" t="s">
         <v>143</v>
@@ -5306,7 +5306,7 @@
     </row>
     <row r="95" spans="1:11" s="48" customFormat="1">
       <c r="A95" s="48" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B95" s="48" t="s">
         <v>143</v>
@@ -5323,12 +5323,12 @@
         <v>143</v>
       </c>
       <c r="C96" s="50" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="48" customFormat="1">
       <c r="A97" s="48" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B97" s="48" t="s">
         <v>143</v>
@@ -5339,16 +5339,16 @@
     </row>
     <row r="98" spans="1:5" s="48" customFormat="1">
       <c r="A98" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B98" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C98" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D98" s="48" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E98" s="48" t="s">
         <v>63</v>
@@ -5356,272 +5356,272 @@
     </row>
     <row r="99" spans="1:5" s="48" customFormat="1">
       <c r="A99" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B99" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C99" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="48" customFormat="1">
       <c r="A100" s="48" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B100" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C100" s="48" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="48" customFormat="1">
       <c r="A101" s="48" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B101" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C101" s="48" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C102" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C103" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C104" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C105" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C106" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C107" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C108" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B109" t="s">
         <v>143</v>
       </c>
       <c r="C109" s="48" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B110" t="s">
         <v>143</v>
       </c>
       <c r="C110" s="48" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B111" t="s">
         <v>143</v>
       </c>
       <c r="C111" s="48" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B112" t="s">
         <v>143</v>
       </c>
       <c r="C112" s="48" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B113" t="s">
         <v>143</v>
       </c>
       <c r="C113" s="48" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B114" t="s">
         <v>143</v>
       </c>
       <c r="C114" s="48" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B115" t="s">
         <v>143</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B116" t="s">
         <v>143</v>
       </c>
       <c r="C116" s="48" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B117" t="s">
         <v>144</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B118" t="s">
         <v>144</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B119" t="s">
         <v>144</v>
       </c>
       <c r="C119" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B120" t="s">
         <v>144</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B121" t="s">
         <v>144</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B122" t="s">
         <v>144</v>
       </c>
       <c r="C122" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B123" t="s">
         <v>144</v>
       </c>
       <c r="C123" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B124" t="s">
         <v>144</v>
       </c>
       <c r="C124" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B125" t="s">
         <v>144</v>
@@ -5632,194 +5632,194 @@
     </row>
     <row r="126" spans="1:3" s="48" customFormat="1">
       <c r="A126" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B126" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C126" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="127" spans="1:3" s="48" customFormat="1">
       <c r="A127" s="48" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B127" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C127" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="128" spans="1:3" s="48" customFormat="1">
       <c r="A128" s="48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B128" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C128" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="129" spans="1:3" s="48" customFormat="1">
       <c r="A129" s="48" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B129" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C129" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="130" spans="1:3" s="48" customFormat="1">
       <c r="A130" s="48" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B130" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C130" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="131" spans="1:3" s="48" customFormat="1">
       <c r="A131" s="48" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B131" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C131" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="132" spans="1:3" s="48" customFormat="1">
       <c r="A132" s="48" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B132" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C132" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="133" spans="1:3" s="48" customFormat="1">
       <c r="A133" s="48" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B133" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C133" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="134" spans="1:3" s="48" customFormat="1">
       <c r="A134" s="48" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B134" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C134" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="135" spans="1:3" s="48" customFormat="1">
       <c r="A135" s="48" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B135" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C135" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="136" spans="1:3" s="48" customFormat="1">
       <c r="A136" s="48" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B136" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C136" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="137" spans="1:3" s="48" customFormat="1">
       <c r="A137" s="48" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B137" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C137" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="138" spans="1:3" s="48" customFormat="1">
       <c r="A138" s="48" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B138" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C138" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="139" spans="1:3" s="48" customFormat="1">
       <c r="A139" s="48" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B139" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C139" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="140" spans="1:3" s="48" customFormat="1">
       <c r="A140" s="48" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B140" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C140" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="141" spans="1:3" s="48" customFormat="1">
       <c r="A141" s="48" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B141" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C141" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="142" spans="1:3" s="48" customFormat="1">
       <c r="A142" s="48" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B142" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C142" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="48" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B143" s="48" t="s">
         <v>132</v>
@@ -5827,7 +5827,7 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="48" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B144" s="48" t="s">
         <v>180</v>
@@ -5856,7 +5856,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5866,20 +5866,20 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>384</v>
+      </c>
+      <c r="B8" t="s">
         <v>385</v>
-      </c>
-      <c r="B8" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Circular convolution implemented as `Z+` with 3 inputs
Circular convolution (`cconv`) implemented as `Z+` with 3 inputs,
including Octave compatibility
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1541,9 +1541,6 @@
     <t>closest values</t>
   </si>
   <si>
-    <t>conv2(…, 'same')</t>
-  </si>
-  <si>
     <t>( ) refererence ind. with initial :</t>
   </si>
   <si>
@@ -1668,6 +1665,9 @@
   </si>
   <si>
     <t>"for" index</t>
+  </si>
+  <si>
+    <t>conv2(…, 'same') / cconv</t>
   </si>
 </sst>
 </file>
@@ -2306,7 +2306,7 @@
   <dimension ref="A1:L302"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F98" sqref="B3:F98"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" customHeight="1"/>
@@ -2423,10 +2423,10 @@
         <v>189</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>262</v>
@@ -2469,7 +2469,7 @@
         <v>37</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>150</v>
@@ -2527,7 +2527,7 @@
         <v>496</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12" customHeight="1">
@@ -2558,8 +2558,8 @@
       <c r="E15" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="F15" s="28" t="s">
-        <v>506</v>
+      <c r="F15" s="52" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12" customHeight="1">
@@ -2567,7 +2567,7 @@
         <v>103</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>47</v>
@@ -2777,7 +2777,7 @@
         <v>170</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>213</v>
@@ -2858,7 +2858,7 @@
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="28" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F35" s="28" t="s">
         <v>98</v>
@@ -2869,10 +2869,10 @@
         <v>105</v>
       </c>
       <c r="C36" s="53" t="s">
+        <v>546</v>
+      </c>
+      <c r="D36" s="53" t="s">
         <v>547</v>
-      </c>
-      <c r="D36" s="53" t="s">
-        <v>548</v>
       </c>
       <c r="E36" s="28" t="s">
         <v>87</v>
@@ -2933,7 +2933,7 @@
         <v>128</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D40" s="28" t="s">
         <v>458</v>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="D42" s="38"/>
       <c r="E42" s="28" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F42" s="38"/>
     </row>
@@ -2985,7 +2985,7 @@
         <v>498</v>
       </c>
       <c r="F43" s="36" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="12" customHeight="1">
@@ -3012,10 +3012,10 @@
         <v>249</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F45" s="52" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
@@ -3080,7 +3080,7 @@
         <v>206</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>203</v>
@@ -3137,7 +3137,7 @@
         <v>335</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="12" customHeight="1">
@@ -3148,13 +3148,13 @@
         <v>41</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>40</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="12" customHeight="1">
@@ -3192,7 +3192,7 @@
         <v>43</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D57" s="28" t="s">
         <v>142</v>
@@ -3216,7 +3216,7 @@
         <v>146</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -3290,7 +3290,7 @@
         <v>205</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="12" customHeight="1">
@@ -3320,7 +3320,7 @@
         <v>236</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="12" customHeight="1">
@@ -3328,7 +3328,7 @@
         <v>93</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
@@ -3362,10 +3362,10 @@
         <v>490</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="12" customHeight="1">
@@ -3406,7 +3406,7 @@
         <v>126</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E72" s="28" t="s">
         <v>246</v>
@@ -3450,16 +3450,16 @@
         <v>131</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D75" s="28" t="s">
         <v>73</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="12" customHeight="1">
@@ -3508,7 +3508,7 @@
         <v>136</v>
       </c>
       <c r="F78" s="52" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="12" customHeight="1">
@@ -3534,7 +3534,7 @@
         <v>288</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E80" s="28" t="s">
         <v>264</v>
@@ -3565,13 +3565,13 @@
         <v>66</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D82" s="28" t="s">
+        <v>521</v>
+      </c>
+      <c r="E82" s="28" t="s">
         <v>522</v>
-      </c>
-      <c r="E82" s="28" t="s">
-        <v>523</v>
       </c>
       <c r="F82" s="46"/>
     </row>
@@ -3580,13 +3580,13 @@
         <v>78</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E83" s="28" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F83" s="28" t="s">
         <v>154</v>
@@ -3657,7 +3657,7 @@
         <v>64</v>
       </c>
       <c r="F87" s="28" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="12" customHeight="1">
@@ -3697,10 +3697,10 @@
       </c>
       <c r="D90" s="46"/>
       <c r="E90" s="28" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F90" s="52" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="12" customHeight="1">
@@ -3752,7 +3752,7 @@
         <v>62</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E94" s="29"/>
       <c r="F94" s="29"/>
@@ -3779,7 +3779,7 @@
         <v>38</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D96" s="28" t="s">
         <v>148</v>
@@ -3796,7 +3796,7 @@
         <v>182</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D97" s="46"/>
       <c r="E97" s="46"/>

</xml_diff>

<commit_message>
`Zc` with single, non-cell input
`Zc` with a single, non-cell input replaces nonzeros by 35 (ASCII for
'#') and converts to char
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -737,9 +737,6 @@
     <t>mod(…-1)+1</t>
   </si>
   <si>
-    <t>strjoin</t>
-  </si>
-  <si>
     <t>hankel</t>
   </si>
   <si>
@@ -1668,6 +1665,9 @@
   </si>
   <si>
     <t>conv2(…, 'same') / cconv</t>
+  </si>
+  <si>
+    <t>strjoin / convert to '#' and char 0</t>
   </si>
 </sst>
 </file>
@@ -2306,7 +2306,7 @@
   <dimension ref="A1:L302"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F98" sqref="B3:F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" customHeight="1"/>
@@ -2332,16 +2332,16 @@
         <v>0</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="12" customHeight="1">
@@ -2356,16 +2356,16 @@
         <v>175</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I3" s="21" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>257</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>258</v>
       </c>
       <c r="L3" s="23" t="s">
         <v>185</v>
@@ -2374,7 +2374,7 @@
     <row r="4" spans="1:12" ht="12" customHeight="1">
       <c r="B4" s="24"/>
       <c r="C4" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -2385,7 +2385,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>92</v>
@@ -2408,10 +2408,10 @@
         <v>16</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -2423,13 +2423,13 @@
         <v>189</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="12" customHeight="1">
@@ -2441,10 +2441,10 @@
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="12" customHeight="1">
@@ -2458,7 +2458,7 @@
         <v>223</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F9" s="34" t="s">
         <v>222</v>
@@ -2469,13 +2469,13 @@
         <v>37</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>150</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F10" s="28" t="s">
         <v>217</v>
@@ -2486,14 +2486,14 @@
         <v>159</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="28" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="12" customHeight="1">
@@ -2501,16 +2501,16 @@
         <v>109</v>
       </c>
       <c r="C12" s="37" t="s">
+        <v>493</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>491</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>494</v>
       </c>
-      <c r="D12" s="37" t="s">
-        <v>492</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>495</v>
-      </c>
       <c r="F12" s="37" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12" customHeight="1">
@@ -2518,16 +2518,16 @@
         <v>110</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12" customHeight="1">
@@ -2544,7 +2544,7 @@
         <v>39</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="12" customHeight="1">
@@ -2559,7 +2559,7 @@
         <v>191</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12" customHeight="1">
@@ -2567,7 +2567,7 @@
         <v>103</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>47</v>
@@ -2636,10 +2636,10 @@
         <v>185</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F20" s="39"/>
     </row>
@@ -2651,10 +2651,10 @@
         <v>185</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F21" s="39"/>
     </row>
@@ -2666,10 +2666,10 @@
         <v>185</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F22" s="39"/>
     </row>
@@ -2681,10 +2681,10 @@
         <v>185</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F23" s="39"/>
     </row>
@@ -2696,10 +2696,10 @@
         <v>185</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F24" s="39"/>
     </row>
@@ -2711,10 +2711,10 @@
         <v>185</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F25" s="39"/>
     </row>
@@ -2726,10 +2726,10 @@
         <v>185</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F26" s="39"/>
     </row>
@@ -2741,7 +2741,7 @@
         <v>185</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E27" s="39"/>
       <c r="F27" s="39"/>
@@ -2754,7 +2754,7 @@
         <v>185</v>
       </c>
       <c r="D28" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E28" s="39"/>
       <c r="F28" s="39"/>
@@ -2767,7 +2767,7 @@
         <v>185</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="39"/>
@@ -2777,7 +2777,7 @@
         <v>170</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>213</v>
@@ -2858,7 +2858,7 @@
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F35" s="28" t="s">
         <v>98</v>
@@ -2869,10 +2869,10 @@
         <v>105</v>
       </c>
       <c r="C36" s="53" t="s">
+        <v>545</v>
+      </c>
+      <c r="D36" s="53" t="s">
         <v>546</v>
-      </c>
-      <c r="D36" s="53" t="s">
-        <v>547</v>
       </c>
       <c r="E36" s="28" t="s">
         <v>87</v>
@@ -2889,13 +2889,13 @@
         <v>7</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E37" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="F37" s="28" t="s">
         <v>308</v>
-      </c>
-      <c r="F37" s="28" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="12" customHeight="1">
@@ -2903,16 +2903,16 @@
         <v>171</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D38" s="28" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="12" customHeight="1">
@@ -2922,10 +2922,10 @@
       <c r="C39" s="46"/>
       <c r="D39" s="46"/>
       <c r="E39" s="28" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="12" customHeight="1">
@@ -2933,13 +2933,13 @@
         <v>128</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F40" s="28" t="s">
         <v>18</v>
@@ -2950,10 +2950,10 @@
         <v>172</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="46"/>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="D42" s="38"/>
       <c r="E42" s="28" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F42" s="38"/>
     </row>
@@ -2976,16 +2976,16 @@
         <v>138</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D43" s="28" t="s">
         <v>100</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F43" s="36" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="12" customHeight="1">
@@ -2993,10 +2993,10 @@
         <v>125</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E44" s="46"/>
       <c r="F44" s="46"/>
@@ -3006,16 +3006,16 @@
         <v>97</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F45" s="52" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
@@ -3023,10 +3023,10 @@
         <v>134</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E46" s="46"/>
       <c r="F46" s="46"/>
@@ -3036,10 +3036,10 @@
         <v>143</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D47" s="40" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E47" s="46"/>
       <c r="F47" s="46"/>
@@ -3049,13 +3049,13 @@
         <v>42</v>
       </c>
       <c r="C48" s="40" t="s">
+        <v>476</v>
+      </c>
+      <c r="D48" s="40" t="s">
         <v>477</v>
       </c>
-      <c r="D48" s="40" t="s">
-        <v>478</v>
-      </c>
       <c r="E48" s="28" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F48" s="46"/>
     </row>
@@ -3064,10 +3064,10 @@
         <v>11</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E49" s="29"/>
       <c r="F49" s="29"/>
@@ -3080,7 +3080,7 @@
         <v>206</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>203</v>
@@ -3094,7 +3094,7 @@
         <v>132</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D51" s="28" t="s">
         <v>210</v>
@@ -3114,13 +3114,13 @@
         <v>72</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="12" customHeight="1">
@@ -3128,16 +3128,16 @@
         <v>121</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="12" customHeight="1">
@@ -3148,13 +3148,13 @@
         <v>41</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>40</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="12" customHeight="1">
@@ -3171,7 +3171,7 @@
         <v>196</v>
       </c>
       <c r="F55" s="28" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="12" customHeight="1">
@@ -3183,7 +3183,7 @@
       </c>
       <c r="D56" s="46"/>
       <c r="E56" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F56" s="38"/>
     </row>
@@ -3192,7 +3192,7 @@
         <v>43</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D57" s="28" t="s">
         <v>142</v>
@@ -3216,7 +3216,7 @@
         <v>146</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -3268,7 +3268,7 @@
         <v>176</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D63" s="36" t="s">
         <v>13</v>
@@ -3290,7 +3290,7 @@
         <v>205</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="12" customHeight="1">
@@ -3298,7 +3298,7 @@
         <v>178</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D65" s="28" t="s">
         <v>12</v>
@@ -3320,7 +3320,7 @@
         <v>236</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="12" customHeight="1">
@@ -3328,7 +3328,7 @@
         <v>93</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
@@ -3339,10 +3339,10 @@
         <v>106</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E68" s="28" t="s">
         <v>234</v>
@@ -3359,13 +3359,13 @@
         <v>5</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="12" customHeight="1">
@@ -3386,7 +3386,7 @@
         <v>75</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D71" s="28" t="s">
         <v>3</v>
@@ -3394,8 +3394,8 @@
       <c r="E71" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="F71" s="28" t="s">
-        <v>238</v>
+      <c r="F71" s="52" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="12" customHeight="1">
@@ -3406,13 +3406,13 @@
         <v>126</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E72" s="28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F72" s="28" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="12" customHeight="1">
@@ -3420,7 +3420,7 @@
         <v>179</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="29"/>
@@ -3450,16 +3450,16 @@
         <v>131</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D75" s="28" t="s">
         <v>73</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="12" customHeight="1">
@@ -3470,13 +3470,13 @@
         <v>201</v>
       </c>
       <c r="D76" s="34" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E76" s="28" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F76" s="28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="12" customHeight="1">
@@ -3490,7 +3490,7 @@
         <v>233</v>
       </c>
       <c r="E77" s="28" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F77" s="46"/>
     </row>
@@ -3499,7 +3499,7 @@
         <v>180</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D78" s="28" t="s">
         <v>135</v>
@@ -3508,7 +3508,7 @@
         <v>136</v>
       </c>
       <c r="F78" s="52" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="12" customHeight="1">
@@ -3516,13 +3516,13 @@
         <v>119</v>
       </c>
       <c r="C79" s="28" t="s">
+        <v>499</v>
+      </c>
+      <c r="D79" s="28" t="s">
         <v>500</v>
       </c>
-      <c r="D79" s="28" t="s">
-        <v>501</v>
-      </c>
       <c r="E79" s="28" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F79" s="46"/>
     </row>
@@ -3531,13 +3531,13 @@
         <v>111</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E80" s="28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F80" s="28" t="s">
         <v>198</v>
@@ -3551,13 +3551,13 @@
         <v>127</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E81" s="28" t="s">
         <v>228</v>
       </c>
       <c r="F81" s="28" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="82" spans="2:6" ht="12" customHeight="1">
@@ -3565,13 +3565,13 @@
         <v>66</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D82" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="E82" s="28" t="s">
         <v>521</v>
-      </c>
-      <c r="E82" s="28" t="s">
-        <v>522</v>
       </c>
       <c r="F82" s="46"/>
     </row>
@@ -3580,13 +3580,13 @@
         <v>78</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E83" s="28" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F83" s="28" t="s">
         <v>154</v>
@@ -3600,13 +3600,13 @@
         <v>63</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E84" s="28" t="s">
         <v>65</v>
       </c>
       <c r="F84" s="28" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="85" spans="2:6" ht="12" customHeight="1">
@@ -3614,13 +3614,13 @@
         <v>120</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E85" s="28" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F85" s="28" t="s">
         <v>88</v>
@@ -3651,13 +3651,13 @@
         <v>60</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E87" s="28" t="s">
         <v>64</v>
       </c>
       <c r="F87" s="28" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="12" customHeight="1">
@@ -3665,7 +3665,7 @@
         <v>129</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D88" s="46"/>
       <c r="E88" s="46"/>
@@ -3697,10 +3697,10 @@
       </c>
       <c r="D90" s="46"/>
       <c r="E90" s="28" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F90" s="52" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="12" customHeight="1">
@@ -3732,7 +3732,7 @@
         <v>147</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D93" s="28" t="s">
         <v>61</v>
@@ -3752,7 +3752,7 @@
         <v>62</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E94" s="29"/>
       <c r="F94" s="29"/>
@@ -3762,7 +3762,7 @@
         <v>181</v>
       </c>
       <c r="C95" s="35" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D95" s="36" t="s">
         <v>140</v>
@@ -3771,7 +3771,7 @@
         <v>139</v>
       </c>
       <c r="F95" s="36" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="96" spans="2:6" ht="12" customHeight="1">
@@ -3779,13 +3779,13 @@
         <v>38</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D96" s="28" t="s">
         <v>148</v>
       </c>
       <c r="E96" s="36" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F96" s="28" t="s">
         <v>220</v>
@@ -3796,12 +3796,12 @@
         <v>182</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D97" s="46"/>
       <c r="E97" s="46"/>
       <c r="F97" s="28" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="98" spans="2:6" ht="12" customHeight="1">
@@ -3879,10 +3879,10 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="50" customFormat="1">
@@ -3898,7 +3898,7 @@
     </row>
     <row r="3" spans="1:11" s="48" customFormat="1">
       <c r="A3" s="48" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>8</v>
@@ -3909,7 +3909,7 @@
     </row>
     <row r="4" spans="1:11" s="48" customFormat="1">
       <c r="A4" s="48" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>8</v>
@@ -3926,13 +3926,13 @@
         <v>171</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F5" s="48" t="s">
         <v>222</v>
@@ -3952,7 +3952,7 @@
     </row>
     <row r="6" spans="1:11" s="48" customFormat="1">
       <c r="A6" s="48" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B6" s="48" t="s">
         <v>8</v>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="7" spans="1:11" s="48" customFormat="1">
       <c r="A7" s="48" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B7" s="48" t="s">
         <v>8</v>
@@ -3974,7 +3974,7 @@
     </row>
     <row r="8" spans="1:11" s="48" customFormat="1">
       <c r="A8" s="48" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B8" s="48" t="s">
         <v>8</v>
@@ -3985,7 +3985,7 @@
     </row>
     <row r="9" spans="1:11" s="48" customFormat="1">
       <c r="A9" s="48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B9" s="48" t="s">
         <v>8</v>
@@ -3996,7 +3996,7 @@
     </row>
     <row r="10" spans="1:11" s="48" customFormat="1">
       <c r="A10" s="48" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B10" s="48" t="s">
         <v>8</v>
@@ -4007,7 +4007,7 @@
     </row>
     <row r="11" spans="1:11" s="48" customFormat="1">
       <c r="A11" s="48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B11" s="48" t="s">
         <v>8</v>
@@ -4018,7 +4018,7 @@
     </row>
     <row r="12" spans="1:11" s="48" customFormat="1">
       <c r="A12" s="48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B12" s="48" t="s">
         <v>8</v>
@@ -4029,7 +4029,7 @@
     </row>
     <row r="13" spans="1:11" s="48" customFormat="1">
       <c r="A13" s="48" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B13" s="48" t="s">
         <v>8</v>
@@ -4043,7 +4043,7 @@
     </row>
     <row r="14" spans="1:11" s="48" customFormat="1">
       <c r="A14" s="48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B14" s="48" t="s">
         <v>8</v>
@@ -4054,7 +4054,7 @@
     </row>
     <row r="15" spans="1:11" s="48" customFormat="1">
       <c r="A15" s="48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B15" s="48" t="s">
         <v>8</v>
@@ -4065,7 +4065,7 @@
     </row>
     <row r="16" spans="1:11" s="48" customFormat="1">
       <c r="A16" s="48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B16" s="48" t="s">
         <v>8</v>
@@ -4082,7 +4082,7 @@
         <v>171</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D17" s="48" t="s">
         <v>222</v>
@@ -4090,18 +4090,18 @@
     </row>
     <row r="18" spans="1:11" s="48" customFormat="1">
       <c r="A18" s="48" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B18" s="48" t="s">
         <v>116</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="48" customFormat="1">
       <c r="A19" s="48" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B19" s="48" t="s">
         <v>116</v>
@@ -4121,13 +4121,13 @@
     </row>
     <row r="20" spans="1:11" s="48" customFormat="1">
       <c r="A20" s="48" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B20" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D20" s="48" t="s">
         <v>222</v>
@@ -4153,13 +4153,13 @@
     </row>
     <row r="21" spans="1:11" s="48" customFormat="1">
       <c r="A21" s="48" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B21" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D21" s="48" t="s">
         <v>222</v>
@@ -4191,7 +4191,7 @@
         <v>171</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D22" s="48" t="s">
         <v>222</v>
@@ -4217,13 +4217,13 @@
     </row>
     <row r="23" spans="1:11" s="48" customFormat="1">
       <c r="A23" s="48" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B23" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D23" s="48" t="s">
         <v>222</v>
@@ -4249,16 +4249,16 @@
     </row>
     <row r="24" spans="1:11" s="48" customFormat="1">
       <c r="A24" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B24" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E24" s="48" t="s">
         <v>223</v>
@@ -4284,7 +4284,7 @@
         <v>171</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D25" s="48" t="s">
         <v>222</v>
@@ -4295,7 +4295,7 @@
     </row>
     <row r="26" spans="1:11" s="48" customFormat="1">
       <c r="A26" s="48" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B26" s="48" t="s">
         <v>171</v>
@@ -4309,7 +4309,7 @@
     </row>
     <row r="27" spans="1:11" s="48" customFormat="1">
       <c r="A27" s="48" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B27" s="48" t="s">
         <v>116</v>
@@ -4329,7 +4329,7 @@
     </row>
     <row r="28" spans="1:11" s="48" customFormat="1">
       <c r="A28" s="48" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B28" s="48" t="s">
         <v>116</v>
@@ -4340,7 +4340,7 @@
     </row>
     <row r="29" spans="1:11" s="48" customFormat="1">
       <c r="A29" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B29" s="48" t="s">
         <v>171</v>
@@ -4357,13 +4357,13 @@
     </row>
     <row r="30" spans="1:11" s="48" customFormat="1">
       <c r="A30" s="48" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B30" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D30" s="48" t="s">
         <v>222</v>
@@ -4389,13 +4389,13 @@
     </row>
     <row r="31" spans="1:11" s="48" customFormat="1">
       <c r="A31" s="48" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B31" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D31" s="48" t="s">
         <v>222</v>
@@ -4421,13 +4421,13 @@
     </row>
     <row r="32" spans="1:11" s="48" customFormat="1">
       <c r="A32" s="48" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B32" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C32" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D32" s="48" t="s">
         <v>222</v>
@@ -4448,7 +4448,7 @@
         <v>221</v>
       </c>
       <c r="J32" s="48" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K32" s="48" t="s">
         <v>27</v>
@@ -4456,13 +4456,13 @@
     </row>
     <row r="33" spans="1:11" s="48" customFormat="1">
       <c r="A33" s="48" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B33" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C33" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D33" s="48" t="s">
         <v>222</v>
@@ -4488,7 +4488,7 @@
     </row>
     <row r="34" spans="1:11" s="48" customFormat="1">
       <c r="A34" s="48" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B34" s="48" t="s">
         <v>4</v>
@@ -4499,7 +4499,7 @@
     </row>
     <row r="35" spans="1:11" s="48" customFormat="1">
       <c r="A35" s="48" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B35" s="48" t="s">
         <v>4</v>
@@ -4510,7 +4510,7 @@
     </row>
     <row r="36" spans="1:11" s="48" customFormat="1">
       <c r="A36" s="48" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B36" s="48" t="s">
         <v>4</v>
@@ -4521,7 +4521,7 @@
     </row>
     <row r="37" spans="1:11" s="48" customFormat="1">
       <c r="A37" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B37" s="48" t="s">
         <v>4</v>
@@ -4532,7 +4532,7 @@
     </row>
     <row r="38" spans="1:11" s="48" customFormat="1">
       <c r="A38" s="48" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B38" s="48" t="s">
         <v>4</v>
@@ -4543,7 +4543,7 @@
     </row>
     <row r="39" spans="1:11" s="48" customFormat="1">
       <c r="A39" s="48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B39" s="48" t="s">
         <v>4</v>
@@ -4554,7 +4554,7 @@
     </row>
     <row r="40" spans="1:11" s="48" customFormat="1">
       <c r="A40" s="48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B40" s="48" t="s">
         <v>4</v>
@@ -4565,7 +4565,7 @@
     </row>
     <row r="41" spans="1:11" s="48" customFormat="1">
       <c r="A41" s="48" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B41" s="48" t="s">
         <v>4</v>
@@ -4576,7 +4576,7 @@
     </row>
     <row r="42" spans="1:11" s="48" customFormat="1">
       <c r="A42" s="48" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B42" s="48" t="s">
         <v>4</v>
@@ -4587,7 +4587,7 @@
     </row>
     <row r="43" spans="1:11" s="48" customFormat="1">
       <c r="A43" s="48" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B43" s="48" t="s">
         <v>4</v>
@@ -4598,7 +4598,7 @@
     </row>
     <row r="44" spans="1:11" s="48" customFormat="1">
       <c r="A44" s="48" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B44" s="48" t="s">
         <v>4</v>
@@ -4609,7 +4609,7 @@
     </row>
     <row r="45" spans="1:11" s="48" customFormat="1">
       <c r="A45" s="48" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B45" s="48" t="s">
         <v>4</v>
@@ -4620,7 +4620,7 @@
     </row>
     <row r="46" spans="1:11" s="48" customFormat="1">
       <c r="A46" s="48" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B46" s="48" t="s">
         <v>4</v>
@@ -4631,7 +4631,7 @@
     </row>
     <row r="47" spans="1:11" s="48" customFormat="1">
       <c r="A47" s="48" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B47" s="48" t="s">
         <v>4</v>
@@ -4642,7 +4642,7 @@
     </row>
     <row r="48" spans="1:11" s="48" customFormat="1">
       <c r="A48" s="48" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B48" s="48" t="s">
         <v>4</v>
@@ -4664,7 +4664,7 @@
     </row>
     <row r="50" spans="1:11" s="48" customFormat="1">
       <c r="A50" s="48" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B50" s="48" t="s">
         <v>128</v>
@@ -4678,7 +4678,7 @@
     </row>
     <row r="51" spans="1:11" s="48" customFormat="1">
       <c r="A51" s="48" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B51" s="48" t="s">
         <v>19</v>
@@ -4689,7 +4689,7 @@
     </row>
     <row r="52" spans="1:11" s="48" customFormat="1">
       <c r="A52" s="48" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B52" s="48" t="s">
         <v>128</v>
@@ -4703,7 +4703,7 @@
     </row>
     <row r="53" spans="1:11" s="48" customFormat="1">
       <c r="A53" s="48" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B53" s="48" t="s">
         <v>128</v>
@@ -4714,7 +4714,7 @@
     </row>
     <row r="54" spans="1:11" s="48" customFormat="1">
       <c r="A54" s="48" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B54" s="48" t="s">
         <v>128</v>
@@ -4723,7 +4723,7 @@
         <v>90</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K54" s="48" t="s">
         <v>27</v>
@@ -4731,7 +4731,7 @@
     </row>
     <row r="55" spans="1:11" s="48" customFormat="1">
       <c r="A55" s="48" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B55" s="48" t="s">
         <v>19</v>
@@ -4742,7 +4742,7 @@
     </row>
     <row r="56" spans="1:11" s="48" customFormat="1">
       <c r="A56" s="48" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B56" s="48" t="s">
         <v>128</v>
@@ -4756,7 +4756,7 @@
     </row>
     <row r="57" spans="1:11" s="48" customFormat="1">
       <c r="A57" s="48" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B57" s="48" t="s">
         <v>128</v>
@@ -4770,7 +4770,7 @@
     </row>
     <row r="58" spans="1:11" s="48" customFormat="1">
       <c r="A58" s="48" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B58" s="48" t="s">
         <v>128</v>
@@ -4781,7 +4781,7 @@
     </row>
     <row r="59" spans="1:11" s="48" customFormat="1">
       <c r="A59" s="48" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B59" s="48" t="s">
         <v>128</v>
@@ -4792,7 +4792,7 @@
     </row>
     <row r="60" spans="1:11" s="48" customFormat="1">
       <c r="A60" s="48" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B60" s="48" t="s">
         <v>172</v>
@@ -4806,7 +4806,7 @@
     </row>
     <row r="61" spans="1:11" s="48" customFormat="1">
       <c r="A61" s="48" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B61" s="48" t="s">
         <v>172</v>
@@ -4817,7 +4817,7 @@
     </row>
     <row r="62" spans="1:11" s="48" customFormat="1">
       <c r="A62" s="48" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B62" s="48" t="s">
         <v>172</v>
@@ -4828,7 +4828,7 @@
     </row>
     <row r="63" spans="1:11" s="48" customFormat="1">
       <c r="A63" s="48" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B63" s="48" t="s">
         <v>172</v>
@@ -4842,18 +4842,18 @@
     </row>
     <row r="64" spans="1:11" s="48" customFormat="1">
       <c r="A64" s="48" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B64" s="48" t="s">
         <v>172</v>
       </c>
       <c r="C64" s="48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="65" spans="1:11" s="48" customFormat="1">
       <c r="A65" s="48" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B65" s="48" t="s">
         <v>172</v>
@@ -4864,88 +4864,88 @@
     </row>
     <row r="66" spans="1:11" s="48" customFormat="1">
       <c r="A66" s="48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B66" s="48" t="s">
         <v>172</v>
       </c>
       <c r="C66" s="48" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="48" customFormat="1">
       <c r="A67" s="48" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B67" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C67" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="D67" s="48" t="s">
         <v>243</v>
-      </c>
-      <c r="D67" s="48" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:11" s="48" customFormat="1">
       <c r="A68" s="48" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B68" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C68" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="D68" s="48" t="s">
         <v>243</v>
-      </c>
-      <c r="D68" s="48" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="48" customFormat="1">
       <c r="A69" s="48" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B69" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C69" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="D69" s="48" t="s">
         <v>243</v>
-      </c>
-      <c r="D69" s="48" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="48" customFormat="1">
       <c r="A70" s="48" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B70" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C70" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="D70" s="48" t="s">
         <v>243</v>
-      </c>
-      <c r="D70" s="48" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="71" spans="1:11" s="48" customFormat="1">
       <c r="A71" s="48" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B71" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C71" s="48" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D71" s="48" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="72" spans="1:11" s="48" customFormat="1">
       <c r="A72" s="48" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B72" s="48" t="s">
         <v>15</v>
@@ -4956,16 +4956,16 @@
     </row>
     <row r="73" spans="1:11" s="48" customFormat="1">
       <c r="A73" s="48" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B73" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C73" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="D73" s="48" t="s">
         <v>243</v>
-      </c>
-      <c r="D73" s="48" t="s">
-        <v>244</v>
       </c>
       <c r="K73" s="48" t="s">
         <v>27</v>
@@ -4973,105 +4973,105 @@
     </row>
     <row r="74" spans="1:11" s="48" customFormat="1">
       <c r="A74" s="48" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B74" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C74" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="D74" s="48" t="s">
         <v>243</v>
-      </c>
-      <c r="D74" s="48" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="75" spans="1:11" s="48" customFormat="1">
       <c r="A75" s="48" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B75" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C75" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="D75" s="48" t="s">
         <v>243</v>
-      </c>
-      <c r="D75" s="48" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="48" customFormat="1">
       <c r="A76" s="48" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B76" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C76" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="D76" s="48" t="s">
         <v>243</v>
-      </c>
-      <c r="D76" s="48" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="48" customFormat="1">
       <c r="A77" s="48" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B77" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C77" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="D77" s="48" t="s">
         <v>243</v>
-      </c>
-      <c r="D77" s="48" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="48" customFormat="1">
       <c r="A78" s="48" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B78" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C78" s="48" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="48" customFormat="1">
       <c r="A79" s="48" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B79" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C79" s="48" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="80" spans="1:11" s="48" customFormat="1">
       <c r="A80" s="48" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B80" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C80" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="D80" s="48" t="s">
         <v>243</v>
-      </c>
-      <c r="D80" s="48" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:11" s="48" customFormat="1">
       <c r="A81" s="48" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B81" s="48" t="s">
         <v>138</v>
       </c>
       <c r="C81" s="48" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D81" s="48" t="s">
         <v>86</v>
@@ -5082,24 +5082,24 @@
     </row>
     <row r="82" spans="1:11" s="48" customFormat="1">
       <c r="A82" s="48" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B82" s="48" t="s">
         <v>131</v>
       </c>
       <c r="C82" s="48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D82" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E82" s="48" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="83" spans="1:11" s="48" customFormat="1">
       <c r="A83" s="49" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B83" s="48" t="s">
         <v>138</v>
@@ -5111,27 +5111,27 @@
         <v>86</v>
       </c>
       <c r="K83" s="48" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="84" spans="1:11" s="48" customFormat="1">
       <c r="A84" s="48" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B84" s="48" t="s">
         <v>138</v>
       </c>
       <c r="C84" s="48" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D84" s="48" t="s">
+        <v>297</v>
+      </c>
+      <c r="E84" s="48" t="s">
         <v>298</v>
       </c>
-      <c r="E84" s="48" t="s">
-        <v>299</v>
-      </c>
       <c r="F84" s="48" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G84" s="48" t="s">
         <v>155</v>
@@ -5139,7 +5139,7 @@
     </row>
     <row r="85" spans="1:11" s="48" customFormat="1">
       <c r="A85" s="48" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B85" s="48" t="s">
         <v>131</v>
@@ -5159,13 +5159,13 @@
     </row>
     <row r="86" spans="1:11" s="48" customFormat="1">
       <c r="A86" s="48" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B86" s="48" t="s">
         <v>138</v>
       </c>
       <c r="C86" s="48" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D86" s="48" t="s">
         <v>150</v>
@@ -5174,18 +5174,18 @@
         <v>149</v>
       </c>
       <c r="F86" s="48" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G86" s="48" t="s">
         <v>155</v>
       </c>
       <c r="K86" s="48" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="87" spans="1:11" s="48" customFormat="1">
       <c r="A87" s="48" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B87" s="48" t="s">
         <v>138</v>
@@ -5203,12 +5203,12 @@
         <v>155</v>
       </c>
       <c r="K87" s="48" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="88" spans="1:11" s="48" customFormat="1">
       <c r="A88" s="49" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B88" s="48" t="s">
         <v>138</v>
@@ -5226,12 +5226,12 @@
         <v>155</v>
       </c>
       <c r="K88" s="48" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="89" spans="1:11" s="47" customFormat="1">
       <c r="A89" s="47" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B89" s="47" t="s">
         <v>125</v>
@@ -5248,7 +5248,7 @@
     </row>
     <row r="90" spans="1:11" s="48" customFormat="1">
       <c r="A90" s="48" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B90" s="48" t="s">
         <v>97</v>
@@ -5262,12 +5262,12 @@
         <v>134</v>
       </c>
       <c r="C91" s="48" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="92" spans="1:11" s="48" customFormat="1">
       <c r="A92" s="48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B92" s="48" t="s">
         <v>134</v>
@@ -5281,7 +5281,7 @@
     </row>
     <row r="93" spans="1:11" s="48" customFormat="1">
       <c r="A93" s="49" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B93" s="48" t="s">
         <v>134</v>
@@ -5290,12 +5290,12 @@
         <v>133</v>
       </c>
       <c r="K93" s="48" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="94" spans="1:11" s="48" customFormat="1">
       <c r="A94" s="48" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B94" s="48" t="s">
         <v>143</v>
@@ -5306,7 +5306,7 @@
     </row>
     <row r="95" spans="1:11" s="48" customFormat="1">
       <c r="A95" s="48" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B95" s="48" t="s">
         <v>143</v>
@@ -5323,12 +5323,12 @@
         <v>143</v>
       </c>
       <c r="C96" s="50" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="48" customFormat="1">
       <c r="A97" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B97" s="48" t="s">
         <v>143</v>
@@ -5339,16 +5339,16 @@
     </row>
     <row r="98" spans="1:5" s="48" customFormat="1">
       <c r="A98" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B98" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C98" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D98" s="48" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E98" s="48" t="s">
         <v>63</v>
@@ -5356,272 +5356,272 @@
     </row>
     <row r="99" spans="1:5" s="48" customFormat="1">
       <c r="A99" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B99" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C99" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="48" customFormat="1">
       <c r="A100" s="48" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B100" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C100" s="48" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="48" customFormat="1">
       <c r="A101" s="48" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B101" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C101" s="48" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C102" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C103" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C104" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C105" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C106" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C107" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C108" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B109" t="s">
         <v>143</v>
       </c>
       <c r="C109" s="48" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B110" t="s">
         <v>143</v>
       </c>
       <c r="C110" s="48" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B111" t="s">
         <v>143</v>
       </c>
       <c r="C111" s="48" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B112" t="s">
         <v>143</v>
       </c>
       <c r="C112" s="48" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B113" t="s">
         <v>143</v>
       </c>
       <c r="C113" s="48" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B114" t="s">
         <v>143</v>
       </c>
       <c r="C114" s="48" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B115" t="s">
         <v>143</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B116" t="s">
         <v>143</v>
       </c>
       <c r="C116" s="48" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B117" t="s">
         <v>144</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B118" t="s">
         <v>144</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B119" t="s">
         <v>144</v>
       </c>
       <c r="C119" s="48" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B120" t="s">
         <v>144</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B121" t="s">
         <v>144</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B122" t="s">
         <v>144</v>
       </c>
       <c r="C122" s="48" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B123" t="s">
         <v>144</v>
       </c>
       <c r="C123" s="48" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B124" t="s">
         <v>144</v>
       </c>
       <c r="C124" s="48" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B125" t="s">
         <v>144</v>
@@ -5632,194 +5632,194 @@
     </row>
     <row r="126" spans="1:3" s="48" customFormat="1">
       <c r="A126" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B126" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C126" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="127" spans="1:3" s="48" customFormat="1">
       <c r="A127" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B127" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C127" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="128" spans="1:3" s="48" customFormat="1">
       <c r="A128" s="48" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B128" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C128" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="129" spans="1:3" s="48" customFormat="1">
       <c r="A129" s="48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B129" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C129" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="130" spans="1:3" s="48" customFormat="1">
       <c r="A130" s="48" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B130" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C130" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="131" spans="1:3" s="48" customFormat="1">
       <c r="A131" s="48" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B131" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C131" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="132" spans="1:3" s="48" customFormat="1">
       <c r="A132" s="48" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B132" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C132" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="133" spans="1:3" s="48" customFormat="1">
       <c r="A133" s="48" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B133" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C133" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="134" spans="1:3" s="48" customFormat="1">
       <c r="A134" s="48" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B134" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C134" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="135" spans="1:3" s="48" customFormat="1">
       <c r="A135" s="48" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B135" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C135" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="136" spans="1:3" s="48" customFormat="1">
       <c r="A136" s="48" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B136" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C136" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="137" spans="1:3" s="48" customFormat="1">
       <c r="A137" s="48" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B137" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C137" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="138" spans="1:3" s="48" customFormat="1">
       <c r="A138" s="48" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B138" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C138" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="139" spans="1:3" s="48" customFormat="1">
       <c r="A139" s="48" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B139" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C139" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="140" spans="1:3" s="48" customFormat="1">
       <c r="A140" s="48" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B140" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C140" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="141" spans="1:3" s="48" customFormat="1">
       <c r="A141" s="48" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B141" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C141" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="142" spans="1:3" s="48" customFormat="1">
       <c r="A142" s="48" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B142" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C142" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="48" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B143" s="48" t="s">
         <v>132</v>
@@ -5827,7 +5827,7 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="48" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B144" s="48" t="s">
         <v>180</v>
@@ -5856,7 +5856,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5866,20 +5866,20 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B8" t="s">
         <v>384</v>
-      </c>
-      <c r="B8" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extended `Zs` with skewness and kurtosis
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1619,9 +1619,6 @@
     <t>numel / size</t>
   </si>
   <si>
-    <t>std / cov</t>
-  </si>
-  <si>
     <t>padarray / unpad array</t>
   </si>
   <si>
@@ -1668,6 +1665,9 @@
   </si>
   <si>
     <t>strjoin / convert to '#' and char 0</t>
+  </si>
+  <si>
+    <t>std / cov / skewness / kurtosis</t>
   </si>
 </sst>
 </file>
@@ -2426,7 +2426,7 @@
         <v>512</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>261</v>
@@ -2559,7 +2559,7 @@
         <v>191</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12" customHeight="1">
@@ -2567,7 +2567,7 @@
         <v>103</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>47</v>
@@ -2777,7 +2777,7 @@
         <v>170</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>213</v>
@@ -2869,10 +2869,10 @@
         <v>105</v>
       </c>
       <c r="C36" s="53" t="s">
+        <v>544</v>
+      </c>
+      <c r="D36" s="53" t="s">
         <v>545</v>
-      </c>
-      <c r="D36" s="53" t="s">
-        <v>546</v>
       </c>
       <c r="E36" s="28" t="s">
         <v>87</v>
@@ -2933,7 +2933,7 @@
         <v>128</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D40" s="28" t="s">
         <v>457</v>
@@ -3015,7 +3015,7 @@
         <v>522</v>
       </c>
       <c r="F45" s="52" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
@@ -3137,7 +3137,7 @@
         <v>334</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="12" customHeight="1">
@@ -3290,7 +3290,7 @@
         <v>205</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="12" customHeight="1">
@@ -3328,7 +3328,7 @@
         <v>93</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
@@ -3362,7 +3362,7 @@
         <v>489</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F69" s="28" t="s">
         <v>511</v>
@@ -3395,7 +3395,7 @@
         <v>141</v>
       </c>
       <c r="F71" s="52" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="12" customHeight="1">
@@ -3508,7 +3508,7 @@
         <v>136</v>
       </c>
       <c r="F78" s="52" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="12" customHeight="1">
@@ -3534,7 +3534,7 @@
         <v>287</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E80" s="28" t="s">
         <v>263</v>
@@ -3656,8 +3656,8 @@
       <c r="E87" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="F87" s="28" t="s">
-        <v>532</v>
+      <c r="F87" s="52" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="12" customHeight="1">
@@ -3700,7 +3700,7 @@
         <v>526</v>
       </c>
       <c r="F90" s="52" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="12" customHeight="1">

</xml_diff>

<commit_message>
fft (FFT), fftn (n-dimensional FFT), fftshift
Including Octave compatibility for fftn whtn the second input contains
zeros
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="550">
   <si>
     <t>Normal function</t>
   </si>
@@ -1436,9 +1436,6 @@
     <t>im2col</t>
   </si>
   <si>
-    <t>sign</t>
-  </si>
-  <si>
     <t>gallery</t>
   </si>
   <si>
@@ -1668,6 +1665,12 @@
   </si>
   <si>
     <t>std / cov / skewness / kurtosis</t>
+  </si>
+  <si>
+    <t>fft, nfft</t>
+  </si>
+  <si>
+    <t>sign / fftshift</t>
   </si>
 </sst>
 </file>
@@ -2423,10 +2426,10 @@
         <v>189</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>261</v>
@@ -2469,13 +2472,13 @@
         <v>37</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>150</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F10" s="28" t="s">
         <v>217</v>
@@ -2493,7 +2496,7 @@
         <v>459</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="12" customHeight="1">
@@ -2501,16 +2504,16 @@
         <v>109</v>
       </c>
       <c r="C12" s="37" t="s">
+        <v>492</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>490</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>493</v>
       </c>
-      <c r="D12" s="37" t="s">
-        <v>491</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>494</v>
-      </c>
       <c r="F12" s="37" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12" customHeight="1">
@@ -2518,16 +2521,16 @@
         <v>110</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12" customHeight="1">
@@ -2559,7 +2562,7 @@
         <v>191</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12" customHeight="1">
@@ -2567,7 +2570,7 @@
         <v>103</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>47</v>
@@ -2777,7 +2780,7 @@
         <v>170</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>213</v>
@@ -2858,7 +2861,7 @@
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="28" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F35" s="28" t="s">
         <v>98</v>
@@ -2869,10 +2872,10 @@
         <v>105</v>
       </c>
       <c r="C36" s="53" t="s">
+        <v>543</v>
+      </c>
+      <c r="D36" s="53" t="s">
         <v>544</v>
-      </c>
-      <c r="D36" s="53" t="s">
-        <v>545</v>
       </c>
       <c r="E36" s="28" t="s">
         <v>87</v>
@@ -2889,7 +2892,7 @@
         <v>7</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E37" s="28" t="s">
         <v>307</v>
@@ -2925,7 +2928,7 @@
         <v>470</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="12" customHeight="1">
@@ -2933,7 +2936,7 @@
         <v>128</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D40" s="28" t="s">
         <v>457</v>
@@ -2950,10 +2953,10 @@
         <v>172</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="46"/>
@@ -2967,25 +2970,27 @@
       </c>
       <c r="D42" s="38"/>
       <c r="E42" s="28" t="s">
-        <v>528</v>
-      </c>
-      <c r="F42" s="38"/>
+        <v>527</v>
+      </c>
+      <c r="F42" s="52" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="43" spans="2:6" ht="12" customHeight="1">
       <c r="B43" s="27" t="s">
         <v>138</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D43" s="28" t="s">
         <v>100</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F43" s="36" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="12" customHeight="1">
@@ -3012,10 +3017,10 @@
         <v>248</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F45" s="52" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
@@ -3049,13 +3054,13 @@
         <v>42</v>
       </c>
       <c r="C48" s="40" t="s">
+        <v>475</v>
+      </c>
+      <c r="D48" s="40" t="s">
         <v>476</v>
       </c>
-      <c r="D48" s="40" t="s">
-        <v>477</v>
-      </c>
       <c r="E48" s="28" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F48" s="46"/>
     </row>
@@ -3064,10 +3069,10 @@
         <v>11</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E49" s="29"/>
       <c r="F49" s="29"/>
@@ -3080,7 +3085,7 @@
         <v>206</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>203</v>
@@ -3128,7 +3133,7 @@
         <v>121</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D53" s="28" t="s">
         <v>382</v>
@@ -3137,7 +3142,7 @@
         <v>334</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="12" customHeight="1">
@@ -3148,13 +3153,13 @@
         <v>41</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>40</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="12" customHeight="1">
@@ -3170,8 +3175,8 @@
       <c r="E55" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="F55" s="28" t="s">
-        <v>471</v>
+      <c r="F55" s="52" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="12" customHeight="1">
@@ -3192,7 +3197,7 @@
         <v>43</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D57" s="28" t="s">
         <v>142</v>
@@ -3216,7 +3221,7 @@
         <v>146</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -3290,7 +3295,7 @@
         <v>205</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="12" customHeight="1">
@@ -3320,7 +3325,7 @@
         <v>236</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="12" customHeight="1">
@@ -3328,7 +3333,7 @@
         <v>93</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
@@ -3359,13 +3364,13 @@
         <v>5</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="12" customHeight="1">
@@ -3386,7 +3391,7 @@
         <v>75</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D71" s="28" t="s">
         <v>3</v>
@@ -3395,7 +3400,7 @@
         <v>141</v>
       </c>
       <c r="F71" s="52" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="12" customHeight="1">
@@ -3406,7 +3411,7 @@
         <v>126</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E72" s="28" t="s">
         <v>245</v>
@@ -3450,16 +3455,16 @@
         <v>131</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D75" s="28" t="s">
         <v>73</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="12" customHeight="1">
@@ -3508,7 +3513,7 @@
         <v>136</v>
       </c>
       <c r="F78" s="52" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="12" customHeight="1">
@@ -3516,13 +3521,13 @@
         <v>119</v>
       </c>
       <c r="C79" s="28" t="s">
+        <v>498</v>
+      </c>
+      <c r="D79" s="28" t="s">
         <v>499</v>
       </c>
-      <c r="D79" s="28" t="s">
-        <v>500</v>
-      </c>
       <c r="E79" s="28" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F79" s="46"/>
     </row>
@@ -3534,7 +3539,7 @@
         <v>287</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E80" s="28" t="s">
         <v>263</v>
@@ -3565,13 +3570,13 @@
         <v>66</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D82" s="28" t="s">
+        <v>519</v>
+      </c>
+      <c r="E82" s="28" t="s">
         <v>520</v>
-      </c>
-      <c r="E82" s="28" t="s">
-        <v>521</v>
       </c>
       <c r="F82" s="46"/>
     </row>
@@ -3580,13 +3585,13 @@
         <v>78</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E83" s="28" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F83" s="28" t="s">
         <v>154</v>
@@ -3600,13 +3605,13 @@
         <v>63</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E84" s="28" t="s">
         <v>65</v>
       </c>
       <c r="F84" s="28" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="85" spans="2:6" ht="12" customHeight="1">
@@ -3614,13 +3619,13 @@
         <v>120</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D85" s="28" t="s">
         <v>388</v>
       </c>
       <c r="E85" s="28" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F85" s="28" t="s">
         <v>88</v>
@@ -3657,7 +3662,7 @@
         <v>64</v>
       </c>
       <c r="F87" s="52" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="12" customHeight="1">
@@ -3665,7 +3670,7 @@
         <v>129</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D88" s="46"/>
       <c r="E88" s="46"/>
@@ -3697,10 +3702,10 @@
       </c>
       <c r="D90" s="46"/>
       <c r="E90" s="28" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F90" s="52" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="12" customHeight="1">
@@ -3732,7 +3737,7 @@
         <v>147</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D93" s="28" t="s">
         <v>61</v>
@@ -3752,7 +3757,7 @@
         <v>62</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E94" s="29"/>
       <c r="F94" s="29"/>
@@ -3779,13 +3784,13 @@
         <v>38</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D96" s="28" t="s">
         <v>148</v>
       </c>
       <c r="E96" s="36" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F96" s="28" t="s">
         <v>220</v>
@@ -3796,7 +3801,7 @@
         <v>182</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D97" s="46"/>
       <c r="E97" s="46"/>

</xml_diff>

<commit_message>
Generalized `Y^` (matrix power)
Generalized `Y^` (matrix power) as suggested by @Sanchises: compute sum
of matrix powers if there are more than one exponent in second input
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -635,12 +635,6 @@
     <t>NaN</t>
   </si>
   <si>
-    <t>matrix /</t>
-  </si>
-  <si>
-    <t>matrix \</t>
-  </si>
-  <si>
     <t>stack size</t>
   </si>
   <si>
@@ -731,9 +725,6 @@
     <t>toc</t>
   </si>
   <si>
-    <t>matrix ^</t>
-  </si>
-  <si>
     <t>mod(…-1)+1</t>
   </si>
   <si>
@@ -1671,6 +1662,15 @@
   </si>
   <si>
     <t>sign / fftshift</t>
+  </si>
+  <si>
+    <t>matrix power, or sum of matrix powers</t>
+  </si>
+  <si>
+    <t>right matrix divide</t>
+  </si>
+  <si>
+    <t>left matrix divide</t>
   </si>
 </sst>
 </file>
@@ -2309,7 +2309,7 @@
   <dimension ref="A1:L302"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F98" sqref="B3:F98"/>
+      <selection activeCell="E14" sqref="E14:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" customHeight="1"/>
@@ -2335,16 +2335,16 @@
         <v>0</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="12" customHeight="1">
@@ -2359,16 +2359,16 @@
         <v>175</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="I3" s="21" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="L3" s="23" t="s">
         <v>185</v>
@@ -2377,7 +2377,7 @@
     <row r="4" spans="1:12" ht="12" customHeight="1">
       <c r="B4" s="24"/>
       <c r="C4" s="25" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -2388,7 +2388,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>92</v>
@@ -2411,10 +2411,10 @@
         <v>16</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -2426,13 +2426,13 @@
         <v>189</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="12" customHeight="1">
@@ -2444,10 +2444,10 @@
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="12" customHeight="1">
@@ -2458,13 +2458,13 @@
         <v>184</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="12" customHeight="1">
@@ -2472,16 +2472,16 @@
         <v>37</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>150</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="12" customHeight="1">
@@ -2489,14 +2489,14 @@
         <v>159</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="28" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="12" customHeight="1">
@@ -2504,16 +2504,16 @@
         <v>109</v>
       </c>
       <c r="C12" s="37" t="s">
+        <v>489</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>487</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>490</v>
+      </c>
+      <c r="F12" s="37" t="s">
         <v>492</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>490</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>493</v>
-      </c>
-      <c r="F12" s="37" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12" customHeight="1">
@@ -2521,16 +2521,16 @@
         <v>110</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D13" s="37" t="s">
+        <v>488</v>
+      </c>
+      <c r="E13" s="37" t="s">
         <v>491</v>
       </c>
-      <c r="E13" s="37" t="s">
-        <v>494</v>
-      </c>
       <c r="F13" s="37" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12" customHeight="1">
@@ -2547,7 +2547,7 @@
         <v>39</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="12" customHeight="1">
@@ -2562,7 +2562,7 @@
         <v>191</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12" customHeight="1">
@@ -2570,7 +2570,7 @@
         <v>103</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>47</v>
@@ -2593,7 +2593,7 @@
         <v>149</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F17" s="29"/>
     </row>
@@ -2611,7 +2611,7 @@
         <v>202</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="12" customHeight="1">
@@ -2622,13 +2622,13 @@
         <v>32</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>230</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>204</v>
+        <v>228</v>
+      </c>
+      <c r="E19" s="52" t="s">
+        <v>548</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="12" customHeight="1">
@@ -2639,10 +2639,10 @@
         <v>185</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F20" s="39"/>
     </row>
@@ -2654,10 +2654,10 @@
         <v>185</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F21" s="39"/>
     </row>
@@ -2669,10 +2669,10 @@
         <v>185</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F22" s="39"/>
     </row>
@@ -2684,10 +2684,10 @@
         <v>185</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F23" s="39"/>
     </row>
@@ -2699,10 +2699,10 @@
         <v>185</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F24" s="39"/>
     </row>
@@ -2714,10 +2714,10 @@
         <v>185</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F25" s="39"/>
     </row>
@@ -2729,10 +2729,10 @@
         <v>185</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F26" s="39"/>
     </row>
@@ -2744,7 +2744,7 @@
         <v>185</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E27" s="39"/>
       <c r="F27" s="39"/>
@@ -2757,7 +2757,7 @@
         <v>185</v>
       </c>
       <c r="D28" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E28" s="39"/>
       <c r="F28" s="39"/>
@@ -2770,7 +2770,7 @@
         <v>185</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="39"/>
@@ -2780,16 +2780,16 @@
         <v>170</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D30" s="37" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E30" s="37" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="12" customHeight="1">
@@ -2861,7 +2861,7 @@
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="28" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F35" s="28" t="s">
         <v>98</v>
@@ -2872,10 +2872,10 @@
         <v>105</v>
       </c>
       <c r="C36" s="53" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="D36" s="53" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="E36" s="28" t="s">
         <v>87</v>
@@ -2892,13 +2892,13 @@
         <v>7</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="F37" s="28" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="12" customHeight="1">
@@ -2906,16 +2906,16 @@
         <v>171</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D38" s="28" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="12" customHeight="1">
@@ -2925,10 +2925,10 @@
       <c r="C39" s="46"/>
       <c r="D39" s="46"/>
       <c r="E39" s="28" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="12" customHeight="1">
@@ -2936,13 +2936,13 @@
         <v>128</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="F40" s="28" t="s">
         <v>18</v>
@@ -2953,10 +2953,10 @@
         <v>172</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="46"/>
@@ -2966,14 +2966,14 @@
         <v>113</v>
       </c>
       <c r="C42" s="35" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D42" s="38"/>
       <c r="E42" s="28" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="F42" s="52" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="12" customHeight="1">
@@ -2981,16 +2981,16 @@
         <v>138</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D43" s="28" t="s">
         <v>100</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F43" s="36" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="12" customHeight="1">
@@ -2998,10 +2998,10 @@
         <v>125</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E44" s="46"/>
       <c r="F44" s="46"/>
@@ -3011,16 +3011,16 @@
         <v>97</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F45" s="52" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
@@ -3028,10 +3028,10 @@
         <v>134</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E46" s="46"/>
       <c r="F46" s="46"/>
@@ -3041,10 +3041,10 @@
         <v>143</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D47" s="40" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E47" s="46"/>
       <c r="F47" s="46"/>
@@ -3054,13 +3054,13 @@
         <v>42</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="F48" s="46"/>
     </row>
@@ -3069,10 +3069,10 @@
         <v>11</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="E49" s="29"/>
       <c r="F49" s="29"/>
@@ -3082,16 +3082,16 @@
         <v>144</v>
       </c>
       <c r="C50" s="42" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>203</v>
       </c>
       <c r="F50" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="2:6" ht="12" customHeight="1">
@@ -3099,16 +3099,16 @@
         <v>132</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D51" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="F51" s="28" t="s">
         <v>210</v>
-      </c>
-      <c r="E51" s="28" t="s">
-        <v>211</v>
-      </c>
-      <c r="F51" s="28" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="52" spans="2:6" ht="12" customHeight="1">
@@ -3119,13 +3119,13 @@
         <v>72</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="12" customHeight="1">
@@ -3133,16 +3133,16 @@
         <v>121</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="12" customHeight="1">
@@ -3153,13 +3153,13 @@
         <v>41</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>40</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="12" customHeight="1">
@@ -3176,7 +3176,7 @@
         <v>196</v>
       </c>
       <c r="F55" s="52" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="12" customHeight="1">
@@ -3184,11 +3184,11 @@
         <v>130</v>
       </c>
       <c r="C56" s="35" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D56" s="46"/>
       <c r="E56" s="36" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F56" s="38"/>
     </row>
@@ -3197,7 +3197,7 @@
         <v>43</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D57" s="28" t="s">
         <v>142</v>
@@ -3221,7 +3221,7 @@
         <v>146</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -3254,7 +3254,7 @@
         <v>94</v>
       </c>
       <c r="F61" s="36" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="62" spans="2:6" ht="12" customHeight="1">
@@ -3273,7 +3273,7 @@
         <v>176</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D63" s="36" t="s">
         <v>13</v>
@@ -3289,13 +3289,13 @@
         <v>9</v>
       </c>
       <c r="D64" s="28" t="s">
-        <v>237</v>
-      </c>
-      <c r="E64" s="28" t="s">
-        <v>205</v>
+        <v>234</v>
+      </c>
+      <c r="E64" s="52" t="s">
+        <v>549</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="12" customHeight="1">
@@ -3303,7 +3303,7 @@
         <v>178</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D65" s="28" t="s">
         <v>12</v>
@@ -3321,11 +3321,11 @@
       <c r="D66" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E66" s="28" t="s">
-        <v>236</v>
+      <c r="E66" s="52" t="s">
+        <v>547</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="12" customHeight="1">
@@ -3333,7 +3333,7 @@
         <v>93</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
@@ -3344,16 +3344,16 @@
         <v>106</v>
       </c>
       <c r="C68" s="31" t="s">
+        <v>455</v>
+      </c>
+      <c r="D68" s="31" t="s">
         <v>458</v>
       </c>
-      <c r="D68" s="31" t="s">
-        <v>461</v>
-      </c>
       <c r="E68" s="28" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F68" s="28" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="12" customHeight="1">
@@ -3364,13 +3364,13 @@
         <v>5</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="12" customHeight="1">
@@ -3382,7 +3382,7 @@
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="28" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F70" s="29"/>
     </row>
@@ -3391,7 +3391,7 @@
         <v>75</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D71" s="28" t="s">
         <v>3</v>
@@ -3400,7 +3400,7 @@
         <v>141</v>
       </c>
       <c r="F71" s="52" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="12" customHeight="1">
@@ -3411,13 +3411,13 @@
         <v>126</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="E72" s="28" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F72" s="28" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="12" customHeight="1">
@@ -3425,7 +3425,7 @@
         <v>179</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="29"/>
@@ -3445,7 +3445,7 @@
         <v>153</v>
       </c>
       <c r="E74" s="28" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F74" s="29"/>
       <c r="G74" s="1"/>
@@ -3455,16 +3455,16 @@
         <v>131</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D75" s="28" t="s">
         <v>73</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="12" customHeight="1">
@@ -3475,13 +3475,13 @@
         <v>201</v>
       </c>
       <c r="D76" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E76" s="28" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F76" s="28" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="12" customHeight="1">
@@ -3492,10 +3492,10 @@
         <v>95</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E77" s="28" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="F77" s="46"/>
     </row>
@@ -3504,7 +3504,7 @@
         <v>180</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D78" s="28" t="s">
         <v>135</v>
@@ -3513,7 +3513,7 @@
         <v>136</v>
       </c>
       <c r="F78" s="52" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="12" customHeight="1">
@@ -3521,13 +3521,13 @@
         <v>119</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D79" s="28" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="E79" s="28" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="F79" s="46"/>
     </row>
@@ -3536,13 +3536,13 @@
         <v>111</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E80" s="28" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F80" s="28" t="s">
         <v>198</v>
@@ -3556,13 +3556,13 @@
         <v>127</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E81" s="28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F81" s="28" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="82" spans="2:6" ht="12" customHeight="1">
@@ -3570,13 +3570,13 @@
         <v>66</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="D82" s="28" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="E82" s="28" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F82" s="46"/>
     </row>
@@ -3585,13 +3585,13 @@
         <v>78</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E83" s="28" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="F83" s="28" t="s">
         <v>154</v>
@@ -3605,13 +3605,13 @@
         <v>63</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="E84" s="28" t="s">
         <v>65</v>
       </c>
       <c r="F84" s="28" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="85" spans="2:6" ht="12" customHeight="1">
@@ -3619,13 +3619,13 @@
         <v>120</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E85" s="28" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="F85" s="28" t="s">
         <v>88</v>
@@ -3656,13 +3656,13 @@
         <v>60</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="E87" s="28" t="s">
         <v>64</v>
       </c>
       <c r="F87" s="52" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="12" customHeight="1">
@@ -3670,12 +3670,12 @@
         <v>129</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D88" s="46"/>
       <c r="E88" s="46"/>
       <c r="F88" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="89" spans="2:6" ht="12" customHeight="1">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="E89" s="44"/>
       <c r="F89" s="28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="90" spans="2:6" ht="12" customHeight="1">
@@ -3702,10 +3702,10 @@
       </c>
       <c r="D90" s="46"/>
       <c r="E90" s="28" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="F90" s="52" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="12" customHeight="1">
@@ -3737,7 +3737,7 @@
         <v>147</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D93" s="28" t="s">
         <v>61</v>
@@ -3757,7 +3757,7 @@
         <v>62</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="E94" s="29"/>
       <c r="F94" s="29"/>
@@ -3767,7 +3767,7 @@
         <v>181</v>
       </c>
       <c r="C95" s="35" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D95" s="36" t="s">
         <v>140</v>
@@ -3776,7 +3776,7 @@
         <v>139</v>
       </c>
       <c r="F95" s="36" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="96" spans="2:6" ht="12" customHeight="1">
@@ -3784,16 +3784,16 @@
         <v>38</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D96" s="28" t="s">
         <v>148</v>
       </c>
       <c r="E96" s="36" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F96" s="28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="97" spans="2:6" ht="12" customHeight="1">
@@ -3801,12 +3801,12 @@
         <v>182</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D97" s="46"/>
       <c r="E97" s="46"/>
       <c r="F97" s="28" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="98" spans="2:6" ht="12" customHeight="1">
@@ -3823,7 +3823,7 @@
         <v>192</v>
       </c>
       <c r="F98" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="99" spans="2:6" ht="12" customHeight="1">
@@ -3884,10 +3884,10 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="45" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="50" customFormat="1">
@@ -3898,29 +3898,29 @@
         <v>8</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="48" customFormat="1">
       <c r="A3" s="48" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="48" customFormat="1">
       <c r="A4" s="48" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="48" customFormat="1">
@@ -3931,16 +3931,16 @@
         <v>171</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F5" s="48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G5" s="48" t="s">
         <v>203</v>
@@ -3949,7 +3949,7 @@
         <v>94</v>
       </c>
       <c r="I5" s="48" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J5" s="48" t="s">
         <v>63</v>
@@ -3957,90 +3957,90 @@
     </row>
     <row r="6" spans="1:11" s="48" customFormat="1">
       <c r="A6" s="48" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B6" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="48" customFormat="1">
       <c r="A7" s="48" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B7" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="48" customFormat="1">
       <c r="A8" s="48" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B8" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="48" customFormat="1">
       <c r="A9" s="48" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B9" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="48" customFormat="1">
       <c r="A10" s="48" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B10" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="48" customFormat="1">
       <c r="A11" s="48" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B11" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="48" customFormat="1">
       <c r="A12" s="48" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B12" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="48" customFormat="1">
       <c r="A13" s="48" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B13" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K13" s="48" t="s">
         <v>27</v>
@@ -4048,35 +4048,35 @@
     </row>
     <row r="14" spans="1:11" s="48" customFormat="1">
       <c r="A14" s="48" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B14" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="48" customFormat="1">
       <c r="A15" s="48" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B15" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="48" customFormat="1">
       <c r="A16" s="48" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B16" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="48" customFormat="1">
@@ -4087,26 +4087,26 @@
         <v>171</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D17" s="48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="48" customFormat="1">
       <c r="A18" s="48" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B18" s="48" t="s">
         <v>116</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="48" customFormat="1">
       <c r="A19" s="48" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B19" s="48" t="s">
         <v>116</v>
@@ -4118,39 +4118,39 @@
         <v>55</v>
       </c>
       <c r="E19" s="48" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F19" s="48" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="48" customFormat="1">
       <c r="A20" s="48" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B20" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D20" s="48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E20" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="G20" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="F20" s="48" t="s">
-        <v>220</v>
-      </c>
-      <c r="G20" s="48" t="s">
+      <c r="H20" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="I20" s="48" t="s">
         <v>219</v>
-      </c>
-      <c r="H20" s="48" t="s">
-        <v>218</v>
-      </c>
-      <c r="I20" s="48" t="s">
-        <v>221</v>
       </c>
       <c r="K20" s="48" t="s">
         <v>27</v>
@@ -4158,31 +4158,31 @@
     </row>
     <row r="21" spans="1:11" s="48" customFormat="1">
       <c r="A21" s="48" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B21" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E21" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="G21" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="F21" s="48" t="s">
-        <v>220</v>
-      </c>
-      <c r="G21" s="48" t="s">
+      <c r="H21" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="I21" s="48" t="s">
         <v>219</v>
-      </c>
-      <c r="H21" s="48" t="s">
-        <v>218</v>
-      </c>
-      <c r="I21" s="48" t="s">
-        <v>221</v>
       </c>
       <c r="K21" s="48" t="s">
         <v>27</v>
@@ -4196,25 +4196,25 @@
         <v>171</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D22" s="48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E22" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="F22" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="G22" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="F22" s="48" t="s">
-        <v>220</v>
-      </c>
-      <c r="G22" s="48" t="s">
+      <c r="H22" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="I22" s="48" t="s">
         <v>219</v>
-      </c>
-      <c r="H22" s="48" t="s">
-        <v>218</v>
-      </c>
-      <c r="I22" s="48" t="s">
-        <v>221</v>
       </c>
       <c r="K22" s="48" t="s">
         <v>27</v>
@@ -4222,31 +4222,31 @@
     </row>
     <row r="23" spans="1:11" s="48" customFormat="1">
       <c r="A23" s="48" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B23" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D23" s="48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E23" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="F23" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="G23" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="F23" s="48" t="s">
-        <v>220</v>
-      </c>
-      <c r="G23" s="48" t="s">
+      <c r="H23" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="I23" s="48" t="s">
         <v>219</v>
-      </c>
-      <c r="H23" s="48" t="s">
-        <v>218</v>
-      </c>
-      <c r="I23" s="48" t="s">
-        <v>221</v>
       </c>
       <c r="K23" s="48" t="s">
         <v>27</v>
@@ -4254,19 +4254,19 @@
     </row>
     <row r="24" spans="1:11" s="48" customFormat="1">
       <c r="A24" s="48" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B24" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E24" s="48" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F24" s="48" t="s">
         <v>203</v>
@@ -4289,10 +4289,10 @@
         <v>171</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="K25" s="48" t="s">
         <v>27</v>
@@ -4300,13 +4300,13 @@
     </row>
     <row r="26" spans="1:11" s="48" customFormat="1">
       <c r="A26" s="48" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B26" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D26" s="48" t="s">
         <v>63</v>
@@ -4314,7 +4314,7 @@
     </row>
     <row r="27" spans="1:11" s="48" customFormat="1">
       <c r="A27" s="48" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B27" s="48" t="s">
         <v>116</v>
@@ -4326,15 +4326,15 @@
         <v>55</v>
       </c>
       <c r="E27" s="48" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F27" s="48" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="48" customFormat="1">
       <c r="A28" s="48" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B28" s="48" t="s">
         <v>116</v>
@@ -4345,13 +4345,13 @@
     </row>
     <row r="29" spans="1:11" s="48" customFormat="1">
       <c r="A29" s="48" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B29" s="48" t="s">
         <v>171</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E29" s="48" t="s">
         <v>203</v>
@@ -4362,31 +4362,31 @@
     </row>
     <row r="30" spans="1:11" s="48" customFormat="1">
       <c r="A30" s="48" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B30" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E30" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="F30" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="G30" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="F30" s="48" t="s">
-        <v>220</v>
-      </c>
-      <c r="G30" s="48" t="s">
+      <c r="H30" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="I30" s="48" t="s">
         <v>219</v>
-      </c>
-      <c r="H30" s="48" t="s">
-        <v>218</v>
-      </c>
-      <c r="I30" s="48" t="s">
-        <v>221</v>
       </c>
       <c r="K30" s="48" t="s">
         <v>27</v>
@@ -4394,31 +4394,31 @@
     </row>
     <row r="31" spans="1:11" s="48" customFormat="1">
       <c r="A31" s="48" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B31" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E31" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="F31" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="G31" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="F31" s="48" t="s">
-        <v>220</v>
-      </c>
-      <c r="G31" s="48" t="s">
+      <c r="H31" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="I31" s="48" t="s">
         <v>219</v>
-      </c>
-      <c r="H31" s="48" t="s">
-        <v>218</v>
-      </c>
-      <c r="I31" s="48" t="s">
-        <v>221</v>
       </c>
       <c r="K31" s="48" t="s">
         <v>27</v>
@@ -4426,34 +4426,34 @@
     </row>
     <row r="32" spans="1:11" s="48" customFormat="1">
       <c r="A32" s="48" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B32" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C32" s="48" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E32" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="F32" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="G32" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="F32" s="48" t="s">
-        <v>220</v>
-      </c>
-      <c r="G32" s="48" t="s">
+      <c r="H32" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="I32" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="H32" s="48" t="s">
-        <v>218</v>
-      </c>
-      <c r="I32" s="48" t="s">
-        <v>221</v>
-      </c>
       <c r="J32" s="48" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K32" s="48" t="s">
         <v>27</v>
@@ -4461,31 +4461,31 @@
     </row>
     <row r="33" spans="1:11" s="48" customFormat="1">
       <c r="A33" s="48" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B33" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C33" s="48" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E33" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="F33" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="G33" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="F33" s="48" t="s">
-        <v>220</v>
-      </c>
-      <c r="G33" s="48" t="s">
+      <c r="H33" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="I33" s="48" t="s">
         <v>219</v>
-      </c>
-      <c r="H33" s="48" t="s">
-        <v>218</v>
-      </c>
-      <c r="I33" s="48" t="s">
-        <v>221</v>
       </c>
       <c r="K33" s="48" t="s">
         <v>27</v>
@@ -4493,7 +4493,7 @@
     </row>
     <row r="34" spans="1:11" s="48" customFormat="1">
       <c r="A34" s="48" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B34" s="48" t="s">
         <v>4</v>
@@ -4504,7 +4504,7 @@
     </row>
     <row r="35" spans="1:11" s="48" customFormat="1">
       <c r="A35" s="48" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B35" s="48" t="s">
         <v>4</v>
@@ -4515,7 +4515,7 @@
     </row>
     <row r="36" spans="1:11" s="48" customFormat="1">
       <c r="A36" s="48" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B36" s="48" t="s">
         <v>4</v>
@@ -4526,7 +4526,7 @@
     </row>
     <row r="37" spans="1:11" s="48" customFormat="1">
       <c r="A37" s="48" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B37" s="48" t="s">
         <v>4</v>
@@ -4537,7 +4537,7 @@
     </row>
     <row r="38" spans="1:11" s="48" customFormat="1">
       <c r="A38" s="48" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B38" s="48" t="s">
         <v>4</v>
@@ -4548,7 +4548,7 @@
     </row>
     <row r="39" spans="1:11" s="48" customFormat="1">
       <c r="A39" s="48" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B39" s="48" t="s">
         <v>4</v>
@@ -4559,7 +4559,7 @@
     </row>
     <row r="40" spans="1:11" s="48" customFormat="1">
       <c r="A40" s="48" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B40" s="48" t="s">
         <v>4</v>
@@ -4570,7 +4570,7 @@
     </row>
     <row r="41" spans="1:11" s="48" customFormat="1">
       <c r="A41" s="48" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B41" s="48" t="s">
         <v>4</v>
@@ -4581,7 +4581,7 @@
     </row>
     <row r="42" spans="1:11" s="48" customFormat="1">
       <c r="A42" s="48" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B42" s="48" t="s">
         <v>4</v>
@@ -4592,7 +4592,7 @@
     </row>
     <row r="43" spans="1:11" s="48" customFormat="1">
       <c r="A43" s="48" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B43" s="48" t="s">
         <v>4</v>
@@ -4603,7 +4603,7 @@
     </row>
     <row r="44" spans="1:11" s="48" customFormat="1">
       <c r="A44" s="48" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B44" s="48" t="s">
         <v>4</v>
@@ -4614,7 +4614,7 @@
     </row>
     <row r="45" spans="1:11" s="48" customFormat="1">
       <c r="A45" s="48" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B45" s="48" t="s">
         <v>4</v>
@@ -4625,7 +4625,7 @@
     </row>
     <row r="46" spans="1:11" s="48" customFormat="1">
       <c r="A46" s="48" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B46" s="48" t="s">
         <v>4</v>
@@ -4636,7 +4636,7 @@
     </row>
     <row r="47" spans="1:11" s="48" customFormat="1">
       <c r="A47" s="48" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B47" s="48" t="s">
         <v>4</v>
@@ -4647,7 +4647,7 @@
     </row>
     <row r="48" spans="1:11" s="48" customFormat="1">
       <c r="A48" s="48" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B48" s="48" t="s">
         <v>4</v>
@@ -4669,7 +4669,7 @@
     </row>
     <row r="50" spans="1:11" s="48" customFormat="1">
       <c r="A50" s="48" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B50" s="48" t="s">
         <v>128</v>
@@ -4683,7 +4683,7 @@
     </row>
     <row r="51" spans="1:11" s="48" customFormat="1">
       <c r="A51" s="48" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B51" s="48" t="s">
         <v>19</v>
@@ -4694,7 +4694,7 @@
     </row>
     <row r="52" spans="1:11" s="48" customFormat="1">
       <c r="A52" s="48" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B52" s="48" t="s">
         <v>128</v>
@@ -4708,7 +4708,7 @@
     </row>
     <row r="53" spans="1:11" s="48" customFormat="1">
       <c r="A53" s="48" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B53" s="48" t="s">
         <v>128</v>
@@ -4719,7 +4719,7 @@
     </row>
     <row r="54" spans="1:11" s="48" customFormat="1">
       <c r="A54" s="48" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B54" s="48" t="s">
         <v>128</v>
@@ -4728,7 +4728,7 @@
         <v>90</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="K54" s="48" t="s">
         <v>27</v>
@@ -4736,7 +4736,7 @@
     </row>
     <row r="55" spans="1:11" s="48" customFormat="1">
       <c r="A55" s="48" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B55" s="48" t="s">
         <v>19</v>
@@ -4747,7 +4747,7 @@
     </row>
     <row r="56" spans="1:11" s="48" customFormat="1">
       <c r="A56" s="48" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B56" s="48" t="s">
         <v>128</v>
@@ -4761,7 +4761,7 @@
     </row>
     <row r="57" spans="1:11" s="48" customFormat="1">
       <c r="A57" s="48" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B57" s="48" t="s">
         <v>128</v>
@@ -4775,7 +4775,7 @@
     </row>
     <row r="58" spans="1:11" s="48" customFormat="1">
       <c r="A58" s="48" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B58" s="48" t="s">
         <v>128</v>
@@ -4786,7 +4786,7 @@
     </row>
     <row r="59" spans="1:11" s="48" customFormat="1">
       <c r="A59" s="48" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B59" s="48" t="s">
         <v>128</v>
@@ -4797,13 +4797,13 @@
     </row>
     <row r="60" spans="1:11" s="48" customFormat="1">
       <c r="A60" s="48" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B60" s="48" t="s">
         <v>172</v>
       </c>
       <c r="C60" s="48" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K60" s="48" t="s">
         <v>27</v>
@@ -4811,35 +4811,35 @@
     </row>
     <row r="61" spans="1:11" s="48" customFormat="1">
       <c r="A61" s="48" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B61" s="48" t="s">
         <v>172</v>
       </c>
       <c r="C61" s="48" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="48" customFormat="1">
       <c r="A62" s="48" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B62" s="48" t="s">
         <v>172</v>
       </c>
       <c r="C62" s="48" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="63" spans="1:11" s="48" customFormat="1">
       <c r="A63" s="48" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B63" s="48" t="s">
         <v>172</v>
       </c>
       <c r="C63" s="48" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K63" s="48" t="s">
         <v>27</v>
@@ -4847,110 +4847,110 @@
     </row>
     <row r="64" spans="1:11" s="48" customFormat="1">
       <c r="A64" s="48" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B64" s="48" t="s">
         <v>172</v>
       </c>
       <c r="C64" s="48" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="65" spans="1:11" s="48" customFormat="1">
       <c r="A65" s="48" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B65" s="48" t="s">
         <v>172</v>
       </c>
       <c r="C65" s="48" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="66" spans="1:11" s="48" customFormat="1">
       <c r="A66" s="48" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B66" s="48" t="s">
         <v>172</v>
       </c>
       <c r="C66" s="48" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="48" customFormat="1">
       <c r="A67" s="48" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B67" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C67" s="48" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D67" s="48" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="68" spans="1:11" s="48" customFormat="1">
       <c r="A68" s="48" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B68" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C68" s="48" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D68" s="48" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="48" customFormat="1">
       <c r="A69" s="48" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B69" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C69" s="48" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D69" s="48" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="48" customFormat="1">
       <c r="A70" s="48" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B70" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C70" s="48" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D70" s="48" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="71" spans="1:11" s="48" customFormat="1">
       <c r="A71" s="48" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B71" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C71" s="48" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D71" s="48" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="72" spans="1:11" s="48" customFormat="1">
       <c r="A72" s="48" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B72" s="48" t="s">
         <v>15</v>
@@ -4961,16 +4961,16 @@
     </row>
     <row r="73" spans="1:11" s="48" customFormat="1">
       <c r="A73" s="48" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B73" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C73" s="48" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D73" s="48" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="K73" s="48" t="s">
         <v>27</v>
@@ -4978,105 +4978,105 @@
     </row>
     <row r="74" spans="1:11" s="48" customFormat="1">
       <c r="A74" s="48" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B74" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C74" s="48" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D74" s="48" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="75" spans="1:11" s="48" customFormat="1">
       <c r="A75" s="48" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B75" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C75" s="48" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D75" s="48" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="48" customFormat="1">
       <c r="A76" s="48" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B76" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C76" s="48" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D76" s="48" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="48" customFormat="1">
       <c r="A77" s="48" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B77" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C77" s="48" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D77" s="48" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="48" customFormat="1">
       <c r="A78" s="48" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B78" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C78" s="48" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="48" customFormat="1">
       <c r="A79" s="48" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B79" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C79" s="48" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="80" spans="1:11" s="48" customFormat="1">
       <c r="A80" s="48" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B80" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C80" s="48" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D80" s="48" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="81" spans="1:11" s="48" customFormat="1">
       <c r="A81" s="48" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B81" s="48" t="s">
         <v>138</v>
       </c>
       <c r="C81" s="48" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D81" s="48" t="s">
         <v>86</v>
@@ -5087,24 +5087,24 @@
     </row>
     <row r="82" spans="1:11" s="48" customFormat="1">
       <c r="A82" s="48" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B82" s="48" t="s">
         <v>131</v>
       </c>
       <c r="C82" s="48" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D82" s="48" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E82" s="48" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="83" spans="1:11" s="48" customFormat="1">
       <c r="A83" s="49" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B83" s="48" t="s">
         <v>138</v>
@@ -5116,27 +5116,27 @@
         <v>86</v>
       </c>
       <c r="K83" s="48" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="84" spans="1:11" s="48" customFormat="1">
       <c r="A84" s="48" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B84" s="48" t="s">
         <v>138</v>
       </c>
       <c r="C84" s="48" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D84" s="48" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E84" s="48" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F84" s="48" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G84" s="48" t="s">
         <v>155</v>
@@ -5144,7 +5144,7 @@
     </row>
     <row r="85" spans="1:11" s="48" customFormat="1">
       <c r="A85" s="48" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B85" s="48" t="s">
         <v>131</v>
@@ -5164,13 +5164,13 @@
     </row>
     <row r="86" spans="1:11" s="48" customFormat="1">
       <c r="A86" s="48" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B86" s="48" t="s">
         <v>138</v>
       </c>
       <c r="C86" s="48" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D86" s="48" t="s">
         <v>150</v>
@@ -5179,18 +5179,18 @@
         <v>149</v>
       </c>
       <c r="F86" s="48" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="G86" s="48" t="s">
         <v>155</v>
       </c>
       <c r="K86" s="48" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="87" spans="1:11" s="48" customFormat="1">
       <c r="A87" s="48" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B87" s="48" t="s">
         <v>138</v>
@@ -5208,12 +5208,12 @@
         <v>155</v>
       </c>
       <c r="K87" s="48" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="88" spans="1:11" s="48" customFormat="1">
       <c r="A88" s="49" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B88" s="48" t="s">
         <v>138</v>
@@ -5231,12 +5231,12 @@
         <v>155</v>
       </c>
       <c r="K88" s="48" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="89" spans="1:11" s="47" customFormat="1">
       <c r="A89" s="47" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B89" s="47" t="s">
         <v>125</v>
@@ -5253,7 +5253,7 @@
     </row>
     <row r="90" spans="1:11" s="48" customFormat="1">
       <c r="A90" s="48" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B90" s="48" t="s">
         <v>97</v>
@@ -5267,12 +5267,12 @@
         <v>134</v>
       </c>
       <c r="C91" s="48" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="92" spans="1:11" s="48" customFormat="1">
       <c r="A92" s="48" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B92" s="48" t="s">
         <v>134</v>
@@ -5286,7 +5286,7 @@
     </row>
     <row r="93" spans="1:11" s="48" customFormat="1">
       <c r="A93" s="49" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B93" s="48" t="s">
         <v>134</v>
@@ -5295,29 +5295,29 @@
         <v>133</v>
       </c>
       <c r="K93" s="48" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="94" spans="1:11" s="48" customFormat="1">
       <c r="A94" s="48" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B94" s="48" t="s">
         <v>143</v>
       </c>
       <c r="C94" s="48" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="95" spans="1:11" s="48" customFormat="1">
       <c r="A95" s="48" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B95" s="48" t="s">
         <v>143</v>
       </c>
       <c r="C95" s="48" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="96" spans="1:11" s="50" customFormat="1">
@@ -5328,32 +5328,32 @@
         <v>143</v>
       </c>
       <c r="C96" s="50" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="48" customFormat="1">
       <c r="A97" s="48" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B97" s="48" t="s">
         <v>143</v>
       </c>
       <c r="C97" s="48" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="48" customFormat="1">
       <c r="A98" s="48" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B98" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C98" s="48" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D98" s="48" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E98" s="48" t="s">
         <v>63</v>
@@ -5361,272 +5361,272 @@
     </row>
     <row r="99" spans="1:5" s="48" customFormat="1">
       <c r="A99" s="48" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B99" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C99" s="48" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="48" customFormat="1">
       <c r="A100" s="48" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B100" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C100" s="48" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="48" customFormat="1">
       <c r="A101" s="48" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B101" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C101" s="48" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C102" s="48" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C103" s="48" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C104" s="48" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C105" s="48" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C106" s="48" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C107" s="48" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C108" s="48" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B109" t="s">
         <v>143</v>
       </c>
       <c r="C109" s="48" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B110" t="s">
         <v>143</v>
       </c>
       <c r="C110" s="48" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B111" t="s">
         <v>143</v>
       </c>
       <c r="C111" s="48" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B112" t="s">
         <v>143</v>
       </c>
       <c r="C112" s="48" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B113" t="s">
         <v>143</v>
       </c>
       <c r="C113" s="48" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B114" t="s">
         <v>143</v>
       </c>
       <c r="C114" s="48" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B115" t="s">
         <v>143</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B116" t="s">
         <v>143</v>
       </c>
       <c r="C116" s="48" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B117" t="s">
         <v>144</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B118" t="s">
         <v>144</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B119" t="s">
         <v>144</v>
       </c>
       <c r="C119" s="48" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B120" t="s">
         <v>144</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B121" t="s">
         <v>144</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B122" t="s">
         <v>144</v>
       </c>
       <c r="C122" s="48" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B123" t="s">
         <v>144</v>
       </c>
       <c r="C123" s="48" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B124" t="s">
         <v>144</v>
       </c>
       <c r="C124" s="48" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B125" t="s">
         <v>144</v>
@@ -5637,194 +5637,194 @@
     </row>
     <row r="126" spans="1:3" s="48" customFormat="1">
       <c r="A126" s="48" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B126" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C126" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="127" spans="1:3" s="48" customFormat="1">
       <c r="A127" s="48" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B127" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C127" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="128" spans="1:3" s="48" customFormat="1">
       <c r="A128" s="48" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B128" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C128" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="129" spans="1:3" s="48" customFormat="1">
       <c r="A129" s="48" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B129" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C129" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="130" spans="1:3" s="48" customFormat="1">
       <c r="A130" s="48" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B130" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C130" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="131" spans="1:3" s="48" customFormat="1">
       <c r="A131" s="48" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B131" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C131" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="132" spans="1:3" s="48" customFormat="1">
       <c r="A132" s="48" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B132" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C132" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="133" spans="1:3" s="48" customFormat="1">
       <c r="A133" s="48" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B133" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C133" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="134" spans="1:3" s="48" customFormat="1">
       <c r="A134" s="48" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B134" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C134" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="135" spans="1:3" s="48" customFormat="1">
       <c r="A135" s="48" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B135" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C135" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="136" spans="1:3" s="48" customFormat="1">
       <c r="A136" s="48" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B136" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C136" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="137" spans="1:3" s="48" customFormat="1">
       <c r="A137" s="48" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B137" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C137" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="138" spans="1:3" s="48" customFormat="1">
       <c r="A138" s="48" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B138" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C138" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="139" spans="1:3" s="48" customFormat="1">
       <c r="A139" s="48" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B139" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C139" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="140" spans="1:3" s="48" customFormat="1">
       <c r="A140" s="48" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B140" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C140" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="141" spans="1:3" s="48" customFormat="1">
       <c r="A141" s="48" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B141" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C141" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="142" spans="1:3" s="48" customFormat="1">
       <c r="A142" s="48" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B142" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C142" s="48" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="48" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B143" s="48" t="s">
         <v>132</v>
@@ -5832,7 +5832,7 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="48" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B144" s="48" t="s">
         <v>180</v>
@@ -5861,7 +5861,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5871,20 +5871,20 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B8" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
`Ye`: matrix exponential / logical "infinite" graph power
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="551">
   <si>
     <t>Normal function</t>
   </si>
@@ -1671,6 +1671,9 @@
   </si>
   <si>
     <t>left matrix divide</t>
+  </si>
+  <si>
+    <t>expm / logical "infinite" graph power</t>
   </si>
 </sst>
 </file>
@@ -2308,8 +2311,8 @@
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:E15"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" customHeight="1"/>
@@ -3428,7 +3431,9 @@
         <v>462</v>
       </c>
       <c r="D73" s="29"/>
-      <c r="E73" s="29"/>
+      <c r="E73" s="52" t="s">
+        <v>550</v>
+      </c>
       <c r="F73" s="28" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Small changes in doc
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1481,27 +1481,12 @@
     <t>any(…, 1)</t>
   </si>
   <si>
-    <t>( ) reference indexing</t>
-  </si>
-  <si>
     <t>{ } assignment indexing</t>
   </si>
   <si>
     <t>{ } reference indexing</t>
   </si>
   <si>
-    <t>( ) assignment indexing / split</t>
-  </si>
-  <si>
-    <t>( ) assignment ind. with final :   / split</t>
-  </si>
-  <si>
-    <t>( ) reference ind. with final :</t>
-  </si>
-  <si>
-    <t>( ) assignment ind. with initial :   / split</t>
-  </si>
-  <si>
     <t>imwrite / imagesc / image / imshow</t>
   </si>
   <si>
@@ -1526,9 +1511,6 @@
     <t>closest values</t>
   </si>
   <si>
-    <t>( ) refererence ind. with initial :</t>
-  </si>
-  <si>
     <t>2 raised to input</t>
   </si>
   <si>
@@ -1674,6 +1656,24 @@
   </si>
   <si>
     <t>expm / logical "infinite" graph power</t>
+  </si>
+  <si>
+    <t>( ) assignment indexing</t>
+  </si>
+  <si>
+    <t>( ) reference indexing / split</t>
+  </si>
+  <si>
+    <t xml:space="preserve">( ) assignment ind. with final : </t>
+  </si>
+  <si>
+    <t>( ) reference ind. with final :  / split</t>
+  </si>
+  <si>
+    <t xml:space="preserve">( ) assignment ind. with initial : </t>
+  </si>
+  <si>
+    <t>( ) refererence ind. with initial :  / split</t>
   </si>
 </sst>
 </file>
@@ -2311,8 +2311,8 @@
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" customHeight="1"/>
@@ -2429,10 +2429,10 @@
         <v>189</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>258</v>
@@ -2475,7 +2475,7 @@
         <v>37</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>150</v>
@@ -2507,16 +2507,16 @@
         <v>109</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>489</v>
+        <v>545</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>490</v>
+        <v>547</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>492</v>
+        <v>549</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12" customHeight="1">
@@ -2524,16 +2524,16 @@
         <v>110</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>486</v>
+        <v>546</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>491</v>
+        <v>548</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>501</v>
+        <v>550</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12" customHeight="1">
@@ -2565,7 +2565,7 @@
         <v>191</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12" customHeight="1">
@@ -2573,7 +2573,7 @@
         <v>103</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>47</v>
@@ -2628,7 +2628,7 @@
         <v>228</v>
       </c>
       <c r="E19" s="52" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="F19" s="28" t="s">
         <v>229</v>
@@ -2783,7 +2783,7 @@
         <v>170</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>211</v>
@@ -2864,7 +2864,7 @@
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="28" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="F35" s="28" t="s">
         <v>98</v>
@@ -2875,10 +2875,10 @@
         <v>105</v>
       </c>
       <c r="C36" s="53" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="D36" s="53" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="E36" s="28" t="s">
         <v>87</v>
@@ -2939,7 +2939,7 @@
         <v>128</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="D40" s="28" t="s">
         <v>454</v>
@@ -2956,10 +2956,10 @@
         <v>172</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="46"/>
@@ -2973,10 +2973,10 @@
       </c>
       <c r="D42" s="38"/>
       <c r="E42" s="28" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="F42" s="52" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="12" customHeight="1">
@@ -2990,10 +2990,10 @@
         <v>100</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="F43" s="36" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="12" customHeight="1">
@@ -3020,10 +3020,10 @@
         <v>245</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="F45" s="52" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
@@ -3075,7 +3075,7 @@
         <v>474</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="E49" s="29"/>
       <c r="F49" s="29"/>
@@ -3088,7 +3088,7 @@
         <v>204</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>203</v>
@@ -3145,7 +3145,7 @@
         <v>331</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="12" customHeight="1">
@@ -3156,13 +3156,13 @@
         <v>41</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>40</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="12" customHeight="1">
@@ -3179,7 +3179,7 @@
         <v>196</v>
       </c>
       <c r="F55" s="52" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="12" customHeight="1">
@@ -3200,7 +3200,7 @@
         <v>43</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="D57" s="28" t="s">
         <v>142</v>
@@ -3224,7 +3224,7 @@
         <v>146</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -3295,10 +3295,10 @@
         <v>234</v>
       </c>
       <c r="E64" s="52" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="12" customHeight="1">
@@ -3325,10 +3325,10 @@
         <v>44</v>
       </c>
       <c r="E66" s="52" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="12" customHeight="1">
@@ -3336,7 +3336,7 @@
         <v>93</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
@@ -3370,10 +3370,10 @@
         <v>485</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="12" customHeight="1">
@@ -3394,7 +3394,7 @@
         <v>75</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D71" s="28" t="s">
         <v>3</v>
@@ -3403,7 +3403,7 @@
         <v>141</v>
       </c>
       <c r="F71" s="52" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="12" customHeight="1">
@@ -3414,7 +3414,7 @@
         <v>126</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="E72" s="28" t="s">
         <v>242</v>
@@ -3432,7 +3432,7 @@
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="52" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="F73" s="28" t="s">
         <v>45</v>
@@ -3460,16 +3460,16 @@
         <v>131</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D75" s="28" t="s">
         <v>73</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="12" customHeight="1">
@@ -3518,7 +3518,7 @@
         <v>136</v>
       </c>
       <c r="F78" s="52" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="12" customHeight="1">
@@ -3526,13 +3526,13 @@
         <v>119</v>
       </c>
       <c r="C79" s="28" t="s">
+        <v>490</v>
+      </c>
+      <c r="D79" s="28" t="s">
+        <v>491</v>
+      </c>
+      <c r="E79" s="28" t="s">
         <v>495</v>
-      </c>
-      <c r="D79" s="28" t="s">
-        <v>496</v>
-      </c>
-      <c r="E79" s="28" t="s">
-        <v>500</v>
       </c>
       <c r="F79" s="46"/>
     </row>
@@ -3544,7 +3544,7 @@
         <v>284</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="E80" s="28" t="s">
         <v>260</v>
@@ -3575,13 +3575,13 @@
         <v>66</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="D82" s="28" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="E82" s="28" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="F82" s="46"/>
     </row>
@@ -3590,13 +3590,13 @@
         <v>78</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>76</v>
       </c>
       <c r="E83" s="28" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="F83" s="28" t="s">
         <v>154</v>
@@ -3667,7 +3667,7 @@
         <v>64</v>
       </c>
       <c r="F87" s="52" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="12" customHeight="1">
@@ -3707,10 +3707,10 @@
       </c>
       <c r="D90" s="46"/>
       <c r="E90" s="28" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="F90" s="52" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="12" customHeight="1">
@@ -3762,7 +3762,7 @@
         <v>62</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="E94" s="29"/>
       <c r="F94" s="29"/>
@@ -3789,7 +3789,7 @@
         <v>38</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="D96" s="28" t="s">
         <v>148</v>
@@ -3806,7 +3806,7 @@
         <v>182</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="D97" s="46"/>
       <c r="E97" s="46"/>

</xml_diff>

<commit_message>
`linspace` added in `ZS`
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Dropbox\MATL\spec\functionTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D883509D-A527-4D91-B7F7-67F80FB6AA0E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="16515" windowHeight="8760"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="16520" windowHeight="8760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -1643,9 +1644,6 @@
     <t>fft, nfft</t>
   </si>
   <si>
-    <t>sign / fftshift</t>
-  </si>
-  <si>
     <t>matrix power, or sum of matrix powers</t>
   </si>
   <si>
@@ -1674,12 +1672,15 @@
   </si>
   <si>
     <t>( ) refererence ind. with initial :  / split</t>
+  </si>
+  <si>
+    <t>sign / fftshift / linspace</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="17">
     <font>
       <sz val="10"/>
@@ -2095,6 +2096,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2130,6 +2148,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2305,25 +2340,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="2.85546875" style="13" customWidth="1"/>
-    <col min="3" max="5" width="32.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" customWidth="1"/>
-    <col min="8" max="12" width="23.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="7.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.81640625" style="13" customWidth="1"/>
+    <col min="3" max="5" width="32.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="32.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" style="1" customWidth="1"/>
+    <col min="8" max="12" width="23.7265625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" customHeight="1">
@@ -2507,16 +2542,16 @@
         <v>109</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D12" s="37" t="s">
         <v>486</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12" customHeight="1">
@@ -2524,16 +2559,16 @@
         <v>110</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D13" s="37" t="s">
         <v>487</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12" customHeight="1">
@@ -2628,7 +2663,7 @@
         <v>228</v>
       </c>
       <c r="E19" s="52" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F19" s="28" t="s">
         <v>229</v>
@@ -3179,7 +3214,7 @@
         <v>196</v>
       </c>
       <c r="F55" s="52" t="s">
-        <v>540</v>
+        <v>550</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="12" customHeight="1">
@@ -3295,7 +3330,7 @@
         <v>234</v>
       </c>
       <c r="E64" s="52" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F64" s="52" t="s">
         <v>526</v>
@@ -3325,7 +3360,7 @@
         <v>44</v>
       </c>
       <c r="E66" s="52" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F66" s="28" t="s">
         <v>517</v>
@@ -3432,7 +3467,7 @@
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="52" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F73" s="28" t="s">
         <v>45</v>
@@ -3873,21 +3908,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K65536"/>
   <sheetViews>
     <sheetView topLeftCell="A139" workbookViewId="0">
       <selection activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" ht="13">
       <c r="A1" s="45" t="s">
         <v>277</v>
       </c>
@@ -5855,14 +5890,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Generalized `z` for cell arrays
Generalized `z` for cell arrays, following Sanchises' suggestion
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Dropbox\MATL\spec\functionTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D883509D-A527-4D91-B7F7-67F80FB6AA0E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="16520" windowHeight="8760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="16515" windowHeight="8760"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -210,9 +209,6 @@
     <t>eye</t>
   </si>
   <si>
-    <t>nnz</t>
-  </si>
-  <si>
     <t>prod</t>
   </si>
   <si>
@@ -1675,12 +1671,15 @@
   </si>
   <si>
     <t>sign / fftshift / linspace</t>
+  </si>
+  <si>
+    <t>nnz / cellfun(@nnz, ...)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="17">
     <font>
       <sz val="10"/>
@@ -2096,23 +2095,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2148,23 +2130,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2340,31 +2305,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="2.81640625" style="13" customWidth="1"/>
-    <col min="3" max="5" width="32.81640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="32.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" style="1" customWidth="1"/>
-    <col min="8" max="12" width="23.7265625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.453125" style="1"/>
+    <col min="1" max="1" width="7.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" style="13" customWidth="1"/>
+    <col min="3" max="5" width="32.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" customWidth="1"/>
+    <col min="8" max="12" width="23.7109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" customHeight="1">
       <c r="A1" s="51"/>
       <c r="C1" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="12" customHeight="1">
@@ -2373,49 +2338,49 @@
         <v>0</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="12" customHeight="1">
       <c r="C3" s="5"/>
       <c r="D3" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>175</v>
-      </c>
       <c r="H3" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I3" s="21" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="K3" s="16" t="s">
-        <v>254</v>
-      </c>
       <c r="L3" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="12" customHeight="1">
       <c r="B4" s="24"/>
       <c r="C4" s="25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -2426,83 +2391,83 @@
         <v>25</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="12" customHeight="1">
       <c r="B6" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:12" ht="12" customHeight="1">
       <c r="B7" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="12" customHeight="1">
       <c r="B8" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="12" customHeight="1">
       <c r="B9" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="12" customHeight="1">
@@ -2510,65 +2475,65 @@
         <v>37</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="12" customHeight="1">
       <c r="B11" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="12" customHeight="1">
       <c r="B12" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12" customHeight="1">
       <c r="B13" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12" customHeight="1">
@@ -2576,16 +2541,16 @@
         <v>27</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E14" s="28" t="s">
         <v>39</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="12" customHeight="1">
@@ -2597,18 +2562,18 @@
       </c>
       <c r="D15" s="46"/>
       <c r="E15" s="28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12" customHeight="1">
       <c r="B16" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>47</v>
@@ -2628,45 +2593,45 @@
         <v>29</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F17" s="29"/>
     </row>
     <row r="18" spans="2:6" ht="12" customHeight="1">
       <c r="B18" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C18" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="D18" s="31" t="s">
-        <v>157</v>
-      </c>
       <c r="E18" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="12" customHeight="1">
       <c r="B19" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C19" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="E19" s="52" t="s">
+        <v>540</v>
+      </c>
+      <c r="F19" s="28" t="s">
         <v>228</v>
-      </c>
-      <c r="E19" s="52" t="s">
-        <v>541</v>
-      </c>
-      <c r="F19" s="28" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="12" customHeight="1">
@@ -2674,165 +2639,165 @@
         <v>57</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F20" s="39"/>
     </row>
     <row r="21" spans="2:6" ht="12" customHeight="1">
       <c r="B21" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F21" s="39"/>
     </row>
     <row r="22" spans="2:6" ht="12" customHeight="1">
       <c r="B22" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F22" s="39"/>
     </row>
     <row r="23" spans="2:6" ht="12" customHeight="1">
       <c r="B23" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F23" s="39"/>
     </row>
     <row r="24" spans="2:6" ht="12" customHeight="1">
       <c r="B24" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C24" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F24" s="39"/>
     </row>
     <row r="25" spans="2:6" ht="12" customHeight="1">
       <c r="B25" s="27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F25" s="39"/>
     </row>
     <row r="26" spans="2:6" ht="12" customHeight="1">
       <c r="B26" s="27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F26" s="39"/>
     </row>
     <row r="27" spans="2:6" ht="12" customHeight="1">
       <c r="B27" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E27" s="39"/>
       <c r="F27" s="39"/>
     </row>
     <row r="28" spans="2:6" ht="12" customHeight="1">
       <c r="B28" s="27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D28" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E28" s="39"/>
       <c r="F28" s="39"/>
     </row>
     <row r="29" spans="2:6" ht="12" customHeight="1">
       <c r="B29" s="27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="39"/>
     </row>
     <row r="30" spans="2:6" ht="12" customHeight="1">
       <c r="B30" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D30" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="E30" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="E30" s="37" t="s">
-        <v>212</v>
-      </c>
       <c r="F30" s="28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="12" customHeight="1">
       <c r="B31" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C31" s="46"/>
       <c r="D31" s="28" t="s">
@@ -2856,7 +2821,7 @@
         <v>54</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F32" s="29"/>
     </row>
@@ -2868,10 +2833,10 @@
         <v>34</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F33" s="29"/>
     </row>
@@ -2886,40 +2851,40 @@
         <v>55</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F34" s="29"/>
     </row>
     <row r="35" spans="2:6" ht="12" customHeight="1">
       <c r="B35" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="28" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="2:6" ht="12" customHeight="1">
       <c r="B36" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C36" s="53" t="s">
+        <v>533</v>
+      </c>
+      <c r="D36" s="53" t="s">
         <v>534</v>
       </c>
-      <c r="D36" s="53" t="s">
-        <v>535</v>
-      </c>
       <c r="E36" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F36" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="12" customHeight="1">
@@ -2930,30 +2895,30 @@
         <v>7</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E37" s="28" t="s">
+        <v>303</v>
+      </c>
+      <c r="F37" s="28" t="s">
         <v>304</v>
-      </c>
-      <c r="F37" s="28" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="12" customHeight="1">
       <c r="B38" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D38" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="12" customHeight="1">
@@ -2963,24 +2928,24 @@
       <c r="C39" s="46"/>
       <c r="D39" s="46"/>
       <c r="E39" s="28" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="12" customHeight="1">
       <c r="B40" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F40" s="28" t="s">
         <v>18</v>
@@ -2988,101 +2953,101 @@
     </row>
     <row r="41" spans="2:6" ht="12" customHeight="1">
       <c r="B41" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="46"/>
     </row>
     <row r="42" spans="2:6" ht="12" customHeight="1">
       <c r="B42" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C42" s="35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D42" s="38"/>
       <c r="E42" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F42" s="52" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="12" customHeight="1">
       <c r="B43" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F43" s="36" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="12" customHeight="1">
       <c r="B44" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E44" s="46"/>
       <c r="F44" s="46"/>
     </row>
     <row r="45" spans="2:6" ht="12" customHeight="1">
       <c r="B45" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F45" s="52" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
       <c r="B46" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E46" s="46"/>
       <c r="F46" s="46"/>
     </row>
     <row r="47" spans="2:6" ht="12" customHeight="1">
       <c r="B47" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D47" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E47" s="46"/>
       <c r="F47" s="46"/>
@@ -3092,13 +3057,13 @@
         <v>42</v>
       </c>
       <c r="C48" s="40" t="s">
+        <v>471</v>
+      </c>
+      <c r="D48" s="40" t="s">
         <v>472</v>
       </c>
-      <c r="D48" s="40" t="s">
-        <v>473</v>
-      </c>
       <c r="E48" s="28" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F48" s="46"/>
     </row>
@@ -3107,97 +3072,97 @@
         <v>11</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E49" s="29"/>
       <c r="F49" s="29"/>
     </row>
     <row r="50" spans="2:6" ht="12" customHeight="1">
       <c r="B50" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C50" s="42" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F50" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="2:6" ht="12" customHeight="1">
       <c r="B51" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D51" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="E51" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="E51" s="28" t="s">
+      <c r="F51" s="28" t="s">
         <v>209</v>
-      </c>
-      <c r="F51" s="28" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="52" spans="2:6" ht="12" customHeight="1">
       <c r="B52" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="12" customHeight="1">
       <c r="B53" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="12" customHeight="1">
       <c r="B54" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C54" s="28" t="s">
         <v>41</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>40</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="12" customHeight="1">
@@ -3211,22 +3176,22 @@
         <v>23</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F55" s="52" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="12" customHeight="1">
       <c r="B56" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C56" s="35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D56" s="46"/>
       <c r="E56" s="36" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F56" s="38"/>
     </row>
@@ -3235,20 +3200,20 @@
         <v>43</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E57" s="29"/>
       <c r="F57" s="29"/>
     </row>
     <row r="58" spans="2:6" ht="12" customHeight="1">
       <c r="B58" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D58" s="29"/>
       <c r="E58" s="29"/>
@@ -3256,10 +3221,10 @@
     </row>
     <row r="59" spans="2:6" ht="12" customHeight="1">
       <c r="B59" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -3267,40 +3232,40 @@
     </row>
     <row r="60" spans="2:6" ht="12" customHeight="1">
       <c r="B60" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C60" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D60" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="E60" s="36" t="s">
         <v>90</v>
-      </c>
-      <c r="E60" s="36" t="s">
-        <v>91</v>
       </c>
       <c r="F60" s="38"/>
     </row>
     <row r="61" spans="2:6" ht="12" customHeight="1">
       <c r="B61" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C61" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D61" s="38"/>
       <c r="E61" s="36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F61" s="36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="2:6" ht="12" customHeight="1">
       <c r="B62" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C62" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D62" s="38"/>
       <c r="E62" s="38"/>
@@ -3308,10 +3273,10 @@
     </row>
     <row r="63" spans="2:6" ht="12" customHeight="1">
       <c r="B63" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D63" s="36" t="s">
         <v>13</v>
@@ -3321,27 +3286,27 @@
     </row>
     <row r="64" spans="2:6" ht="12" customHeight="1">
       <c r="B64" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C64" s="28" t="s">
         <v>9</v>
       </c>
       <c r="D64" s="28" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E64" s="52" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="12" customHeight="1">
       <c r="B65" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D65" s="28" t="s">
         <v>12</v>
@@ -3360,18 +3325,18 @@
         <v>44</v>
       </c>
       <c r="E66" s="52" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="12" customHeight="1">
       <c r="B67" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
@@ -3379,19 +3344,19 @@
     </row>
     <row r="68" spans="1:7" ht="12" customHeight="1">
       <c r="B68" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E68" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="F68" s="28" t="s">
         <v>232</v>
-      </c>
-      <c r="F68" s="28" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="12" customHeight="1">
@@ -3402,43 +3367,43 @@
         <v>5</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="12" customHeight="1">
       <c r="B70" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C70" s="42" t="s">
         <v>59</v>
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="28" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F70" s="29"/>
     </row>
     <row r="71" spans="1:7" ht="12" customHeight="1">
       <c r="B71" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D71" s="28" t="s">
         <v>3</v>
       </c>
       <c r="E71" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F71" s="52" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="12" customHeight="1">
@@ -3446,28 +3411,28 @@
         <v>19</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E72" s="28" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F72" s="28" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="12" customHeight="1">
       <c r="B73" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="52" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F73" s="28" t="s">
         <v>45</v>
@@ -3482,110 +3447,110 @@
         <v>14</v>
       </c>
       <c r="D74" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E74" s="28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F74" s="29"/>
       <c r="G74" s="1"/>
     </row>
     <row r="75" spans="1:7" ht="12" customHeight="1">
       <c r="B75" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D75" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="12" customHeight="1">
       <c r="B76" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D76" s="34" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E76" s="28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F76" s="28" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="12" customHeight="1">
       <c r="B77" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E77" s="28" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F77" s="46"/>
     </row>
     <row r="78" spans="1:7" ht="12" customHeight="1">
       <c r="B78" s="27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D78" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="E78" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="E78" s="28" t="s">
-        <v>136</v>
-      </c>
       <c r="F78" s="52" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="12" customHeight="1">
       <c r="B79" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C79" s="28" t="s">
+        <v>489</v>
+      </c>
+      <c r="D79" s="28" t="s">
         <v>490</v>
       </c>
-      <c r="D79" s="28" t="s">
-        <v>491</v>
-      </c>
       <c r="E79" s="28" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F79" s="46"/>
     </row>
     <row r="80" spans="1:7" ht="12" customHeight="1">
       <c r="B80" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E80" s="28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F80" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="81" spans="2:6" ht="12" customHeight="1">
@@ -3593,82 +3558,82 @@
         <v>10</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E81" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F81" s="28" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="82" spans="2:6" ht="12" customHeight="1">
       <c r="B82" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D82" s="28" t="s">
+        <v>509</v>
+      </c>
+      <c r="E82" s="28" t="s">
         <v>510</v>
-      </c>
-      <c r="E82" s="28" t="s">
-        <v>511</v>
       </c>
       <c r="F82" s="46"/>
     </row>
     <row r="83" spans="2:6" ht="12" customHeight="1">
       <c r="B83" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E83" s="28" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F83" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="84" spans="2:6" ht="12" customHeight="1">
       <c r="B84" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E84" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F84" s="28" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="85" spans="2:6" ht="12" customHeight="1">
       <c r="B85" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E85" s="28" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F85" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="86" spans="2:6" ht="12" customHeight="1">
@@ -3676,16 +3641,16 @@
         <v>17</v>
       </c>
       <c r="C86" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D86" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="D86" s="28" t="s">
+      <c r="E86" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="E86" s="28" t="s">
-        <v>81</v>
-      </c>
       <c r="F86" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="2:6" ht="12" customHeight="1">
@@ -3696,26 +3661,26 @@
         <v>60</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E87" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F87" s="52" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="12" customHeight="1">
       <c r="B88" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D88" s="46"/>
       <c r="E88" s="46"/>
       <c r="F88" s="28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="89" spans="2:6" ht="12" customHeight="1">
@@ -3723,34 +3688,34 @@
         <v>58</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D89" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E89" s="44"/>
       <c r="F89" s="28" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="90" spans="2:6" ht="12" customHeight="1">
       <c r="B90" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C90" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D90" s="46"/>
       <c r="E90" s="28" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F90" s="52" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="12" customHeight="1">
       <c r="B91" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C91" s="42" t="s">
         <v>56</v>
@@ -3761,23 +3726,23 @@
     </row>
     <row r="92" spans="2:6" ht="12" customHeight="1">
       <c r="B92" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C92" s="42" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D92" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E92" s="29"/>
       <c r="F92" s="29"/>
     </row>
     <row r="93" spans="2:6" ht="12" customHeight="1">
       <c r="B93" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D93" s="28" t="s">
         <v>61</v>
@@ -3786,37 +3751,37 @@
         <v>52</v>
       </c>
       <c r="F93" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="94" spans="2:6" ht="12" customHeight="1">
       <c r="B94" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="C94" s="28" t="s">
-        <v>62</v>
+        <v>113</v>
+      </c>
+      <c r="C94" s="52" t="s">
+        <v>550</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E94" s="29"/>
       <c r="F94" s="29"/>
     </row>
     <row r="95" spans="2:6" ht="12" customHeight="1">
       <c r="B95" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C95" s="35" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D95" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E95" s="36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F95" s="36" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="96" spans="2:6" ht="12" customHeight="1">
@@ -3824,46 +3789,46 @@
         <v>38</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D96" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E96" s="36" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F96" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="97" spans="2:6" ht="12" customHeight="1">
       <c r="B97" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D97" s="46"/>
       <c r="E97" s="46"/>
       <c r="F97" s="28" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="98" spans="2:6" ht="12" customHeight="1">
       <c r="B98" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F98" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="99" spans="2:6" ht="12" customHeight="1">
@@ -3908,26 +3873,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65536"/>
   <sheetViews>
     <sheetView topLeftCell="A139" workbookViewId="0">
       <selection activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13">
+    <row r="1" spans="1:11">
       <c r="A1" s="45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="50" customFormat="1">
@@ -3938,149 +3903,149 @@
         <v>8</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="48" customFormat="1">
       <c r="A3" s="48" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="48" customFormat="1">
       <c r="A4" s="48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="48" customFormat="1">
       <c r="A5" s="48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F5" s="48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G5" s="48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H5" s="48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I5" s="48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J5" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="48" customFormat="1">
       <c r="A6" s="48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B6" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="48" customFormat="1">
       <c r="A7" s="48" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B7" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="48" customFormat="1">
       <c r="A8" s="48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B8" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="48" customFormat="1">
       <c r="A9" s="48" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B9" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="48" customFormat="1">
       <c r="A10" s="48" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B10" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="48" customFormat="1">
       <c r="A11" s="48" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B11" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="48" customFormat="1">
       <c r="A12" s="48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B12" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="48" customFormat="1">
       <c r="A13" s="48" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B13" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K13" s="48" t="s">
         <v>27</v>
@@ -4088,68 +4053,68 @@
     </row>
     <row r="14" spans="1:11" s="48" customFormat="1">
       <c r="A14" s="48" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B14" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="48" customFormat="1">
       <c r="A15" s="48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B15" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="48" customFormat="1">
       <c r="A16" s="48" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B16" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="48" customFormat="1">
       <c r="A17" s="48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D17" s="48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="48" customFormat="1">
       <c r="A18" s="48" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B18" s="48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="48" customFormat="1">
       <c r="A19" s="48" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B19" s="48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C19" s="48" t="s">
         <v>54</v>
@@ -4158,39 +4123,39 @@
         <v>55</v>
       </c>
       <c r="E19" s="48" t="s">
+        <v>225</v>
+      </c>
+      <c r="F19" s="48" t="s">
         <v>226</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="48" customFormat="1">
       <c r="A20" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B20" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D20" s="48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E20" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="G20" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="H20" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="F20" s="48" t="s">
+      <c r="I20" s="48" t="s">
         <v>218</v>
-      </c>
-      <c r="G20" s="48" t="s">
-        <v>217</v>
-      </c>
-      <c r="H20" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="I20" s="48" t="s">
-        <v>219</v>
       </c>
       <c r="K20" s="48" t="s">
         <v>27</v>
@@ -4198,31 +4163,31 @@
     </row>
     <row r="21" spans="1:11" s="48" customFormat="1">
       <c r="A21" s="48" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B21" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E21" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="G21" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="H21" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="F21" s="48" t="s">
+      <c r="I21" s="48" t="s">
         <v>218</v>
-      </c>
-      <c r="G21" s="48" t="s">
-        <v>217</v>
-      </c>
-      <c r="H21" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="I21" s="48" t="s">
-        <v>219</v>
       </c>
       <c r="K21" s="48" t="s">
         <v>27</v>
@@ -4230,31 +4195,31 @@
     </row>
     <row r="22" spans="1:11" s="48" customFormat="1">
       <c r="A22" s="48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D22" s="48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E22" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="F22" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="G22" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="H22" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="F22" s="48" t="s">
+      <c r="I22" s="48" t="s">
         <v>218</v>
-      </c>
-      <c r="G22" s="48" t="s">
-        <v>217</v>
-      </c>
-      <c r="H22" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="I22" s="48" t="s">
-        <v>219</v>
       </c>
       <c r="K22" s="48" t="s">
         <v>27</v>
@@ -4262,31 +4227,31 @@
     </row>
     <row r="23" spans="1:11" s="48" customFormat="1">
       <c r="A23" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B23" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D23" s="48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E23" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="F23" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="G23" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="H23" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="I23" s="48" t="s">
         <v>218</v>
-      </c>
-      <c r="G23" s="48" t="s">
-        <v>217</v>
-      </c>
-      <c r="H23" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="I23" s="48" t="s">
-        <v>219</v>
       </c>
       <c r="K23" s="48" t="s">
         <v>27</v>
@@ -4294,45 +4259,45 @@
     </row>
     <row r="24" spans="1:11" s="48" customFormat="1">
       <c r="A24" s="48" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B24" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E24" s="48" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F24" s="48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G24" s="48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H24" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="I24" s="48" t="s">
         <v>80</v>
-      </c>
-      <c r="I24" s="48" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="48" customFormat="1">
       <c r="A25" s="48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B25" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K25" s="48" t="s">
         <v>27</v>
@@ -4340,24 +4305,24 @@
     </row>
     <row r="26" spans="1:11" s="48" customFormat="1">
       <c r="A26" s="48" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B26" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="48" customFormat="1">
       <c r="A27" s="48" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B27" s="48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C27" s="48" t="s">
         <v>54</v>
@@ -4366,67 +4331,67 @@
         <v>55</v>
       </c>
       <c r="E27" s="48" t="s">
+        <v>225</v>
+      </c>
+      <c r="F27" s="48" t="s">
         <v>226</v>
-      </c>
-      <c r="F27" s="48" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="48" customFormat="1">
       <c r="A28" s="48" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B28" s="48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="48" customFormat="1">
       <c r="A29" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B29" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E29" s="48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F29" s="48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="48" customFormat="1">
       <c r="A30" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B30" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E30" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="F30" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="G30" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="H30" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="F30" s="48" t="s">
+      <c r="I30" s="48" t="s">
         <v>218</v>
-      </c>
-      <c r="G30" s="48" t="s">
-        <v>217</v>
-      </c>
-      <c r="H30" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="I30" s="48" t="s">
-        <v>219</v>
       </c>
       <c r="K30" s="48" t="s">
         <v>27</v>
@@ -4434,31 +4399,31 @@
     </row>
     <row r="31" spans="1:11" s="48" customFormat="1">
       <c r="A31" s="48" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B31" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E31" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="F31" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="G31" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="H31" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="F31" s="48" t="s">
+      <c r="I31" s="48" t="s">
         <v>218</v>
-      </c>
-      <c r="G31" s="48" t="s">
-        <v>217</v>
-      </c>
-      <c r="H31" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="I31" s="48" t="s">
-        <v>219</v>
       </c>
       <c r="K31" s="48" t="s">
         <v>27</v>
@@ -4466,34 +4431,34 @@
     </row>
     <row r="32" spans="1:11" s="48" customFormat="1">
       <c r="A32" s="48" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B32" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C32" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E32" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="F32" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="G32" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="H32" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="F32" s="48" t="s">
+      <c r="I32" s="48" t="s">
         <v>218</v>
       </c>
-      <c r="G32" s="48" t="s">
-        <v>217</v>
-      </c>
-      <c r="H32" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="I32" s="48" t="s">
-        <v>219</v>
-      </c>
       <c r="J32" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K32" s="48" t="s">
         <v>27</v>
@@ -4501,31 +4466,31 @@
     </row>
     <row r="33" spans="1:11" s="48" customFormat="1">
       <c r="A33" s="48" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B33" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C33" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E33" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="F33" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="G33" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="H33" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="F33" s="48" t="s">
+      <c r="I33" s="48" t="s">
         <v>218</v>
-      </c>
-      <c r="G33" s="48" t="s">
-        <v>217</v>
-      </c>
-      <c r="H33" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="I33" s="48" t="s">
-        <v>219</v>
       </c>
       <c r="K33" s="48" t="s">
         <v>27</v>
@@ -4533,167 +4498,167 @@
     </row>
     <row r="34" spans="1:11" s="48" customFormat="1">
       <c r="A34" s="48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B34" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="48" customFormat="1">
       <c r="A35" s="48" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B35" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="48" customFormat="1">
       <c r="A36" s="48" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B36" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="48" customFormat="1">
       <c r="A37" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B37" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C37" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="48" customFormat="1">
       <c r="A38" s="48" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B38" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="48" customFormat="1">
       <c r="A39" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B39" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C39" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="48" customFormat="1">
       <c r="A40" s="48" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B40" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C40" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="48" customFormat="1">
       <c r="A41" s="48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B41" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C41" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="48" customFormat="1">
       <c r="A42" s="48" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B42" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C42" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="48" customFormat="1">
       <c r="A43" s="48" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B43" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C43" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="48" customFormat="1">
       <c r="A44" s="48" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B44" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C44" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="48" customFormat="1">
       <c r="A45" s="48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B45" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C45" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:11" s="48" customFormat="1">
       <c r="A46" s="48" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B46" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C46" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:11" s="48" customFormat="1">
       <c r="A47" s="48" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B47" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="48" customFormat="1">
       <c r="A48" s="48" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B48" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:11" s="48" customFormat="1">
@@ -4704,18 +4669,18 @@
         <v>4</v>
       </c>
       <c r="C49" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:11" s="48" customFormat="1">
       <c r="A50" s="48" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B50" s="48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K50" s="48" t="s">
         <v>27</v>
@@ -4723,24 +4688,24 @@
     </row>
     <row r="51" spans="1:11" s="48" customFormat="1">
       <c r="A51" s="48" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B51" s="48" t="s">
         <v>19</v>
       </c>
       <c r="C51" s="48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:11" s="48" customFormat="1">
       <c r="A52" s="48" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B52" s="48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C52" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K52" s="48" t="s">
         <v>27</v>
@@ -4748,27 +4713,27 @@
     </row>
     <row r="53" spans="1:11" s="48" customFormat="1">
       <c r="A53" s="48" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B53" s="48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C53" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="48" customFormat="1">
       <c r="A54" s="48" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B54" s="48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C54" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K54" s="48" t="s">
         <v>27</v>
@@ -4776,24 +4741,24 @@
     </row>
     <row r="55" spans="1:11" s="48" customFormat="1">
       <c r="A55" s="48" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B55" s="48" t="s">
         <v>19</v>
       </c>
       <c r="C55" s="48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:11" s="48" customFormat="1">
       <c r="A56" s="48" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B56" s="48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C56" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K56" s="48" t="s">
         <v>27</v>
@@ -4801,13 +4766,13 @@
     </row>
     <row r="57" spans="1:11" s="48" customFormat="1">
       <c r="A57" s="48" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B57" s="48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C57" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K57" s="48" t="s">
         <v>27</v>
@@ -4815,35 +4780,35 @@
     </row>
     <row r="58" spans="1:11" s="48" customFormat="1">
       <c r="A58" s="48" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B58" s="48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C58" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="48" customFormat="1">
       <c r="A59" s="48" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B59" s="48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C59" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="48" customFormat="1">
       <c r="A60" s="48" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B60" s="48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C60" s="48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K60" s="48" t="s">
         <v>27</v>
@@ -4851,35 +4816,35 @@
     </row>
     <row r="61" spans="1:11" s="48" customFormat="1">
       <c r="A61" s="48" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B61" s="48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C61" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="48" customFormat="1">
       <c r="A62" s="48" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B62" s="48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C62" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:11" s="48" customFormat="1">
       <c r="A63" s="48" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B63" s="48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C63" s="48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K63" s="48" t="s">
         <v>27</v>
@@ -4887,110 +4852,110 @@
     </row>
     <row r="64" spans="1:11" s="48" customFormat="1">
       <c r="A64" s="48" t="s">
+        <v>333</v>
+      </c>
+      <c r="B64" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="C64" s="48" t="s">
         <v>334</v>
-      </c>
-      <c r="B64" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="C64" s="48" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="65" spans="1:11" s="48" customFormat="1">
       <c r="A65" s="48" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B65" s="48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C65" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="66" spans="1:11" s="48" customFormat="1">
       <c r="A66" s="48" t="s">
+        <v>391</v>
+      </c>
+      <c r="B66" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="C66" s="48" t="s">
         <v>392</v>
-      </c>
-      <c r="B66" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="C66" s="48" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="48" customFormat="1">
       <c r="A67" s="48" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B67" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C67" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="D67" s="48" t="s">
         <v>239</v>
-      </c>
-      <c r="D67" s="48" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="68" spans="1:11" s="48" customFormat="1">
       <c r="A68" s="48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B68" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C68" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="D68" s="48" t="s">
         <v>239</v>
-      </c>
-      <c r="D68" s="48" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="48" customFormat="1">
       <c r="A69" s="48" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B69" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C69" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="D69" s="48" t="s">
         <v>239</v>
-      </c>
-      <c r="D69" s="48" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="48" customFormat="1">
       <c r="A70" s="48" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B70" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C70" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="D70" s="48" t="s">
         <v>239</v>
-      </c>
-      <c r="D70" s="48" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="71" spans="1:11" s="48" customFormat="1">
       <c r="A71" s="48" t="s">
+        <v>335</v>
+      </c>
+      <c r="B71" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C71" s="48" t="s">
         <v>336</v>
       </c>
-      <c r="B71" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="C71" s="48" t="s">
-        <v>337</v>
-      </c>
       <c r="D71" s="48" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="72" spans="1:11" s="48" customFormat="1">
       <c r="A72" s="48" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B72" s="48" t="s">
         <v>15</v>
@@ -5001,16 +4966,16 @@
     </row>
     <row r="73" spans="1:11" s="48" customFormat="1">
       <c r="A73" s="48" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B73" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C73" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="D73" s="48" t="s">
         <v>239</v>
-      </c>
-      <c r="D73" s="48" t="s">
-        <v>240</v>
       </c>
       <c r="K73" s="48" t="s">
         <v>27</v>
@@ -5018,108 +4983,108 @@
     </row>
     <row r="74" spans="1:11" s="48" customFormat="1">
       <c r="A74" s="48" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B74" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C74" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="D74" s="48" t="s">
         <v>239</v>
-      </c>
-      <c r="D74" s="48" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="75" spans="1:11" s="48" customFormat="1">
       <c r="A75" s="48" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B75" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C75" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="D75" s="48" t="s">
         <v>239</v>
-      </c>
-      <c r="D75" s="48" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="48" customFormat="1">
       <c r="A76" s="48" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B76" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C76" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="D76" s="48" t="s">
         <v>239</v>
-      </c>
-      <c r="D76" s="48" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="48" customFormat="1">
       <c r="A77" s="48" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B77" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C77" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="D77" s="48" t="s">
         <v>239</v>
-      </c>
-      <c r="D77" s="48" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="48" customFormat="1">
       <c r="A78" s="48" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B78" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C78" s="48" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="48" customFormat="1">
       <c r="A79" s="48" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B79" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C79" s="48" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="80" spans="1:11" s="48" customFormat="1">
       <c r="A80" s="48" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B80" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C80" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="D80" s="48" t="s">
         <v>239</v>
-      </c>
-      <c r="D80" s="48" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="81" spans="1:11" s="48" customFormat="1">
       <c r="A81" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="B81" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="C81" s="48" t="s">
         <v>264</v>
       </c>
-      <c r="B81" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="C81" s="48" t="s">
-        <v>265</v>
-      </c>
       <c r="D81" s="48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K81" s="48" t="s">
         <v>27</v>
@@ -5127,76 +5092,76 @@
     </row>
     <row r="82" spans="1:11" s="48" customFormat="1">
       <c r="A82" s="48" t="s">
+        <v>307</v>
+      </c>
+      <c r="B82" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C82" s="48" t="s">
         <v>308</v>
       </c>
-      <c r="B82" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="C82" s="48" t="s">
-        <v>309</v>
-      </c>
       <c r="D82" s="48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E82" s="48" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="83" spans="1:11" s="48" customFormat="1">
       <c r="A83" s="49" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B83" s="48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C83" s="48" t="s">
         <v>14</v>
       </c>
       <c r="D83" s="48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K83" s="48" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="84" spans="1:11" s="48" customFormat="1">
       <c r="A84" s="48" t="s">
+        <v>270</v>
+      </c>
+      <c r="B84" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" s="48" t="s">
         <v>271</v>
       </c>
-      <c r="B84" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="C84" s="48" t="s">
-        <v>272</v>
-      </c>
       <c r="D84" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="E84" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="E84" s="48" t="s">
-        <v>295</v>
-      </c>
       <c r="F84" s="48" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G84" s="48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:11" s="48" customFormat="1">
       <c r="A85" s="48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B85" s="48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C85" s="48" t="s">
+        <v>193</v>
+      </c>
+      <c r="D85" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="D85" s="48" t="s">
-        <v>195</v>
-      </c>
       <c r="E85" s="48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K85" s="48" t="s">
         <v>27</v>
@@ -5204,88 +5169,88 @@
     </row>
     <row r="86" spans="1:11" s="48" customFormat="1">
       <c r="A86" s="48" t="s">
+        <v>267</v>
+      </c>
+      <c r="B86" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="C86" s="48" t="s">
         <v>268</v>
       </c>
-      <c r="B86" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="C86" s="48" t="s">
-        <v>269</v>
-      </c>
       <c r="D86" s="48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E86" s="48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F86" s="48" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G86" s="48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K86" s="48" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="87" spans="1:11" s="48" customFormat="1">
       <c r="A87" s="48" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B87" s="48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C87" s="48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D87" s="48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E87" s="48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F87" s="48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K87" s="48" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="88" spans="1:11" s="48" customFormat="1">
       <c r="A88" s="49" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B88" s="48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C88" s="48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D88" s="48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E88" s="48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F88" s="48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K88" s="48" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="89" spans="1:11" s="47" customFormat="1">
       <c r="A89" s="47" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B89" s="47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C89" s="47" t="s">
         <v>20</v>
       </c>
       <c r="D89" s="47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K89" s="47" t="s">
         <v>27</v>
@@ -5293,32 +5258,32 @@
     </row>
     <row r="90" spans="1:11" s="48" customFormat="1">
       <c r="A90" s="48" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B90" s="48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="91" spans="1:11" s="48" customFormat="1">
       <c r="A91" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B91" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C91" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="92" spans="1:11" s="48" customFormat="1">
       <c r="A92" s="48" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B92" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C92" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K92" s="48" t="s">
         <v>27</v>
@@ -5326,38 +5291,38 @@
     </row>
     <row r="93" spans="1:11" s="48" customFormat="1">
       <c r="A93" s="49" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B93" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C93" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K93" s="48" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="94" spans="1:11" s="48" customFormat="1">
       <c r="A94" s="48" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B94" s="48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C94" s="48" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="95" spans="1:11" s="48" customFormat="1">
       <c r="A95" s="48" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B95" s="48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C95" s="48" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="96" spans="1:11" s="50" customFormat="1">
@@ -5365,517 +5330,517 @@
         <v>22</v>
       </c>
       <c r="B96" s="50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C96" s="50" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="48" customFormat="1">
       <c r="A97" s="48" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B97" s="48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C97" s="48" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="48" customFormat="1">
       <c r="A98" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B98" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C98" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D98" s="48" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E98" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="48" customFormat="1">
       <c r="A99" s="48" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B99" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C99" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="48" customFormat="1">
       <c r="A100" s="48" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B100" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C100" s="48" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="48" customFormat="1">
       <c r="A101" s="48" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B101" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C101" s="48" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C102" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C103" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C104" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C105" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C106" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C107" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C108" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B109" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C109" s="48" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B110" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C110" s="48" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B111" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C111" s="48" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B112" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C112" s="48" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B113" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C113" s="48" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B114" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C114" s="48" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B115" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
+        <v>422</v>
+      </c>
+      <c r="B116" t="s">
+        <v>142</v>
+      </c>
+      <c r="C116" s="48" t="s">
         <v>423</v>
-      </c>
-      <c r="B116" t="s">
-        <v>143</v>
-      </c>
-      <c r="C116" s="48" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B117" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B118" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B119" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C119" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B120" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B121" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B122" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C122" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B123" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C123" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B124" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C124" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B125" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C125" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="126" spans="1:3" s="48" customFormat="1">
       <c r="A126" s="48" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B126" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C126" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="127" spans="1:3" s="48" customFormat="1">
       <c r="A127" s="48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B127" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C127" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="128" spans="1:3" s="48" customFormat="1">
       <c r="A128" s="48" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B128" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C128" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="129" spans="1:3" s="48" customFormat="1">
       <c r="A129" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B129" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C129" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="130" spans="1:3" s="48" customFormat="1">
       <c r="A130" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B130" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C130" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="131" spans="1:3" s="48" customFormat="1">
       <c r="A131" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B131" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C131" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="132" spans="1:3" s="48" customFormat="1">
       <c r="A132" s="48" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B132" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C132" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="133" spans="1:3" s="48" customFormat="1">
       <c r="A133" s="48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B133" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C133" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="134" spans="1:3" s="48" customFormat="1">
       <c r="A134" s="48" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B134" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C134" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="135" spans="1:3" s="48" customFormat="1">
       <c r="A135" s="48" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B135" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C135" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="136" spans="1:3" s="48" customFormat="1">
       <c r="A136" s="48" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B136" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C136" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="137" spans="1:3" s="48" customFormat="1">
       <c r="A137" s="48" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B137" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C137" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="138" spans="1:3" s="48" customFormat="1">
       <c r="A138" s="48" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B138" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C138" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="139" spans="1:3" s="48" customFormat="1">
       <c r="A139" s="48" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B139" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C139" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="140" spans="1:3" s="48" customFormat="1">
       <c r="A140" s="48" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B140" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C140" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="141" spans="1:3" s="48" customFormat="1">
       <c r="A141" s="48" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B141" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C141" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="142" spans="1:3" s="48" customFormat="1">
       <c r="A142" s="48" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B142" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C142" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="48" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B143" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="48" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B144" s="48" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65536" spans="3:3">
@@ -5890,18 +5855,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5911,20 +5876,20 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B8" t="s">
         <v>380</v>
-      </c>
-      <c r="B8" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Matlab does not support char input to `vpa` anymore
`str2sym` needs to be applied to the first input of `vpa+  in Matlab.  On the other hand, Octave does not have `str2sym`, and allows char input to `vpa`. This is handled by the compiler by using `vpa(str2sym(...), ...)` in the compiled code but defining `str2sym` as the identity function in Octave
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Dropbox\MATL\spec\functionTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2C8ED0-996E-4AFA-A023-3578D9E7D8B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="16515" windowHeight="8760"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -908,9 +909,6 @@
     <t>setdiff, but I don't think it will be used</t>
   </si>
   <si>
-    <t>char(vpa(...))</t>
-  </si>
-  <si>
     <t>Paste from clipboard H</t>
   </si>
   <si>
@@ -1674,12 +1672,15 @@
   </si>
   <si>
     <t>nnz / cellfun(@nnz, ...)</t>
+  </si>
+  <si>
+    <t>char(vpa(str2sym(…), ...))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="17">
     <font>
       <sz val="10"/>
@@ -2095,6 +2096,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2130,6 +2148,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2305,25 +2340,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F98" sqref="F98"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="2.85546875" style="13" customWidth="1"/>
-    <col min="3" max="5" width="32.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" customWidth="1"/>
-    <col min="8" max="12" width="23.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="7.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.81640625" style="13" customWidth="1"/>
+    <col min="3" max="5" width="32.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="32.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" style="1" customWidth="1"/>
+    <col min="8" max="12" width="23.7265625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" customHeight="1">
@@ -2391,7 +2426,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>91</v>
@@ -2414,10 +2449,10 @@
         <v>16</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -2429,10 +2464,10 @@
         <v>188</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>257</v>
@@ -2447,7 +2482,7 @@
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="9" t="s">
-        <v>295</v>
+        <v>550</v>
       </c>
       <c r="F8" s="43" t="s">
         <v>256</v>
@@ -2475,13 +2510,13 @@
         <v>37</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>149</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F10" s="28" t="s">
         <v>214</v>
@@ -2492,14 +2527,14 @@
         <v>158</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="28" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="12" customHeight="1">
@@ -2507,16 +2542,16 @@
         <v>108</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12" customHeight="1">
@@ -2524,16 +2559,16 @@
         <v>109</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12" customHeight="1">
@@ -2565,7 +2600,7 @@
         <v>190</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12" customHeight="1">
@@ -2573,7 +2608,7 @@
         <v>102</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>47</v>
@@ -2628,7 +2663,7 @@
         <v>227</v>
       </c>
       <c r="E19" s="52" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F19" s="28" t="s">
         <v>228</v>
@@ -2642,10 +2677,10 @@
         <v>184</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F20" s="39"/>
     </row>
@@ -2657,10 +2692,10 @@
         <v>184</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F21" s="39"/>
     </row>
@@ -2672,10 +2707,10 @@
         <v>184</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F22" s="39"/>
     </row>
@@ -2687,10 +2722,10 @@
         <v>184</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F23" s="39"/>
     </row>
@@ -2702,10 +2737,10 @@
         <v>184</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F24" s="39"/>
     </row>
@@ -2717,10 +2752,10 @@
         <v>184</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F25" s="39"/>
     </row>
@@ -2732,10 +2767,10 @@
         <v>184</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F26" s="39"/>
     </row>
@@ -2747,7 +2782,7 @@
         <v>184</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E27" s="39"/>
       <c r="F27" s="39"/>
@@ -2760,7 +2795,7 @@
         <v>184</v>
       </c>
       <c r="D28" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E28" s="39"/>
       <c r="F28" s="39"/>
@@ -2773,7 +2808,7 @@
         <v>184</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="39"/>
@@ -2783,7 +2818,7 @@
         <v>169</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>210</v>
@@ -2864,7 +2899,7 @@
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="28" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F35" s="28" t="s">
         <v>97</v>
@@ -2875,10 +2910,10 @@
         <v>104</v>
       </c>
       <c r="C36" s="53" t="s">
+        <v>532</v>
+      </c>
+      <c r="D36" s="53" t="s">
         <v>533</v>
-      </c>
-      <c r="D36" s="53" t="s">
-        <v>534</v>
       </c>
       <c r="E36" s="28" t="s">
         <v>86</v>
@@ -2895,13 +2930,13 @@
         <v>7</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E37" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="F37" s="28" t="s">
         <v>303</v>
-      </c>
-      <c r="F37" s="28" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="12" customHeight="1">
@@ -2909,16 +2944,16 @@
         <v>170</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D38" s="28" t="s">
         <v>247</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="12" customHeight="1">
@@ -2928,10 +2963,10 @@
       <c r="C39" s="46"/>
       <c r="D39" s="46"/>
       <c r="E39" s="28" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="12" customHeight="1">
@@ -2939,13 +2974,13 @@
         <v>127</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F40" s="28" t="s">
         <v>18</v>
@@ -2956,10 +2991,10 @@
         <v>171</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="46"/>
@@ -2973,10 +3008,10 @@
       </c>
       <c r="D42" s="38"/>
       <c r="E42" s="28" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F42" s="52" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="12" customHeight="1">
@@ -2984,16 +3019,16 @@
         <v>137</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D43" s="28" t="s">
         <v>99</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F43" s="36" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="12" customHeight="1">
@@ -3001,7 +3036,7 @@
         <v>124</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D44" s="40" t="s">
         <v>245</v>
@@ -3014,16 +3049,16 @@
         <v>96</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D45" s="40" t="s">
         <v>244</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F45" s="52" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
@@ -3031,7 +3066,7 @@
         <v>133</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D46" s="40" t="s">
         <v>243</v>
@@ -3044,7 +3079,7 @@
         <v>142</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D47" s="40" t="s">
         <v>242</v>
@@ -3057,13 +3092,13 @@
         <v>42</v>
       </c>
       <c r="C48" s="40" t="s">
+        <v>470</v>
+      </c>
+      <c r="D48" s="40" t="s">
         <v>471</v>
       </c>
-      <c r="D48" s="40" t="s">
-        <v>472</v>
-      </c>
       <c r="E48" s="28" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F48" s="46"/>
     </row>
@@ -3072,10 +3107,10 @@
         <v>11</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E49" s="29"/>
       <c r="F49" s="29"/>
@@ -3088,7 +3123,7 @@
         <v>203</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>202</v>
@@ -3102,7 +3137,7 @@
         <v>131</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D51" s="28" t="s">
         <v>207</v>
@@ -3122,10 +3157,10 @@
         <v>71</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F52" s="28" t="s">
         <v>239</v>
@@ -3136,16 +3171,16 @@
         <v>120</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="12" customHeight="1">
@@ -3156,13 +3191,13 @@
         <v>41</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>40</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="12" customHeight="1">
@@ -3179,7 +3214,7 @@
         <v>195</v>
       </c>
       <c r="F55" s="52" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="12" customHeight="1">
@@ -3200,7 +3235,7 @@
         <v>43</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D57" s="28" t="s">
         <v>141</v>
@@ -3224,7 +3259,7 @@
         <v>145</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -3276,7 +3311,7 @@
         <v>175</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D63" s="36" t="s">
         <v>13</v>
@@ -3295,10 +3330,10 @@
         <v>233</v>
       </c>
       <c r="E64" s="52" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="12" customHeight="1">
@@ -3325,10 +3360,10 @@
         <v>44</v>
       </c>
       <c r="E66" s="52" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="12" customHeight="1">
@@ -3336,7 +3371,7 @@
         <v>92</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
@@ -3347,10 +3382,10 @@
         <v>105</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E68" s="28" t="s">
         <v>231</v>
@@ -3367,13 +3402,13 @@
         <v>5</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="12" customHeight="1">
@@ -3394,7 +3429,7 @@
         <v>74</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D71" s="28" t="s">
         <v>3</v>
@@ -3403,7 +3438,7 @@
         <v>140</v>
       </c>
       <c r="F71" s="52" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="12" customHeight="1">
@@ -3414,13 +3449,13 @@
         <v>125</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E72" s="28" t="s">
         <v>241</v>
       </c>
       <c r="F72" s="28" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="12" customHeight="1">
@@ -3428,11 +3463,11 @@
         <v>178</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="52" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F73" s="28" t="s">
         <v>45</v>
@@ -3460,16 +3495,16 @@
         <v>130</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D75" s="28" t="s">
         <v>72</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="12" customHeight="1">
@@ -3500,7 +3535,7 @@
         <v>230</v>
       </c>
       <c r="E77" s="28" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F77" s="46"/>
     </row>
@@ -3518,7 +3553,7 @@
         <v>135</v>
       </c>
       <c r="F78" s="52" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="12" customHeight="1">
@@ -3526,13 +3561,13 @@
         <v>118</v>
       </c>
       <c r="C79" s="28" t="s">
+        <v>488</v>
+      </c>
+      <c r="D79" s="28" t="s">
         <v>489</v>
       </c>
-      <c r="D79" s="28" t="s">
-        <v>490</v>
-      </c>
       <c r="E79" s="28" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F79" s="46"/>
     </row>
@@ -3544,7 +3579,7 @@
         <v>283</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E80" s="28" t="s">
         <v>259</v>
@@ -3561,13 +3596,13 @@
         <v>126</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E81" s="28" t="s">
         <v>225</v>
       </c>
       <c r="F81" s="28" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="82" spans="2:6" ht="12" customHeight="1">
@@ -3575,13 +3610,13 @@
         <v>65</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D82" s="28" t="s">
+        <v>508</v>
+      </c>
+      <c r="E82" s="28" t="s">
         <v>509</v>
-      </c>
-      <c r="E82" s="28" t="s">
-        <v>510</v>
       </c>
       <c r="F82" s="46"/>
     </row>
@@ -3590,13 +3625,13 @@
         <v>77</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>75</v>
       </c>
       <c r="E83" s="28" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F83" s="28" t="s">
         <v>153</v>
@@ -3610,13 +3645,13 @@
         <v>62</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E84" s="28" t="s">
         <v>64</v>
       </c>
       <c r="F84" s="28" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="85" spans="2:6" ht="12" customHeight="1">
@@ -3624,13 +3659,13 @@
         <v>119</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E85" s="28" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F85" s="28" t="s">
         <v>87</v>
@@ -3661,13 +3696,13 @@
         <v>60</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E87" s="28" t="s">
         <v>63</v>
       </c>
       <c r="F87" s="52" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="12" customHeight="1">
@@ -3675,7 +3710,7 @@
         <v>128</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D88" s="46"/>
       <c r="E88" s="46"/>
@@ -3707,10 +3742,10 @@
       </c>
       <c r="D90" s="46"/>
       <c r="E90" s="28" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F90" s="52" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="12" customHeight="1">
@@ -3742,7 +3777,7 @@
         <v>146</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D93" s="28" t="s">
         <v>61</v>
@@ -3759,10 +3794,10 @@
         <v>113</v>
       </c>
       <c r="C94" s="52" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E94" s="29"/>
       <c r="F94" s="29"/>
@@ -3772,7 +3807,7 @@
         <v>180</v>
       </c>
       <c r="C95" s="35" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D95" s="36" t="s">
         <v>139</v>
@@ -3789,13 +3824,13 @@
         <v>38</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D96" s="28" t="s">
         <v>147</v>
       </c>
       <c r="E96" s="36" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F96" s="28" t="s">
         <v>217</v>
@@ -3806,12 +3841,12 @@
         <v>181</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D97" s="46"/>
       <c r="E97" s="46"/>
       <c r="F97" s="28" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="98" spans="2:6" ht="12" customHeight="1">
@@ -3867,27 +3902,27 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="31" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="32" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K65536"/>
   <sheetViews>
     <sheetView topLeftCell="A139" workbookViewId="0">
       <selection activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" ht="13">
       <c r="A1" s="45" t="s">
         <v>276</v>
       </c>
@@ -3908,7 +3943,7 @@
     </row>
     <row r="3" spans="1:11" s="48" customFormat="1">
       <c r="A3" s="48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>8</v>
@@ -3919,7 +3954,7 @@
     </row>
     <row r="4" spans="1:11" s="48" customFormat="1">
       <c r="A4" s="48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>8</v>
@@ -3942,7 +3977,7 @@
         <v>282</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F5" s="48" t="s">
         <v>219</v>
@@ -3962,7 +3997,7 @@
     </row>
     <row r="6" spans="1:11" s="48" customFormat="1">
       <c r="A6" s="48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B6" s="48" t="s">
         <v>8</v>
@@ -3973,7 +4008,7 @@
     </row>
     <row r="7" spans="1:11" s="48" customFormat="1">
       <c r="A7" s="48" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B7" s="48" t="s">
         <v>8</v>
@@ -3984,7 +4019,7 @@
     </row>
     <row r="8" spans="1:11" s="48" customFormat="1">
       <c r="A8" s="48" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B8" s="48" t="s">
         <v>8</v>
@@ -3995,7 +4030,7 @@
     </row>
     <row r="9" spans="1:11" s="48" customFormat="1">
       <c r="A9" s="48" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B9" s="48" t="s">
         <v>8</v>
@@ -4006,7 +4041,7 @@
     </row>
     <row r="10" spans="1:11" s="48" customFormat="1">
       <c r="A10" s="48" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B10" s="48" t="s">
         <v>8</v>
@@ -4017,7 +4052,7 @@
     </row>
     <row r="11" spans="1:11" s="48" customFormat="1">
       <c r="A11" s="48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B11" s="48" t="s">
         <v>8</v>
@@ -4028,7 +4063,7 @@
     </row>
     <row r="12" spans="1:11" s="48" customFormat="1">
       <c r="A12" s="48" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B12" s="48" t="s">
         <v>8</v>
@@ -4039,7 +4074,7 @@
     </row>
     <row r="13" spans="1:11" s="48" customFormat="1">
       <c r="A13" s="48" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B13" s="48" t="s">
         <v>8</v>
@@ -4053,7 +4088,7 @@
     </row>
     <row r="14" spans="1:11" s="48" customFormat="1">
       <c r="A14" s="48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B14" s="48" t="s">
         <v>8</v>
@@ -4064,7 +4099,7 @@
     </row>
     <row r="15" spans="1:11" s="48" customFormat="1">
       <c r="A15" s="48" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B15" s="48" t="s">
         <v>8</v>
@@ -4075,7 +4110,7 @@
     </row>
     <row r="16" spans="1:11" s="48" customFormat="1">
       <c r="A16" s="48" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B16" s="48" t="s">
         <v>8</v>
@@ -4092,7 +4127,7 @@
         <v>170</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D17" s="48" t="s">
         <v>219</v>
@@ -4100,13 +4135,13 @@
     </row>
     <row r="18" spans="1:11" s="48" customFormat="1">
       <c r="A18" s="48" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B18" s="48" t="s">
         <v>115</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="48" customFormat="1">
@@ -4294,7 +4329,7 @@
         <v>170</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D25" s="48" t="s">
         <v>219</v>
@@ -4305,7 +4340,7 @@
     </row>
     <row r="26" spans="1:11" s="48" customFormat="1">
       <c r="A26" s="48" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B26" s="48" t="s">
         <v>170</v>
@@ -4339,7 +4374,7 @@
     </row>
     <row r="28" spans="1:11" s="48" customFormat="1">
       <c r="A28" s="48" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B28" s="48" t="s">
         <v>115</v>
@@ -4498,7 +4533,7 @@
     </row>
     <row r="34" spans="1:11" s="48" customFormat="1">
       <c r="A34" s="48" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B34" s="48" t="s">
         <v>4</v>
@@ -4509,7 +4544,7 @@
     </row>
     <row r="35" spans="1:11" s="48" customFormat="1">
       <c r="A35" s="48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B35" s="48" t="s">
         <v>4</v>
@@ -4520,7 +4555,7 @@
     </row>
     <row r="36" spans="1:11" s="48" customFormat="1">
       <c r="A36" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B36" s="48" t="s">
         <v>4</v>
@@ -4531,7 +4566,7 @@
     </row>
     <row r="37" spans="1:11" s="48" customFormat="1">
       <c r="A37" s="48" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B37" s="48" t="s">
         <v>4</v>
@@ -4542,7 +4577,7 @@
     </row>
     <row r="38" spans="1:11" s="48" customFormat="1">
       <c r="A38" s="48" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B38" s="48" t="s">
         <v>4</v>
@@ -4553,7 +4588,7 @@
     </row>
     <row r="39" spans="1:11" s="48" customFormat="1">
       <c r="A39" s="48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B39" s="48" t="s">
         <v>4</v>
@@ -4564,7 +4599,7 @@
     </row>
     <row r="40" spans="1:11" s="48" customFormat="1">
       <c r="A40" s="48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B40" s="48" t="s">
         <v>4</v>
@@ -4575,7 +4610,7 @@
     </row>
     <row r="41" spans="1:11" s="48" customFormat="1">
       <c r="A41" s="48" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B41" s="48" t="s">
         <v>4</v>
@@ -4586,7 +4621,7 @@
     </row>
     <row r="42" spans="1:11" s="48" customFormat="1">
       <c r="A42" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B42" s="48" t="s">
         <v>4</v>
@@ -4597,7 +4632,7 @@
     </row>
     <row r="43" spans="1:11" s="48" customFormat="1">
       <c r="A43" s="48" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B43" s="48" t="s">
         <v>4</v>
@@ -4608,7 +4643,7 @@
     </row>
     <row r="44" spans="1:11" s="48" customFormat="1">
       <c r="A44" s="48" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B44" s="48" t="s">
         <v>4</v>
@@ -4619,7 +4654,7 @@
     </row>
     <row r="45" spans="1:11" s="48" customFormat="1">
       <c r="A45" s="48" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B45" s="48" t="s">
         <v>4</v>
@@ -4630,7 +4665,7 @@
     </row>
     <row r="46" spans="1:11" s="48" customFormat="1">
       <c r="A46" s="48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B46" s="48" t="s">
         <v>4</v>
@@ -4641,7 +4676,7 @@
     </row>
     <row r="47" spans="1:11" s="48" customFormat="1">
       <c r="A47" s="48" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B47" s="48" t="s">
         <v>4</v>
@@ -4652,7 +4687,7 @@
     </row>
     <row r="48" spans="1:11" s="48" customFormat="1">
       <c r="A48" s="48" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B48" s="48" t="s">
         <v>4</v>
@@ -4674,7 +4709,7 @@
     </row>
     <row r="50" spans="1:11" s="48" customFormat="1">
       <c r="A50" s="48" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B50" s="48" t="s">
         <v>127</v>
@@ -4688,7 +4723,7 @@
     </row>
     <row r="51" spans="1:11" s="48" customFormat="1">
       <c r="A51" s="48" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B51" s="48" t="s">
         <v>19</v>
@@ -4699,7 +4734,7 @@
     </row>
     <row r="52" spans="1:11" s="48" customFormat="1">
       <c r="A52" s="48" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B52" s="48" t="s">
         <v>127</v>
@@ -4713,7 +4748,7 @@
     </row>
     <row r="53" spans="1:11" s="48" customFormat="1">
       <c r="A53" s="48" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B53" s="48" t="s">
         <v>127</v>
@@ -4724,7 +4759,7 @@
     </row>
     <row r="54" spans="1:11" s="48" customFormat="1">
       <c r="A54" s="48" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B54" s="48" t="s">
         <v>127</v>
@@ -4733,7 +4768,7 @@
         <v>89</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K54" s="48" t="s">
         <v>27</v>
@@ -4741,7 +4776,7 @@
     </row>
     <row r="55" spans="1:11" s="48" customFormat="1">
       <c r="A55" s="48" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B55" s="48" t="s">
         <v>19</v>
@@ -4752,7 +4787,7 @@
     </row>
     <row r="56" spans="1:11" s="48" customFormat="1">
       <c r="A56" s="48" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B56" s="48" t="s">
         <v>127</v>
@@ -4766,7 +4801,7 @@
     </row>
     <row r="57" spans="1:11" s="48" customFormat="1">
       <c r="A57" s="48" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B57" s="48" t="s">
         <v>127</v>
@@ -4780,7 +4815,7 @@
     </row>
     <row r="58" spans="1:11" s="48" customFormat="1">
       <c r="A58" s="48" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B58" s="48" t="s">
         <v>127</v>
@@ -4791,7 +4826,7 @@
     </row>
     <row r="59" spans="1:11" s="48" customFormat="1">
       <c r="A59" s="48" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B59" s="48" t="s">
         <v>127</v>
@@ -4802,7 +4837,7 @@
     </row>
     <row r="60" spans="1:11" s="48" customFormat="1">
       <c r="A60" s="48" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B60" s="48" t="s">
         <v>171</v>
@@ -4816,7 +4851,7 @@
     </row>
     <row r="61" spans="1:11" s="48" customFormat="1">
       <c r="A61" s="48" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B61" s="48" t="s">
         <v>171</v>
@@ -4827,7 +4862,7 @@
     </row>
     <row r="62" spans="1:11" s="48" customFormat="1">
       <c r="A62" s="48" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B62" s="48" t="s">
         <v>171</v>
@@ -4838,7 +4873,7 @@
     </row>
     <row r="63" spans="1:11" s="48" customFormat="1">
       <c r="A63" s="48" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B63" s="48" t="s">
         <v>171</v>
@@ -4852,18 +4887,18 @@
     </row>
     <row r="64" spans="1:11" s="48" customFormat="1">
       <c r="A64" s="48" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B64" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C64" s="48" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="65" spans="1:11" s="48" customFormat="1">
       <c r="A65" s="48" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B65" s="48" t="s">
         <v>171</v>
@@ -4874,18 +4909,18 @@
     </row>
     <row r="66" spans="1:11" s="48" customFormat="1">
       <c r="A66" s="48" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B66" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C66" s="48" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="48" customFormat="1">
       <c r="A67" s="48" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B67" s="48" t="s">
         <v>112</v>
@@ -4899,7 +4934,7 @@
     </row>
     <row r="68" spans="1:11" s="48" customFormat="1">
       <c r="A68" s="48" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B68" s="48" t="s">
         <v>112</v>
@@ -4913,7 +4948,7 @@
     </row>
     <row r="69" spans="1:11" s="48" customFormat="1">
       <c r="A69" s="48" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B69" s="48" t="s">
         <v>112</v>
@@ -4927,7 +4962,7 @@
     </row>
     <row r="70" spans="1:11" s="48" customFormat="1">
       <c r="A70" s="48" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B70" s="48" t="s">
         <v>112</v>
@@ -4941,13 +4976,13 @@
     </row>
     <row r="71" spans="1:11" s="48" customFormat="1">
       <c r="A71" s="48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B71" s="48" t="s">
         <v>112</v>
       </c>
       <c r="C71" s="48" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D71" s="48" t="s">
         <v>239</v>
@@ -4955,7 +4990,7 @@
     </row>
     <row r="72" spans="1:11" s="48" customFormat="1">
       <c r="A72" s="48" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B72" s="48" t="s">
         <v>15</v>
@@ -4966,7 +5001,7 @@
     </row>
     <row r="73" spans="1:11" s="48" customFormat="1">
       <c r="A73" s="48" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B73" s="48" t="s">
         <v>112</v>
@@ -4983,7 +5018,7 @@
     </row>
     <row r="74" spans="1:11" s="48" customFormat="1">
       <c r="A74" s="48" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B74" s="48" t="s">
         <v>112</v>
@@ -4997,7 +5032,7 @@
     </row>
     <row r="75" spans="1:11" s="48" customFormat="1">
       <c r="A75" s="48" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B75" s="48" t="s">
         <v>112</v>
@@ -5011,7 +5046,7 @@
     </row>
     <row r="76" spans="1:11" s="48" customFormat="1">
       <c r="A76" s="48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B76" s="48" t="s">
         <v>112</v>
@@ -5025,7 +5060,7 @@
     </row>
     <row r="77" spans="1:11" s="48" customFormat="1">
       <c r="A77" s="48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B77" s="48" t="s">
         <v>112</v>
@@ -5039,7 +5074,7 @@
     </row>
     <row r="78" spans="1:11" s="48" customFormat="1">
       <c r="A78" s="48" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B78" s="48" t="s">
         <v>112</v>
@@ -5050,7 +5085,7 @@
     </row>
     <row r="79" spans="1:11" s="48" customFormat="1">
       <c r="A79" s="48" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B79" s="48" t="s">
         <v>112</v>
@@ -5061,7 +5096,7 @@
     </row>
     <row r="80" spans="1:11" s="48" customFormat="1">
       <c r="A80" s="48" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B80" s="48" t="s">
         <v>112</v>
@@ -5092,19 +5127,19 @@
     </row>
     <row r="82" spans="1:11" s="48" customFormat="1">
       <c r="A82" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B82" s="48" t="s">
         <v>130</v>
       </c>
       <c r="C82" s="48" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D82" s="48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E82" s="48" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="83" spans="1:11" s="48" customFormat="1">
@@ -5121,7 +5156,7 @@
         <v>85</v>
       </c>
       <c r="K83" s="48" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="84" spans="1:11" s="48" customFormat="1">
@@ -5141,7 +5176,7 @@
         <v>294</v>
       </c>
       <c r="F84" s="48" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G84" s="48" t="s">
         <v>154</v>
@@ -5149,7 +5184,7 @@
     </row>
     <row r="85" spans="1:11" s="48" customFormat="1">
       <c r="A85" s="48" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B85" s="48" t="s">
         <v>130</v>
@@ -5184,13 +5219,13 @@
         <v>148</v>
       </c>
       <c r="F86" s="48" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G86" s="48" t="s">
         <v>154</v>
       </c>
       <c r="K86" s="48" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="87" spans="1:11" s="48" customFormat="1">
@@ -5213,7 +5248,7 @@
         <v>154</v>
       </c>
       <c r="K87" s="48" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="88" spans="1:11" s="48" customFormat="1">
@@ -5236,7 +5271,7 @@
         <v>154</v>
       </c>
       <c r="K88" s="48" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="89" spans="1:11" s="47" customFormat="1">
@@ -5258,7 +5293,7 @@
     </row>
     <row r="90" spans="1:11" s="48" customFormat="1">
       <c r="A90" s="48" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B90" s="48" t="s">
         <v>96</v>
@@ -5272,12 +5307,12 @@
         <v>133</v>
       </c>
       <c r="C91" s="48" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="92" spans="1:11" s="48" customFormat="1">
       <c r="A92" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B92" s="48" t="s">
         <v>133</v>
@@ -5291,7 +5326,7 @@
     </row>
     <row r="93" spans="1:11" s="48" customFormat="1">
       <c r="A93" s="49" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B93" s="48" t="s">
         <v>133</v>
@@ -5300,12 +5335,12 @@
         <v>132</v>
       </c>
       <c r="K93" s="48" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="94" spans="1:11" s="48" customFormat="1">
       <c r="A94" s="48" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B94" s="48" t="s">
         <v>142</v>
@@ -5316,7 +5351,7 @@
     </row>
     <row r="95" spans="1:11" s="48" customFormat="1">
       <c r="A95" s="48" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B95" s="48" t="s">
         <v>142</v>
@@ -5338,7 +5373,7 @@
     </row>
     <row r="97" spans="1:5" s="48" customFormat="1">
       <c r="A97" s="48" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B97" s="48" t="s">
         <v>142</v>
@@ -5358,7 +5393,7 @@
         <v>281</v>
       </c>
       <c r="D98" s="48" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E98" s="48" t="s">
         <v>62</v>
@@ -5377,29 +5412,29 @@
     </row>
     <row r="100" spans="1:5" s="48" customFormat="1">
       <c r="A100" s="48" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B100" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C100" s="48" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="48" customFormat="1">
       <c r="A101" s="48" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B101" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C101" s="48" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C102" s="48" t="s">
         <v>281</v>
@@ -5407,7 +5442,7 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C103" s="48" t="s">
         <v>281</v>
@@ -5415,7 +5450,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C104" s="48" t="s">
         <v>281</v>
@@ -5423,7 +5458,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C105" s="48" t="s">
         <v>281</v>
@@ -5431,7 +5466,7 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C106" s="48" t="s">
         <v>281</v>
@@ -5439,7 +5474,7 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C107" s="48" t="s">
         <v>281</v>
@@ -5447,7 +5482,7 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C108" s="48" t="s">
         <v>281</v>
@@ -5455,183 +5490,183 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B109" t="s">
         <v>142</v>
       </c>
       <c r="C109" s="48" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B110" t="s">
         <v>142</v>
       </c>
       <c r="C110" s="48" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B111" t="s">
         <v>142</v>
       </c>
       <c r="C111" s="48" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B112" t="s">
         <v>142</v>
       </c>
       <c r="C112" s="48" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B113" t="s">
         <v>142</v>
       </c>
       <c r="C113" s="48" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B114" t="s">
         <v>142</v>
       </c>
       <c r="C114" s="48" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B115" t="s">
         <v>142</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B116" t="s">
         <v>142</v>
       </c>
       <c r="C116" s="48" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B117" t="s">
         <v>143</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B118" t="s">
         <v>143</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B119" t="s">
         <v>143</v>
       </c>
       <c r="C119" s="48" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B120" t="s">
         <v>143</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B121" t="s">
         <v>143</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B122" t="s">
         <v>143</v>
       </c>
       <c r="C122" s="48" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B123" t="s">
         <v>143</v>
       </c>
       <c r="C123" s="48" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B124" t="s">
         <v>143</v>
       </c>
       <c r="C124" s="48" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B125" t="s">
         <v>143</v>
@@ -5642,194 +5677,194 @@
     </row>
     <row r="126" spans="1:3" s="48" customFormat="1">
       <c r="A126" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B126" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C126" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="127" spans="1:3" s="48" customFormat="1">
       <c r="A127" s="48" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B127" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C127" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="128" spans="1:3" s="48" customFormat="1">
       <c r="A128" s="48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B128" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C128" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="129" spans="1:3" s="48" customFormat="1">
       <c r="A129" s="48" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B129" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C129" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="130" spans="1:3" s="48" customFormat="1">
       <c r="A130" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B130" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C130" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="131" spans="1:3" s="48" customFormat="1">
       <c r="A131" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B131" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C131" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="132" spans="1:3" s="48" customFormat="1">
       <c r="A132" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B132" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C132" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="133" spans="1:3" s="48" customFormat="1">
       <c r="A133" s="48" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B133" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C133" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="134" spans="1:3" s="48" customFormat="1">
       <c r="A134" s="48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B134" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C134" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="135" spans="1:3" s="48" customFormat="1">
       <c r="A135" s="48" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B135" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C135" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="136" spans="1:3" s="48" customFormat="1">
       <c r="A136" s="48" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B136" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C136" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="137" spans="1:3" s="48" customFormat="1">
       <c r="A137" s="48" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B137" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C137" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="138" spans="1:3" s="48" customFormat="1">
       <c r="A138" s="48" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B138" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C138" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="139" spans="1:3" s="48" customFormat="1">
       <c r="A139" s="48" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B139" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C139" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="140" spans="1:3" s="48" customFormat="1">
       <c r="A140" s="48" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B140" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C140" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="141" spans="1:3" s="48" customFormat="1">
       <c r="A141" s="48" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B141" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C141" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="142" spans="1:3" s="48" customFormat="1">
       <c r="A142" s="48" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B142" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C142" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="48" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B143" s="48" t="s">
         <v>131</v>
@@ -5837,7 +5872,7 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="48" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B144" s="48" t="s">
         <v>179</v>
@@ -5855,18 +5890,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5876,20 +5911,20 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B8" t="s">
         <v>379</v>
-      </c>
-      <c r="B8" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added advanced plotting functions: `YH`
`plot3`, `surf`, `mesh`, `stem`, `stairs`, `bar`
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Dropbox\MATL\spec\functionTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2C8ED0-996E-4AFA-A023-3578D9E7D8B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29829E89-DBAC-4DE5-AA64-1F5CAE6CB00C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="552">
   <si>
     <t>Normal function</t>
   </si>
@@ -1675,6 +1675,9 @@
   </si>
   <si>
     <t>char(vpa(str2sym(…), ...))</t>
+  </si>
+  <si>
+    <t>advanced plotting functions</t>
   </si>
 </sst>
 </file>
@@ -2346,8 +2349,8 @@
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12" customHeight="1"/>
@@ -3042,7 +3045,9 @@
         <v>245</v>
       </c>
       <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
+      <c r="F44" s="52" t="s">
+        <v>551</v>
+      </c>
     </row>
     <row r="45" spans="2:6" ht="12" customHeight="1">
       <c r="B45" s="27" t="s">

</xml_diff>

<commit_message>
Added "shuffle" in `Zr`
Added "shuffle" (apply a random permutation to input) in `Zr`. Suggested by @flawr
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Dropbox\MATL\spec\functionTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29829E89-DBAC-4DE5-AA64-1F5CAE6CB00C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3D9A6B-205B-448E-8E98-04FBAD15EB22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -270,9 +270,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>randsample</t>
-  </si>
-  <si>
     <t>isequal</t>
   </si>
   <si>
@@ -1678,6 +1675,9 @@
   </si>
   <si>
     <t>advanced plotting functions</t>
+  </si>
+  <si>
+    <t>randsample / shuffle</t>
   </si>
 </sst>
 </file>
@@ -2349,8 +2349,8 @@
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12" customHeight="1"/>
@@ -2367,7 +2367,7 @@
     <row r="1" spans="1:12" ht="12" customHeight="1">
       <c r="A1" s="51"/>
       <c r="C1" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="12" customHeight="1">
@@ -2376,49 +2376,49 @@
         <v>0</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="12" customHeight="1">
       <c r="C3" s="5"/>
       <c r="D3" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>174</v>
-      </c>
       <c r="H3" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I3" s="21" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="K3" s="16" t="s">
-        <v>253</v>
-      </c>
       <c r="L3" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="12" customHeight="1">
       <c r="B4" s="24"/>
       <c r="C4" s="25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -2429,33 +2429,33 @@
         <v>25</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="12" customHeight="1">
       <c r="B6" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -2464,16 +2464,16 @@
         <v>69</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="12" customHeight="1">
@@ -2481,31 +2481,31 @@
         <v>68</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="9" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="12" customHeight="1">
       <c r="B9" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="12" customHeight="1">
@@ -2513,65 +2513,65 @@
         <v>37</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="12" customHeight="1">
       <c r="B11" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="28" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="12" customHeight="1">
       <c r="B12" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12" customHeight="1">
       <c r="B13" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12" customHeight="1">
@@ -2579,16 +2579,16 @@
         <v>27</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E14" s="28" t="s">
         <v>39</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="12" customHeight="1">
@@ -2600,18 +2600,18 @@
       </c>
       <c r="D15" s="46"/>
       <c r="E15" s="28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12" customHeight="1">
       <c r="B16" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>47</v>
@@ -2631,45 +2631,45 @@
         <v>29</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F17" s="29"/>
     </row>
     <row r="18" spans="2:6" ht="12" customHeight="1">
       <c r="B18" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C18" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="D18" s="31" t="s">
-        <v>156</v>
-      </c>
       <c r="E18" s="36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="12" customHeight="1">
       <c r="B19" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C19" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="E19" s="52" t="s">
+        <v>538</v>
+      </c>
+      <c r="F19" s="28" t="s">
         <v>227</v>
-      </c>
-      <c r="E19" s="52" t="s">
-        <v>539</v>
-      </c>
-      <c r="F19" s="28" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="12" customHeight="1">
@@ -2677,13 +2677,13 @@
         <v>57</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F20" s="39"/>
     </row>
@@ -2692,150 +2692,150 @@
         <v>70</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F21" s="39"/>
     </row>
     <row r="22" spans="2:6" ht="12" customHeight="1">
       <c r="B22" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F22" s="39"/>
     </row>
     <row r="23" spans="2:6" ht="12" customHeight="1">
       <c r="B23" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F23" s="39"/>
     </row>
     <row r="24" spans="2:6" ht="12" customHeight="1">
       <c r="B24" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C24" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F24" s="39"/>
     </row>
     <row r="25" spans="2:6" ht="12" customHeight="1">
       <c r="B25" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F25" s="39"/>
     </row>
     <row r="26" spans="2:6" ht="12" customHeight="1">
       <c r="B26" s="27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F26" s="39"/>
     </row>
     <row r="27" spans="2:6" ht="12" customHeight="1">
       <c r="B27" s="27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E27" s="39"/>
       <c r="F27" s="39"/>
     </row>
     <row r="28" spans="2:6" ht="12" customHeight="1">
       <c r="B28" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D28" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E28" s="39"/>
       <c r="F28" s="39"/>
     </row>
     <row r="29" spans="2:6" ht="12" customHeight="1">
       <c r="B29" s="27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="39"/>
     </row>
     <row r="30" spans="2:6" ht="12" customHeight="1">
       <c r="B30" s="27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D30" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="E30" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="E30" s="37" t="s">
-        <v>211</v>
-      </c>
       <c r="F30" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="12" customHeight="1">
       <c r="B31" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" s="46"/>
       <c r="D31" s="28" t="s">
@@ -2859,7 +2859,7 @@
         <v>54</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F32" s="29"/>
     </row>
@@ -2871,10 +2871,10 @@
         <v>34</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F33" s="29"/>
     </row>
@@ -2889,40 +2889,40 @@
         <v>55</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F34" s="29"/>
     </row>
     <row r="35" spans="2:6" ht="12" customHeight="1">
       <c r="B35" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="28" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="2:6" ht="12" customHeight="1">
       <c r="B36" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C36" s="53" t="s">
+        <v>531</v>
+      </c>
+      <c r="D36" s="53" t="s">
         <v>532</v>
       </c>
-      <c r="D36" s="53" t="s">
-        <v>533</v>
-      </c>
       <c r="E36" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F36" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="12" customHeight="1">
@@ -2933,30 +2933,30 @@
         <v>7</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E37" s="28" t="s">
+        <v>301</v>
+      </c>
+      <c r="F37" s="28" t="s">
         <v>302</v>
-      </c>
-      <c r="F37" s="28" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="12" customHeight="1">
       <c r="B38" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D38" s="28" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="12" customHeight="1">
@@ -2966,24 +2966,24 @@
       <c r="C39" s="46"/>
       <c r="D39" s="46"/>
       <c r="E39" s="28" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="12" customHeight="1">
       <c r="B40" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F40" s="28" t="s">
         <v>18</v>
@@ -2991,103 +2991,103 @@
     </row>
     <row r="41" spans="2:6" ht="12" customHeight="1">
       <c r="B41" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="46"/>
     </row>
     <row r="42" spans="2:6" ht="12" customHeight="1">
       <c r="B42" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C42" s="35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D42" s="38"/>
       <c r="E42" s="28" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F42" s="52" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="12" customHeight="1">
       <c r="B43" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F43" s="36" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="12" customHeight="1">
       <c r="B44" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E44" s="46"/>
       <c r="F44" s="52" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="12" customHeight="1">
       <c r="B45" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F45" s="52" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
       <c r="B46" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E46" s="46"/>
       <c r="F46" s="46"/>
     </row>
     <row r="47" spans="2:6" ht="12" customHeight="1">
       <c r="B47" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D47" s="40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E47" s="46"/>
       <c r="F47" s="46"/>
@@ -3097,13 +3097,13 @@
         <v>42</v>
       </c>
       <c r="C48" s="40" t="s">
+        <v>469</v>
+      </c>
+      <c r="D48" s="40" t="s">
         <v>470</v>
       </c>
-      <c r="D48" s="40" t="s">
-        <v>471</v>
-      </c>
       <c r="E48" s="28" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F48" s="46"/>
     </row>
@@ -3112,80 +3112,80 @@
         <v>11</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E49" s="29"/>
       <c r="F49" s="29"/>
     </row>
     <row r="50" spans="2:6" ht="12" customHeight="1">
       <c r="B50" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C50" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F50" s="28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="51" spans="2:6" ht="12" customHeight="1">
       <c r="B51" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D51" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="E51" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="E51" s="28" t="s">
+      <c r="F51" s="28" t="s">
         <v>208</v>
-      </c>
-      <c r="F51" s="28" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="52" spans="2:6" ht="12" customHeight="1">
       <c r="B52" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C52" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="12" customHeight="1">
       <c r="B53" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="12" customHeight="1">
@@ -3196,13 +3196,13 @@
         <v>41</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>40</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="12" customHeight="1">
@@ -3216,22 +3216,22 @@
         <v>23</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F55" s="52" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="12" customHeight="1">
       <c r="B56" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C56" s="35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D56" s="46"/>
       <c r="E56" s="36" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F56" s="38"/>
     </row>
@@ -3240,17 +3240,17 @@
         <v>43</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E57" s="29"/>
       <c r="F57" s="29"/>
     </row>
     <row r="58" spans="2:6" ht="12" customHeight="1">
       <c r="B58" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C58" s="28" t="s">
         <v>67</v>
@@ -3261,10 +3261,10 @@
     </row>
     <row r="59" spans="2:6" ht="12" customHeight="1">
       <c r="B59" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -3272,40 +3272,40 @@
     </row>
     <row r="60" spans="2:6" ht="12" customHeight="1">
       <c r="B60" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C60" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D60" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="E60" s="36" t="s">
         <v>89</v>
-      </c>
-      <c r="E60" s="36" t="s">
-        <v>90</v>
       </c>
       <c r="F60" s="38"/>
     </row>
     <row r="61" spans="2:6" ht="12" customHeight="1">
       <c r="B61" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C61" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D61" s="38"/>
       <c r="E61" s="36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F61" s="36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="62" spans="2:6" ht="12" customHeight="1">
       <c r="B62" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C62" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D62" s="38"/>
       <c r="E62" s="38"/>
@@ -3313,10 +3313,10 @@
     </row>
     <row r="63" spans="2:6" ht="12" customHeight="1">
       <c r="B63" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D63" s="36" t="s">
         <v>13</v>
@@ -3326,27 +3326,27 @@
     </row>
     <row r="64" spans="2:6" ht="12" customHeight="1">
       <c r="B64" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C64" s="28" t="s">
         <v>9</v>
       </c>
       <c r="D64" s="28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E64" s="52" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="12" customHeight="1">
       <c r="B65" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D65" s="28" t="s">
         <v>12</v>
@@ -3365,18 +3365,18 @@
         <v>44</v>
       </c>
       <c r="E66" s="52" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="12" customHeight="1">
       <c r="B67" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
@@ -3384,19 +3384,19 @@
     </row>
     <row r="68" spans="1:7" ht="12" customHeight="1">
       <c r="B68" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E68" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="F68" s="28" t="s">
         <v>231</v>
-      </c>
-      <c r="F68" s="28" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="12" customHeight="1">
@@ -3407,25 +3407,25 @@
         <v>5</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="12" customHeight="1">
       <c r="B70" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C70" s="42" t="s">
         <v>59</v>
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F70" s="29"/>
     </row>
@@ -3434,16 +3434,16 @@
         <v>74</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D71" s="28" t="s">
         <v>3</v>
       </c>
       <c r="E71" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F71" s="52" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="12" customHeight="1">
@@ -3451,28 +3451,28 @@
         <v>19</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E72" s="28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F72" s="28" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="12" customHeight="1">
       <c r="B73" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="52" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F73" s="28" t="s">
         <v>45</v>
@@ -3487,110 +3487,110 @@
         <v>14</v>
       </c>
       <c r="D74" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E74" s="28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F74" s="29"/>
       <c r="G74" s="1"/>
     </row>
     <row r="75" spans="1:7" ht="12" customHeight="1">
       <c r="B75" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D75" s="28" t="s">
         <v>72</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="12" customHeight="1">
       <c r="B76" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D76" s="34" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E76" s="28" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F76" s="28" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="12" customHeight="1">
       <c r="B77" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E77" s="28" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F77" s="46"/>
     </row>
     <row r="78" spans="1:7" ht="12" customHeight="1">
       <c r="B78" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D78" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E78" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="E78" s="28" t="s">
-        <v>135</v>
-      </c>
       <c r="F78" s="52" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="12" customHeight="1">
       <c r="B79" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C79" s="28" t="s">
+        <v>487</v>
+      </c>
+      <c r="D79" s="28" t="s">
         <v>488</v>
       </c>
-      <c r="D79" s="28" t="s">
-        <v>489</v>
-      </c>
       <c r="E79" s="28" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F79" s="46"/>
     </row>
     <row r="80" spans="1:7" ht="12" customHeight="1">
       <c r="B80" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E80" s="28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F80" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" spans="2:6" ht="12" customHeight="1">
@@ -3598,16 +3598,16 @@
         <v>10</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E81" s="28" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F81" s="28" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="82" spans="2:6" ht="12" customHeight="1">
@@ -3615,13 +3615,13 @@
         <v>65</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D82" s="28" t="s">
+        <v>507</v>
+      </c>
+      <c r="E82" s="28" t="s">
         <v>508</v>
-      </c>
-      <c r="E82" s="28" t="s">
-        <v>509</v>
       </c>
       <c r="F82" s="46"/>
     </row>
@@ -3630,50 +3630,50 @@
         <v>77</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>75</v>
       </c>
       <c r="E83" s="28" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F83" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84" spans="2:6" ht="12" customHeight="1">
       <c r="B84" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C84" s="28" t="s">
         <v>62</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E84" s="28" t="s">
         <v>64</v>
       </c>
       <c r="F84" s="28" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="85" spans="2:6" ht="12" customHeight="1">
       <c r="B85" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E85" s="28" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F85" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="86" spans="2:6" ht="12" customHeight="1">
@@ -3689,8 +3689,8 @@
       <c r="E86" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="F86" s="28" t="s">
-        <v>82</v>
+      <c r="F86" s="52" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="87" spans="2:6" ht="12" customHeight="1">
@@ -3701,26 +3701,26 @@
         <v>60</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E87" s="28" t="s">
         <v>63</v>
       </c>
       <c r="F87" s="52" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="12" customHeight="1">
       <c r="B88" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D88" s="46"/>
       <c r="E88" s="46"/>
       <c r="F88" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="2:6" ht="12" customHeight="1">
@@ -3728,34 +3728,34 @@
         <v>58</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D89" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E89" s="44"/>
       <c r="F89" s="28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="90" spans="2:6" ht="12" customHeight="1">
       <c r="B90" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C90" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D90" s="46"/>
       <c r="E90" s="28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F90" s="52" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="12" customHeight="1">
       <c r="B91" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C91" s="42" t="s">
         <v>56</v>
@@ -3766,10 +3766,10 @@
     </row>
     <row r="92" spans="2:6" ht="12" customHeight="1">
       <c r="B92" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C92" s="42" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D92" s="28" t="s">
         <v>66</v>
@@ -3779,10 +3779,10 @@
     </row>
     <row r="93" spans="2:6" ht="12" customHeight="1">
       <c r="B93" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D93" s="28" t="s">
         <v>61</v>
@@ -3791,37 +3791,37 @@
         <v>52</v>
       </c>
       <c r="F93" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="94" spans="2:6" ht="12" customHeight="1">
       <c r="B94" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C94" s="52" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E94" s="29"/>
       <c r="F94" s="29"/>
     </row>
     <row r="95" spans="2:6" ht="12" customHeight="1">
       <c r="B95" s="27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C95" s="35" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D95" s="36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E95" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F95" s="36" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="96" spans="2:6" ht="12" customHeight="1">
@@ -3829,46 +3829,46 @@
         <v>38</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D96" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E96" s="36" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F96" s="28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="97" spans="2:6" ht="12" customHeight="1">
       <c r="B97" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D97" s="46"/>
       <c r="E97" s="46"/>
       <c r="F97" s="28" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="98" spans="2:6" ht="12" customHeight="1">
       <c r="B98" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F98" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="99" spans="2:6" ht="12" customHeight="1">
@@ -3929,10 +3929,10 @@
   <sheetData>
     <row r="1" spans="1:11" ht="13">
       <c r="A1" s="45" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="50" customFormat="1">
@@ -3943,29 +3943,29 @@
         <v>8</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="48" customFormat="1">
       <c r="A3" s="48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="48" customFormat="1">
       <c r="A4" s="48" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="48" customFormat="1">
@@ -3973,28 +3973,28 @@
         <v>76</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F5" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G5" s="48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H5" s="48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I5" s="48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J5" s="48" t="s">
         <v>62</v>
@@ -4002,90 +4002,90 @@
     </row>
     <row r="6" spans="1:11" s="48" customFormat="1">
       <c r="A6" s="48" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B6" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="48" customFormat="1">
       <c r="A7" s="48" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B7" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="48" customFormat="1">
       <c r="A8" s="48" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B8" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="48" customFormat="1">
       <c r="A9" s="48" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B9" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="48" customFormat="1">
       <c r="A10" s="48" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B10" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="48" customFormat="1">
       <c r="A11" s="48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B11" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="48" customFormat="1">
       <c r="A12" s="48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B12" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="48" customFormat="1">
       <c r="A13" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B13" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K13" s="48" t="s">
         <v>27</v>
@@ -4093,35 +4093,35 @@
     </row>
     <row r="14" spans="1:11" s="48" customFormat="1">
       <c r="A14" s="48" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B14" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="48" customFormat="1">
       <c r="A15" s="48" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B15" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="48" customFormat="1">
       <c r="A16" s="48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B16" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="48" customFormat="1">
@@ -4129,32 +4129,32 @@
         <v>73</v>
       </c>
       <c r="B17" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D17" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="48" customFormat="1">
       <c r="A18" s="48" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B18" s="48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="48" customFormat="1">
       <c r="A19" s="48" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B19" s="48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" s="48" t="s">
         <v>54</v>
@@ -4163,39 +4163,39 @@
         <v>55</v>
       </c>
       <c r="E19" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="F19" s="48" t="s">
         <v>225</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="48" customFormat="1">
       <c r="A20" s="48" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B20" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D20" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E20" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="G20" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="H20" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="F20" s="48" t="s">
+      <c r="I20" s="48" t="s">
         <v>217</v>
-      </c>
-      <c r="G20" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="H20" s="48" t="s">
-        <v>215</v>
-      </c>
-      <c r="I20" s="48" t="s">
-        <v>218</v>
       </c>
       <c r="K20" s="48" t="s">
         <v>27</v>
@@ -4203,31 +4203,31 @@
     </row>
     <row r="21" spans="1:11" s="48" customFormat="1">
       <c r="A21" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B21" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E21" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="G21" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="H21" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="F21" s="48" t="s">
+      <c r="I21" s="48" t="s">
         <v>217</v>
-      </c>
-      <c r="G21" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="H21" s="48" t="s">
-        <v>215</v>
-      </c>
-      <c r="I21" s="48" t="s">
-        <v>218</v>
       </c>
       <c r="K21" s="48" t="s">
         <v>27</v>
@@ -4238,28 +4238,28 @@
         <v>75</v>
       </c>
       <c r="B22" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D22" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E22" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="F22" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="G22" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="H22" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="F22" s="48" t="s">
+      <c r="I22" s="48" t="s">
         <v>217</v>
-      </c>
-      <c r="G22" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="H22" s="48" t="s">
-        <v>215</v>
-      </c>
-      <c r="I22" s="48" t="s">
-        <v>218</v>
       </c>
       <c r="K22" s="48" t="s">
         <v>27</v>
@@ -4267,31 +4267,31 @@
     </row>
     <row r="23" spans="1:11" s="48" customFormat="1">
       <c r="A23" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B23" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D23" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E23" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="F23" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="G23" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="H23" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="I23" s="48" t="s">
         <v>217</v>
-      </c>
-      <c r="G23" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="H23" s="48" t="s">
-        <v>215</v>
-      </c>
-      <c r="I23" s="48" t="s">
-        <v>218</v>
       </c>
       <c r="K23" s="48" t="s">
         <v>27</v>
@@ -4299,25 +4299,25 @@
     </row>
     <row r="24" spans="1:11" s="48" customFormat="1">
       <c r="A24" s="48" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B24" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E24" s="48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F24" s="48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G24" s="48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H24" s="48" t="s">
         <v>79</v>
@@ -4328,16 +4328,16 @@
     </row>
     <row r="25" spans="1:11" s="48" customFormat="1">
       <c r="A25" s="48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B25" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K25" s="48" t="s">
         <v>27</v>
@@ -4345,13 +4345,13 @@
     </row>
     <row r="26" spans="1:11" s="48" customFormat="1">
       <c r="A26" s="48" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B26" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D26" s="48" t="s">
         <v>62</v>
@@ -4359,10 +4359,10 @@
     </row>
     <row r="27" spans="1:11" s="48" customFormat="1">
       <c r="A27" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B27" s="48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C27" s="48" t="s">
         <v>54</v>
@@ -4371,67 +4371,67 @@
         <v>55</v>
       </c>
       <c r="E27" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="F27" s="48" t="s">
         <v>225</v>
-      </c>
-      <c r="F27" s="48" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="48" customFormat="1">
       <c r="A28" s="48" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B28" s="48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="48" customFormat="1">
       <c r="A29" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B29" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E29" s="48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F29" s="48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="48" customFormat="1">
       <c r="A30" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B30" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E30" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="F30" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="G30" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="H30" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="F30" s="48" t="s">
+      <c r="I30" s="48" t="s">
         <v>217</v>
-      </c>
-      <c r="G30" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="H30" s="48" t="s">
-        <v>215</v>
-      </c>
-      <c r="I30" s="48" t="s">
-        <v>218</v>
       </c>
       <c r="K30" s="48" t="s">
         <v>27</v>
@@ -4439,31 +4439,31 @@
     </row>
     <row r="31" spans="1:11" s="48" customFormat="1">
       <c r="A31" s="48" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B31" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E31" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="F31" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="G31" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="H31" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="F31" s="48" t="s">
+      <c r="I31" s="48" t="s">
         <v>217</v>
-      </c>
-      <c r="G31" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="H31" s="48" t="s">
-        <v>215</v>
-      </c>
-      <c r="I31" s="48" t="s">
-        <v>218</v>
       </c>
       <c r="K31" s="48" t="s">
         <v>27</v>
@@ -4471,34 +4471,34 @@
     </row>
     <row r="32" spans="1:11" s="48" customFormat="1">
       <c r="A32" s="48" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B32" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C32" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E32" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="F32" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="G32" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="H32" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="F32" s="48" t="s">
+      <c r="I32" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="G32" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="H32" s="48" t="s">
-        <v>215</v>
-      </c>
-      <c r="I32" s="48" t="s">
-        <v>218</v>
-      </c>
       <c r="J32" s="48" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K32" s="48" t="s">
         <v>27</v>
@@ -4506,31 +4506,31 @@
     </row>
     <row r="33" spans="1:11" s="48" customFormat="1">
       <c r="A33" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B33" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C33" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E33" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="F33" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="G33" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="H33" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="F33" s="48" t="s">
+      <c r="I33" s="48" t="s">
         <v>217</v>
-      </c>
-      <c r="G33" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="H33" s="48" t="s">
-        <v>215</v>
-      </c>
-      <c r="I33" s="48" t="s">
-        <v>218</v>
       </c>
       <c r="K33" s="48" t="s">
         <v>27</v>
@@ -4538,167 +4538,167 @@
     </row>
     <row r="34" spans="1:11" s="48" customFormat="1">
       <c r="A34" s="48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B34" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="48" customFormat="1">
       <c r="A35" s="48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B35" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="48" customFormat="1">
       <c r="A36" s="48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B36" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="48" customFormat="1">
       <c r="A37" s="48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B37" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C37" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="48" customFormat="1">
       <c r="A38" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B38" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="48" customFormat="1">
       <c r="A39" s="48" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B39" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C39" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="48" customFormat="1">
       <c r="A40" s="48" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B40" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C40" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="48" customFormat="1">
       <c r="A41" s="48" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B41" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C41" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="48" customFormat="1">
       <c r="A42" s="48" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B42" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C42" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="48" customFormat="1">
       <c r="A43" s="48" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B43" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C43" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="48" customFormat="1">
       <c r="A44" s="48" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B44" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C44" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="48" customFormat="1">
       <c r="A45" s="48" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B45" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C45" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:11" s="48" customFormat="1">
       <c r="A46" s="48" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B46" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C46" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:11" s="48" customFormat="1">
       <c r="A47" s="48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B47" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="48" customFormat="1">
       <c r="A48" s="48" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B48" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:11" s="48" customFormat="1">
@@ -4709,18 +4709,18 @@
         <v>4</v>
       </c>
       <c r="C49" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:11" s="48" customFormat="1">
       <c r="A50" s="48" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B50" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K50" s="48" t="s">
         <v>27</v>
@@ -4728,24 +4728,24 @@
     </row>
     <row r="51" spans="1:11" s="48" customFormat="1">
       <c r="A51" s="48" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B51" s="48" t="s">
         <v>19</v>
       </c>
       <c r="C51" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:11" s="48" customFormat="1">
       <c r="A52" s="48" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B52" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C52" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K52" s="48" t="s">
         <v>27</v>
@@ -4753,27 +4753,27 @@
     </row>
     <row r="53" spans="1:11" s="48" customFormat="1">
       <c r="A53" s="48" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B53" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C53" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="48" customFormat="1">
       <c r="A54" s="48" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B54" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C54" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K54" s="48" t="s">
         <v>27</v>
@@ -4781,24 +4781,24 @@
     </row>
     <row r="55" spans="1:11" s="48" customFormat="1">
       <c r="A55" s="48" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B55" s="48" t="s">
         <v>19</v>
       </c>
       <c r="C55" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:11" s="48" customFormat="1">
       <c r="A56" s="48" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B56" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C56" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K56" s="48" t="s">
         <v>27</v>
@@ -4806,13 +4806,13 @@
     </row>
     <row r="57" spans="1:11" s="48" customFormat="1">
       <c r="A57" s="48" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B57" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C57" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K57" s="48" t="s">
         <v>27</v>
@@ -4820,35 +4820,35 @@
     </row>
     <row r="58" spans="1:11" s="48" customFormat="1">
       <c r="A58" s="48" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B58" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C58" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="48" customFormat="1">
       <c r="A59" s="48" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B59" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C59" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="48" customFormat="1">
       <c r="A60" s="48" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B60" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C60" s="48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K60" s="48" t="s">
         <v>27</v>
@@ -4856,35 +4856,35 @@
     </row>
     <row r="61" spans="1:11" s="48" customFormat="1">
       <c r="A61" s="48" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B61" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C61" s="48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="48" customFormat="1">
       <c r="A62" s="48" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B62" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C62" s="48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="63" spans="1:11" s="48" customFormat="1">
       <c r="A63" s="48" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B63" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C63" s="48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K63" s="48" t="s">
         <v>27</v>
@@ -4892,110 +4892,110 @@
     </row>
     <row r="64" spans="1:11" s="48" customFormat="1">
       <c r="A64" s="48" t="s">
+        <v>331</v>
+      </c>
+      <c r="B64" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="C64" s="48" t="s">
         <v>332</v>
-      </c>
-      <c r="B64" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="C64" s="48" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="65" spans="1:11" s="48" customFormat="1">
       <c r="A65" s="48" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B65" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C65" s="48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="66" spans="1:11" s="48" customFormat="1">
       <c r="A66" s="48" t="s">
+        <v>389</v>
+      </c>
+      <c r="B66" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="C66" s="48" t="s">
         <v>390</v>
-      </c>
-      <c r="B66" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="C66" s="48" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="48" customFormat="1">
       <c r="A67" s="48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B67" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C67" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D67" s="48" t="s">
         <v>238</v>
-      </c>
-      <c r="D67" s="48" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="68" spans="1:11" s="48" customFormat="1">
       <c r="A68" s="48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B68" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C68" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D68" s="48" t="s">
         <v>238</v>
-      </c>
-      <c r="D68" s="48" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="48" customFormat="1">
       <c r="A69" s="48" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B69" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C69" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D69" s="48" t="s">
         <v>238</v>
-      </c>
-      <c r="D69" s="48" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="48" customFormat="1">
       <c r="A70" s="48" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B70" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C70" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D70" s="48" t="s">
         <v>238</v>
-      </c>
-      <c r="D70" s="48" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="71" spans="1:11" s="48" customFormat="1">
       <c r="A71" s="48" t="s">
+        <v>333</v>
+      </c>
+      <c r="B71" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="C71" s="48" t="s">
         <v>334</v>
       </c>
-      <c r="B71" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="C71" s="48" t="s">
-        <v>335</v>
-      </c>
       <c r="D71" s="48" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="72" spans="1:11" s="48" customFormat="1">
       <c r="A72" s="48" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B72" s="48" t="s">
         <v>15</v>
@@ -5006,16 +5006,16 @@
     </row>
     <row r="73" spans="1:11" s="48" customFormat="1">
       <c r="A73" s="48" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B73" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C73" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D73" s="48" t="s">
         <v>238</v>
-      </c>
-      <c r="D73" s="48" t="s">
-        <v>239</v>
       </c>
       <c r="K73" s="48" t="s">
         <v>27</v>
@@ -5023,108 +5023,108 @@
     </row>
     <row r="74" spans="1:11" s="48" customFormat="1">
       <c r="A74" s="48" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B74" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C74" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D74" s="48" t="s">
         <v>238</v>
-      </c>
-      <c r="D74" s="48" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="75" spans="1:11" s="48" customFormat="1">
       <c r="A75" s="48" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B75" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C75" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D75" s="48" t="s">
         <v>238</v>
-      </c>
-      <c r="D75" s="48" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="48" customFormat="1">
       <c r="A76" s="48" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B76" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C76" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D76" s="48" t="s">
         <v>238</v>
-      </c>
-      <c r="D76" s="48" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="48" customFormat="1">
       <c r="A77" s="48" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B77" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C77" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D77" s="48" t="s">
         <v>238</v>
-      </c>
-      <c r="D77" s="48" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="48" customFormat="1">
       <c r="A78" s="48" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B78" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C78" s="48" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="48" customFormat="1">
       <c r="A79" s="48" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B79" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C79" s="48" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="80" spans="1:11" s="48" customFormat="1">
       <c r="A80" s="48" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B80" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C80" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D80" s="48" t="s">
         <v>238</v>
-      </c>
-      <c r="D80" s="48" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="81" spans="1:11" s="48" customFormat="1">
       <c r="A81" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="B81" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C81" s="48" t="s">
         <v>263</v>
       </c>
-      <c r="B81" s="48" t="s">
-        <v>137</v>
-      </c>
-      <c r="C81" s="48" t="s">
-        <v>264</v>
-      </c>
       <c r="D81" s="48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K81" s="48" t="s">
         <v>27</v>
@@ -5132,73 +5132,73 @@
     </row>
     <row r="82" spans="1:11" s="48" customFormat="1">
       <c r="A82" s="48" t="s">
+        <v>305</v>
+      </c>
+      <c r="B82" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C82" s="48" t="s">
         <v>306</v>
       </c>
-      <c r="B82" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="C82" s="48" t="s">
-        <v>307</v>
-      </c>
       <c r="D82" s="48" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E82" s="48" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="83" spans="1:11" s="48" customFormat="1">
       <c r="A83" s="49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B83" s="48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C83" s="48" t="s">
         <v>14</v>
       </c>
       <c r="D83" s="48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K83" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="84" spans="1:11" s="48" customFormat="1">
       <c r="A84" s="48" t="s">
+        <v>269</v>
+      </c>
+      <c r="B84" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C84" s="48" t="s">
         <v>270</v>
       </c>
-      <c r="B84" s="48" t="s">
-        <v>137</v>
-      </c>
-      <c r="C84" s="48" t="s">
-        <v>271</v>
-      </c>
       <c r="D84" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="E84" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="E84" s="48" t="s">
-        <v>294</v>
-      </c>
       <c r="F84" s="48" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G84" s="48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85" spans="1:11" s="48" customFormat="1">
       <c r="A85" s="48" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B85" s="48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C85" s="48" t="s">
+        <v>192</v>
+      </c>
+      <c r="D85" s="48" t="s">
         <v>193</v>
-      </c>
-      <c r="D85" s="48" t="s">
-        <v>194</v>
       </c>
       <c r="E85" s="48" t="s">
         <v>64</v>
@@ -5209,82 +5209,82 @@
     </row>
     <row r="86" spans="1:11" s="48" customFormat="1">
       <c r="A86" s="48" t="s">
+        <v>266</v>
+      </c>
+      <c r="B86" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C86" s="48" t="s">
         <v>267</v>
       </c>
-      <c r="B86" s="48" t="s">
-        <v>137</v>
-      </c>
-      <c r="C86" s="48" t="s">
-        <v>268</v>
-      </c>
       <c r="D86" s="48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E86" s="48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F86" s="48" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G86" s="48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K86" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="87" spans="1:11" s="48" customFormat="1">
       <c r="A87" s="48" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B87" s="48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C87" s="48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D87" s="48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E87" s="48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F87" s="48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K87" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="88" spans="1:11" s="48" customFormat="1">
       <c r="A88" s="49" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B88" s="48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C88" s="48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D88" s="48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E88" s="48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F88" s="48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K88" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="89" spans="1:11" s="47" customFormat="1">
       <c r="A89" s="47" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B89" s="47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C89" s="47" t="s">
         <v>20</v>
@@ -5298,32 +5298,32 @@
     </row>
     <row r="90" spans="1:11" s="48" customFormat="1">
       <c r="A90" s="48" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B90" s="48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="91" spans="1:11" s="48" customFormat="1">
       <c r="A91" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B91" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C91" s="48" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="92" spans="1:11" s="48" customFormat="1">
       <c r="A92" s="48" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B92" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C92" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K92" s="48" t="s">
         <v>27</v>
@@ -5331,38 +5331,38 @@
     </row>
     <row r="93" spans="1:11" s="48" customFormat="1">
       <c r="A93" s="49" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B93" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C93" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K93" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="94" spans="1:11" s="48" customFormat="1">
       <c r="A94" s="48" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B94" s="48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C94" s="48" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="95" spans="1:11" s="48" customFormat="1">
       <c r="A95" s="48" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B95" s="48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C95" s="48" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="96" spans="1:11" s="50" customFormat="1">
@@ -5370,35 +5370,35 @@
         <v>22</v>
       </c>
       <c r="B96" s="50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C96" s="50" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="48" customFormat="1">
       <c r="A97" s="48" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B97" s="48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C97" s="48" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="48" customFormat="1">
       <c r="A98" s="48" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B98" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C98" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D98" s="48" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E98" s="48" t="s">
         <v>62</v>
@@ -5406,481 +5406,481 @@
     </row>
     <row r="99" spans="1:5" s="48" customFormat="1">
       <c r="A99" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B99" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C99" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="48" customFormat="1">
       <c r="A100" s="48" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B100" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C100" s="48" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="48" customFormat="1">
       <c r="A101" s="48" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B101" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C101" s="48" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C102" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C103" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C104" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C105" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C106" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C107" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C108" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B109" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C109" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B110" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C110" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B111" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C111" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B112" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C112" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B113" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C113" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B114" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C114" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B115" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
+        <v>420</v>
+      </c>
+      <c r="B116" t="s">
+        <v>141</v>
+      </c>
+      <c r="C116" s="48" t="s">
         <v>421</v>
-      </c>
-      <c r="B116" t="s">
-        <v>142</v>
-      </c>
-      <c r="C116" s="48" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B117" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B118" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B119" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C119" s="48" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B120" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B121" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B122" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C122" s="48" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B123" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C123" s="48" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B124" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C124" s="48" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B125" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C125" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="126" spans="1:3" s="48" customFormat="1">
       <c r="A126" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B126" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C126" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="127" spans="1:3" s="48" customFormat="1">
       <c r="A127" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B127" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C127" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="128" spans="1:3" s="48" customFormat="1">
       <c r="A128" s="48" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B128" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C128" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="129" spans="1:3" s="48" customFormat="1">
       <c r="A129" s="48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B129" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C129" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="130" spans="1:3" s="48" customFormat="1">
       <c r="A130" s="48" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B130" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C130" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="131" spans="1:3" s="48" customFormat="1">
       <c r="A131" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B131" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C131" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="132" spans="1:3" s="48" customFormat="1">
       <c r="A132" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B132" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C132" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="133" spans="1:3" s="48" customFormat="1">
       <c r="A133" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B133" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C133" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="134" spans="1:3" s="48" customFormat="1">
       <c r="A134" s="48" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B134" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C134" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="135" spans="1:3" s="48" customFormat="1">
       <c r="A135" s="48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B135" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C135" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="136" spans="1:3" s="48" customFormat="1">
       <c r="A136" s="48" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B136" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C136" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="137" spans="1:3" s="48" customFormat="1">
       <c r="A137" s="48" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B137" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C137" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="138" spans="1:3" s="48" customFormat="1">
       <c r="A138" s="48" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B138" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C138" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="139" spans="1:3" s="48" customFormat="1">
       <c r="A139" s="48" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B139" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C139" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="140" spans="1:3" s="48" customFormat="1">
       <c r="A140" s="48" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B140" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C140" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="141" spans="1:3" s="48" customFormat="1">
       <c r="A141" s="48" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B141" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C141" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="142" spans="1:3" s="48" customFormat="1">
       <c r="A142" s="48" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B142" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C142" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="48" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B143" s="48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="48" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B144" s="48" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="65536" spans="3:3">
@@ -5906,7 +5906,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5916,20 +5916,20 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B8" t="s">
         <v>378</v>
-      </c>
-      <c r="B8" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved "execute Matlab function" from `X$` to `X'`; and changed input order
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Dropbox\MATL\spec\functionTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3D9A6B-205B-448E-8E98-04FBAD15EB22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E403CBEB-CCE4-4490-9B5B-5A0C5B616BBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="553">
   <si>
     <t>Normal function</t>
   </si>
@@ -1678,6 +1678,9 @@
   </si>
   <si>
     <t>randsample / shuffle</t>
+  </si>
+  <si>
+    <t>execute Matlab function</t>
   </si>
 </sst>
 </file>
@@ -2349,8 +2352,8 @@
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12" customHeight="1"/>
@@ -2483,7 +2486,6 @@
       <c r="C8" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="D8" s="46"/>
       <c r="E8" s="9" t="s">
         <v>549</v>
       </c>
@@ -2532,7 +2534,9 @@
       <c r="C11" s="35" t="s">
         <v>383</v>
       </c>
-      <c r="D11" s="46"/>
+      <c r="D11" s="52" t="s">
+        <v>552</v>
+      </c>
       <c r="E11" s="28" t="s">
         <v>453</v>
       </c>

</xml_diff>

<commit_message>
Added `X$`, which converts to `sym`
as suggested by @Sanchises
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Dropbox\MATL\spec\functionTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E403CBEB-CCE4-4490-9B5B-5A0C5B616BBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458CEA9F-0643-49AE-B0BE-554FCA1729B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="554">
   <si>
     <t>Normal function</t>
   </si>
@@ -1681,6 +1681,9 @@
   </si>
   <si>
     <t>execute Matlab function</t>
+  </si>
+  <si>
+    <t>sym / str2sym</t>
   </si>
 </sst>
 </file>
@@ -2353,7 +2356,7 @@
   <dimension ref="A1:L302"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12" customHeight="1"/>
@@ -2485,6 +2488,9 @@
       </c>
       <c r="C8" s="33" t="s">
         <v>188</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>553</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>549</v>

</xml_diff>

<commit_message>
`ZP` with 1 iput and output
gives a row vector with entries below the diagonal (like Matlabn's `squareform(···,'tovector')` but the input need not be a square, symmetric matrix
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Dropbox\MATL\spec\functionTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE704D66-65C1-42FA-8E1B-A17493B2FF38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9BC019-503B-4A19-8E9B-C8DEE716AFFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="555">
   <si>
     <t>Normal function</t>
   </si>
@@ -1684,6 +1684,9 @@
   </si>
   <si>
     <t>exp / Levenshtein distance</t>
+  </si>
+  <si>
+    <t>pdist2 / entries below diagonal</t>
   </si>
 </sst>
 </file>
@@ -2355,8 +2358,8 @@
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12" customHeight="1"/>
@@ -3177,8 +3180,8 @@
       <c r="E52" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="F52" s="28" t="s">
-        <v>237</v>
+      <c r="F52" s="52" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="12" customHeight="1">

</xml_diff>

<commit_message>
`Yf` with a vector of two numbers
divides each number by their gcd
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Dropbox\MATL\spec\functionTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9BC019-503B-4A19-8E9B-C8DEE716AFFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F333A510-8FD6-4E05-A269-A23CC30724DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -636,9 +636,6 @@
     <t>Not used. True (literal)</t>
   </si>
   <si>
-    <t>factor</t>
-  </si>
-  <si>
     <t>datestr</t>
   </si>
   <si>
@@ -1687,6 +1684,9 @@
   </si>
   <si>
     <t>pdist2 / entries below diagonal</t>
+  </si>
+  <si>
+    <t>factor / divide by gcd</t>
   </si>
 </sst>
 </file>
@@ -2358,8 +2358,8 @@
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12" customHeight="1"/>
@@ -2385,16 +2385,16 @@
         <v>0</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="12" customHeight="1">
@@ -2409,16 +2409,16 @@
         <v>172</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I3" s="21" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>250</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>251</v>
       </c>
       <c r="L3" s="23" t="s">
         <v>182</v>
@@ -2427,7 +2427,7 @@
     <row r="4" spans="1:12" ht="12" customHeight="1">
       <c r="B4" s="24"/>
       <c r="C4" s="25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -2438,7 +2438,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>89</v>
@@ -2461,10 +2461,10 @@
         <v>16</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -2476,13 +2476,13 @@
         <v>186</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="12" customHeight="1">
@@ -2493,13 +2493,13 @@
         <v>187</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="12" customHeight="1">
@@ -2510,13 +2510,13 @@
         <v>181</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="12" customHeight="1">
@@ -2524,16 +2524,16 @@
         <v>37</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>147</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="12" customHeight="1">
@@ -2541,16 +2541,16 @@
         <v>156</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="12" customHeight="1">
@@ -2558,16 +2558,16 @@
         <v>106</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12" customHeight="1">
@@ -2575,16 +2575,16 @@
         <v>107</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12" customHeight="1">
@@ -2601,7 +2601,7 @@
         <v>39</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="12" customHeight="1">
@@ -2616,7 +2616,7 @@
         <v>188</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12" customHeight="1">
@@ -2624,7 +2624,7 @@
         <v>100</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>46</v>
@@ -2647,7 +2647,7 @@
         <v>146</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F17" s="29"/>
     </row>
@@ -2665,7 +2665,7 @@
         <v>199</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="12" customHeight="1">
@@ -2676,13 +2676,13 @@
         <v>32</v>
       </c>
       <c r="D19" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="E19" s="52" t="s">
+        <v>536</v>
+      </c>
+      <c r="F19" s="28" t="s">
         <v>225</v>
-      </c>
-      <c r="E19" s="52" t="s">
-        <v>537</v>
-      </c>
-      <c r="F19" s="28" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="12" customHeight="1">
@@ -2693,10 +2693,10 @@
         <v>182</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F20" s="39"/>
     </row>
@@ -2708,10 +2708,10 @@
         <v>182</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F21" s="39"/>
     </row>
@@ -2723,10 +2723,10 @@
         <v>182</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F22" s="39"/>
     </row>
@@ -2738,10 +2738,10 @@
         <v>182</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F23" s="39"/>
     </row>
@@ -2753,10 +2753,10 @@
         <v>182</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F24" s="39"/>
     </row>
@@ -2768,10 +2768,10 @@
         <v>182</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F25" s="39"/>
     </row>
@@ -2783,10 +2783,10 @@
         <v>182</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F26" s="39"/>
     </row>
@@ -2798,7 +2798,7 @@
         <v>182</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E27" s="39"/>
       <c r="F27" s="39"/>
@@ -2811,7 +2811,7 @@
         <v>182</v>
       </c>
       <c r="D28" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E28" s="39"/>
       <c r="F28" s="39"/>
@@ -2824,7 +2824,7 @@
         <v>182</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="39"/>
@@ -2834,16 +2834,16 @@
         <v>167</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D30" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="E30" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="E30" s="37" t="s">
-        <v>209</v>
-      </c>
       <c r="F30" s="28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="12" customHeight="1">
@@ -2915,7 +2915,7 @@
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="28" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F35" s="28" t="s">
         <v>95</v>
@@ -2926,10 +2926,10 @@
         <v>102</v>
       </c>
       <c r="C36" s="53" t="s">
+        <v>529</v>
+      </c>
+      <c r="D36" s="53" t="s">
         <v>530</v>
-      </c>
-      <c r="D36" s="53" t="s">
-        <v>531</v>
       </c>
       <c r="E36" s="28" t="s">
         <v>84</v>
@@ -2946,13 +2946,13 @@
         <v>7</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E37" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="F37" s="28" t="s">
         <v>300</v>
-      </c>
-      <c r="F37" s="28" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="12" customHeight="1">
@@ -2960,16 +2960,16 @@
         <v>168</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D38" s="28" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="12" customHeight="1">
@@ -2979,10 +2979,10 @@
       <c r="C39" s="46"/>
       <c r="D39" s="46"/>
       <c r="E39" s="28" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="12" customHeight="1">
@@ -2990,13 +2990,13 @@
         <v>125</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F40" s="28" t="s">
         <v>18</v>
@@ -3007,10 +3007,10 @@
         <v>169</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="46"/>
@@ -3024,10 +3024,10 @@
       </c>
       <c r="D42" s="38"/>
       <c r="E42" s="28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F42" s="52" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="12" customHeight="1">
@@ -3035,16 +3035,16 @@
         <v>135</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D43" s="28" t="s">
         <v>97</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F43" s="36" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="12" customHeight="1">
@@ -3052,14 +3052,14 @@
         <v>122</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E44" s="46"/>
       <c r="F44" s="52" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="12" customHeight="1">
@@ -3067,16 +3067,16 @@
         <v>94</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F45" s="52" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="12" customHeight="1">
@@ -3084,10 +3084,10 @@
         <v>131</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E46" s="46"/>
       <c r="F46" s="46"/>
@@ -3097,10 +3097,10 @@
         <v>140</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D47" s="40" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E47" s="46"/>
       <c r="F47" s="46"/>
@@ -3110,13 +3110,13 @@
         <v>42</v>
       </c>
       <c r="C48" s="40" t="s">
+        <v>467</v>
+      </c>
+      <c r="D48" s="40" t="s">
         <v>468</v>
       </c>
-      <c r="D48" s="40" t="s">
-        <v>469</v>
-      </c>
       <c r="E48" s="28" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F48" s="46"/>
     </row>
@@ -3125,10 +3125,10 @@
         <v>11</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E49" s="29"/>
       <c r="F49" s="29"/>
@@ -3141,13 +3141,13 @@
         <v>201</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>200</v>
       </c>
       <c r="F50" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="2:6" ht="12" customHeight="1">
@@ -3155,16 +3155,16 @@
         <v>129</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D51" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="E51" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="E51" s="28" t="s">
+      <c r="F51" s="28" t="s">
         <v>206</v>
-      </c>
-      <c r="F51" s="28" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="52" spans="2:6" ht="12" customHeight="1">
@@ -3175,13 +3175,13 @@
         <v>70</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F52" s="52" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="12" customHeight="1">
@@ -3189,16 +3189,16 @@
         <v>118</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="12" customHeight="1">
@@ -3209,13 +3209,13 @@
         <v>41</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>40</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="12" customHeight="1">
@@ -3232,7 +3232,7 @@
         <v>193</v>
       </c>
       <c r="F55" s="52" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="12" customHeight="1">
@@ -3244,7 +3244,7 @@
       </c>
       <c r="D56" s="46"/>
       <c r="E56" s="36" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F56" s="38"/>
     </row>
@@ -3253,7 +3253,7 @@
         <v>43</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D57" s="28" t="s">
         <v>139</v>
@@ -3277,7 +3277,7 @@
         <v>143</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -3310,7 +3310,7 @@
         <v>91</v>
       </c>
       <c r="F61" s="36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="62" spans="2:6" ht="12" customHeight="1">
@@ -3329,7 +3329,7 @@
         <v>173</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D63" s="36" t="s">
         <v>13</v>
@@ -3345,13 +3345,13 @@
         <v>9</v>
       </c>
       <c r="D64" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E64" s="52" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F64" s="52" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="12" customHeight="1">
@@ -3359,7 +3359,7 @@
         <v>175</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D65" s="28" t="s">
         <v>12</v>
@@ -3378,10 +3378,10 @@
         <v>44</v>
       </c>
       <c r="E66" s="52" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="12" customHeight="1">
@@ -3389,7 +3389,7 @@
         <v>90</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
@@ -3400,16 +3400,16 @@
         <v>103</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E68" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="F68" s="28" t="s">
         <v>229</v>
-      </c>
-      <c r="F68" s="28" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="12" customHeight="1">
@@ -3420,13 +3420,13 @@
         <v>5</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="12" customHeight="1">
@@ -3438,7 +3438,7 @@
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F70" s="29"/>
     </row>
@@ -3447,7 +3447,7 @@
         <v>73</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D71" s="28" t="s">
         <v>3</v>
@@ -3456,7 +3456,7 @@
         <v>138</v>
       </c>
       <c r="F71" s="52" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="12" customHeight="1">
@@ -3467,13 +3467,13 @@
         <v>123</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E72" s="28" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F72" s="28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="12" customHeight="1">
@@ -3481,14 +3481,14 @@
         <v>176</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="52" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F73" s="52" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="74" spans="1:7" customFormat="1" ht="12" customHeight="1">
@@ -3502,8 +3502,8 @@
       <c r="D74" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="E74" s="28" t="s">
-        <v>204</v>
+      <c r="E74" s="52" t="s">
+        <v>554</v>
       </c>
       <c r="F74" s="29"/>
       <c r="G74" s="1"/>
@@ -3513,16 +3513,16 @@
         <v>128</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D75" s="28" t="s">
         <v>71</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="12" customHeight="1">
@@ -3533,13 +3533,13 @@
         <v>198</v>
       </c>
       <c r="D76" s="34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E76" s="28" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F76" s="28" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="12" customHeight="1">
@@ -3550,10 +3550,10 @@
         <v>92</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E77" s="28" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F77" s="46"/>
     </row>
@@ -3562,7 +3562,7 @@
         <v>177</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D78" s="28" t="s">
         <v>132</v>
@@ -3571,7 +3571,7 @@
         <v>133</v>
       </c>
       <c r="F78" s="52" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="12" customHeight="1">
@@ -3579,13 +3579,13 @@
         <v>116</v>
       </c>
       <c r="C79" s="28" t="s">
+        <v>485</v>
+      </c>
+      <c r="D79" s="28" t="s">
         <v>486</v>
       </c>
-      <c r="D79" s="28" t="s">
-        <v>487</v>
-      </c>
       <c r="E79" s="28" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F79" s="46"/>
     </row>
@@ -3594,13 +3594,13 @@
         <v>108</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E80" s="28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F80" s="28" t="s">
         <v>195</v>
@@ -3614,13 +3614,13 @@
         <v>124</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E81" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F81" s="28" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="82" spans="2:6" ht="12" customHeight="1">
@@ -3628,13 +3628,13 @@
         <v>64</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D82" s="28" t="s">
+        <v>505</v>
+      </c>
+      <c r="E82" s="28" t="s">
         <v>506</v>
-      </c>
-      <c r="E82" s="28" t="s">
-        <v>507</v>
       </c>
       <c r="F82" s="46"/>
     </row>
@@ -3643,13 +3643,13 @@
         <v>76</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>74</v>
       </c>
       <c r="E83" s="28" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F83" s="28" t="s">
         <v>151</v>
@@ -3663,13 +3663,13 @@
         <v>61</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E84" s="28" t="s">
         <v>63</v>
       </c>
       <c r="F84" s="28" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="85" spans="2:6" ht="12" customHeight="1">
@@ -3677,13 +3677,13 @@
         <v>117</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E85" s="28" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F85" s="28" t="s">
         <v>85</v>
@@ -3703,7 +3703,7 @@
         <v>79</v>
       </c>
       <c r="F86" s="52" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="87" spans="2:6" ht="12" customHeight="1">
@@ -3714,13 +3714,13 @@
         <v>59</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E87" s="28" t="s">
         <v>62</v>
       </c>
       <c r="F87" s="52" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="12" customHeight="1">
@@ -3728,12 +3728,12 @@
         <v>126</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D88" s="46"/>
       <c r="E88" s="46"/>
       <c r="F88" s="28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="89" spans="2:6" ht="12" customHeight="1">
@@ -3748,7 +3748,7 @@
       </c>
       <c r="E89" s="44"/>
       <c r="F89" s="28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="90" spans="2:6" ht="12" customHeight="1">
@@ -3760,10 +3760,10 @@
       </c>
       <c r="D90" s="46"/>
       <c r="E90" s="28" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F90" s="52" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="12" customHeight="1">
@@ -3795,7 +3795,7 @@
         <v>144</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D93" s="28" t="s">
         <v>60</v>
@@ -3812,10 +3812,10 @@
         <v>111</v>
       </c>
       <c r="C94" s="52" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E94" s="29"/>
       <c r="F94" s="29"/>
@@ -3825,7 +3825,7 @@
         <v>178</v>
       </c>
       <c r="C95" s="35" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D95" s="36" t="s">
         <v>137</v>
@@ -3834,7 +3834,7 @@
         <v>136</v>
       </c>
       <c r="F95" s="36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="96" spans="2:6" ht="12" customHeight="1">
@@ -3842,16 +3842,16 @@
         <v>38</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D96" s="28" t="s">
         <v>145</v>
       </c>
       <c r="E96" s="36" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F96" s="28" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="97" spans="2:6" ht="12" customHeight="1">
@@ -3859,12 +3859,12 @@
         <v>179</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D97" s="46"/>
       <c r="E97" s="46"/>
       <c r="F97" s="28" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="98" spans="2:6" ht="12" customHeight="1">
@@ -3881,7 +3881,7 @@
         <v>189</v>
       </c>
       <c r="F98" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="99" spans="2:6" ht="12" customHeight="1">
@@ -3942,10 +3942,10 @@
   <sheetData>
     <row r="1" spans="1:11" ht="13">
       <c r="A1" s="45" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="50" customFormat="1">
@@ -3956,29 +3956,29 @@
         <v>8</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="48" customFormat="1">
       <c r="A3" s="48" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="48" customFormat="1">
       <c r="A4" s="48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="48" customFormat="1">
@@ -3989,16 +3989,16 @@
         <v>168</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F5" s="48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G5" s="48" t="s">
         <v>200</v>
@@ -4007,7 +4007,7 @@
         <v>91</v>
       </c>
       <c r="I5" s="48" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J5" s="48" t="s">
         <v>61</v>
@@ -4015,90 +4015,90 @@
     </row>
     <row r="6" spans="1:11" s="48" customFormat="1">
       <c r="A6" s="48" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B6" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="48" customFormat="1">
       <c r="A7" s="48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B7" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="48" customFormat="1">
       <c r="A8" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B8" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="48" customFormat="1">
       <c r="A9" s="48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B9" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="48" customFormat="1">
       <c r="A10" s="48" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B10" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="48" customFormat="1">
       <c r="A11" s="48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B11" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="48" customFormat="1">
       <c r="A12" s="48" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B12" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="48" customFormat="1">
       <c r="A13" s="48" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B13" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K13" s="48" t="s">
         <v>27</v>
@@ -4106,35 +4106,35 @@
     </row>
     <row r="14" spans="1:11" s="48" customFormat="1">
       <c r="A14" s="48" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B14" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="48" customFormat="1">
       <c r="A15" s="48" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B15" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="48" customFormat="1">
       <c r="A16" s="48" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B16" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="48" customFormat="1">
@@ -4145,26 +4145,26 @@
         <v>168</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D17" s="48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="48" customFormat="1">
       <c r="A18" s="48" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B18" s="48" t="s">
         <v>113</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="48" customFormat="1">
       <c r="A19" s="48" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B19" s="48" t="s">
         <v>113</v>
@@ -4176,39 +4176,39 @@
         <v>54</v>
       </c>
       <c r="E19" s="48" t="s">
+        <v>222</v>
+      </c>
+      <c r="F19" s="48" t="s">
         <v>223</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="48" customFormat="1">
       <c r="A20" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B20" s="48" t="s">
         <v>168</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D20" s="48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E20" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="G20" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="H20" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="F20" s="48" t="s">
+      <c r="I20" s="48" t="s">
         <v>215</v>
-      </c>
-      <c r="G20" s="48" t="s">
-        <v>214</v>
-      </c>
-      <c r="H20" s="48" t="s">
-        <v>213</v>
-      </c>
-      <c r="I20" s="48" t="s">
-        <v>216</v>
       </c>
       <c r="K20" s="48" t="s">
         <v>27</v>
@@ -4216,31 +4216,31 @@
     </row>
     <row r="21" spans="1:11" s="48" customFormat="1">
       <c r="A21" s="48" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B21" s="48" t="s">
         <v>168</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E21" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="G21" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="H21" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="F21" s="48" t="s">
+      <c r="I21" s="48" t="s">
         <v>215</v>
-      </c>
-      <c r="G21" s="48" t="s">
-        <v>214</v>
-      </c>
-      <c r="H21" s="48" t="s">
-        <v>213</v>
-      </c>
-      <c r="I21" s="48" t="s">
-        <v>216</v>
       </c>
       <c r="K21" s="48" t="s">
         <v>27</v>
@@ -4254,25 +4254,25 @@
         <v>168</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D22" s="48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E22" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="F22" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="G22" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="H22" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="F22" s="48" t="s">
+      <c r="I22" s="48" t="s">
         <v>215</v>
-      </c>
-      <c r="G22" s="48" t="s">
-        <v>214</v>
-      </c>
-      <c r="H22" s="48" t="s">
-        <v>213</v>
-      </c>
-      <c r="I22" s="48" t="s">
-        <v>216</v>
       </c>
       <c r="K22" s="48" t="s">
         <v>27</v>
@@ -4280,31 +4280,31 @@
     </row>
     <row r="23" spans="1:11" s="48" customFormat="1">
       <c r="A23" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B23" s="48" t="s">
         <v>168</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D23" s="48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E23" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="F23" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="G23" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="H23" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="I23" s="48" t="s">
         <v>215</v>
-      </c>
-      <c r="G23" s="48" t="s">
-        <v>214</v>
-      </c>
-      <c r="H23" s="48" t="s">
-        <v>213</v>
-      </c>
-      <c r="I23" s="48" t="s">
-        <v>216</v>
       </c>
       <c r="K23" s="48" t="s">
         <v>27</v>
@@ -4312,19 +4312,19 @@
     </row>
     <row r="24" spans="1:11" s="48" customFormat="1">
       <c r="A24" s="48" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B24" s="48" t="s">
         <v>168</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E24" s="48" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F24" s="48" t="s">
         <v>200</v>
@@ -4347,10 +4347,10 @@
         <v>168</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K25" s="48" t="s">
         <v>27</v>
@@ -4358,13 +4358,13 @@
     </row>
     <row r="26" spans="1:11" s="48" customFormat="1">
       <c r="A26" s="48" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B26" s="48" t="s">
         <v>168</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D26" s="48" t="s">
         <v>61</v>
@@ -4372,7 +4372,7 @@
     </row>
     <row r="27" spans="1:11" s="48" customFormat="1">
       <c r="A27" s="48" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B27" s="48" t="s">
         <v>113</v>
@@ -4384,15 +4384,15 @@
         <v>54</v>
       </c>
       <c r="E27" s="48" t="s">
+        <v>222</v>
+      </c>
+      <c r="F27" s="48" t="s">
         <v>223</v>
-      </c>
-      <c r="F27" s="48" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="48" customFormat="1">
       <c r="A28" s="48" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B28" s="48" t="s">
         <v>113</v>
@@ -4403,13 +4403,13 @@
     </row>
     <row r="29" spans="1:11" s="48" customFormat="1">
       <c r="A29" s="48" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B29" s="48" t="s">
         <v>168</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E29" s="48" t="s">
         <v>200</v>
@@ -4420,31 +4420,31 @@
     </row>
     <row r="30" spans="1:11" s="48" customFormat="1">
       <c r="A30" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B30" s="48" t="s">
         <v>168</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E30" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="F30" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="G30" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="H30" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="F30" s="48" t="s">
+      <c r="I30" s="48" t="s">
         <v>215</v>
-      </c>
-      <c r="G30" s="48" t="s">
-        <v>214</v>
-      </c>
-      <c r="H30" s="48" t="s">
-        <v>213</v>
-      </c>
-      <c r="I30" s="48" t="s">
-        <v>216</v>
       </c>
       <c r="K30" s="48" t="s">
         <v>27</v>
@@ -4452,31 +4452,31 @@
     </row>
     <row r="31" spans="1:11" s="48" customFormat="1">
       <c r="A31" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B31" s="48" t="s">
         <v>168</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E31" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="F31" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="G31" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="H31" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="F31" s="48" t="s">
+      <c r="I31" s="48" t="s">
         <v>215</v>
-      </c>
-      <c r="G31" s="48" t="s">
-        <v>214</v>
-      </c>
-      <c r="H31" s="48" t="s">
-        <v>213</v>
-      </c>
-      <c r="I31" s="48" t="s">
-        <v>216</v>
       </c>
       <c r="K31" s="48" t="s">
         <v>27</v>
@@ -4484,34 +4484,34 @@
     </row>
     <row r="32" spans="1:11" s="48" customFormat="1">
       <c r="A32" s="48" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B32" s="48" t="s">
         <v>168</v>
       </c>
       <c r="C32" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E32" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="F32" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="G32" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="H32" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="F32" s="48" t="s">
+      <c r="I32" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="G32" s="48" t="s">
-        <v>214</v>
-      </c>
-      <c r="H32" s="48" t="s">
-        <v>213</v>
-      </c>
-      <c r="I32" s="48" t="s">
-        <v>216</v>
-      </c>
       <c r="J32" s="48" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K32" s="48" t="s">
         <v>27</v>
@@ -4519,31 +4519,31 @@
     </row>
     <row r="33" spans="1:11" s="48" customFormat="1">
       <c r="A33" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B33" s="48" t="s">
         <v>168</v>
       </c>
       <c r="C33" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E33" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="F33" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="G33" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="H33" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="F33" s="48" t="s">
+      <c r="I33" s="48" t="s">
         <v>215</v>
-      </c>
-      <c r="G33" s="48" t="s">
-        <v>214</v>
-      </c>
-      <c r="H33" s="48" t="s">
-        <v>213</v>
-      </c>
-      <c r="I33" s="48" t="s">
-        <v>216</v>
       </c>
       <c r="K33" s="48" t="s">
         <v>27</v>
@@ -4551,7 +4551,7 @@
     </row>
     <row r="34" spans="1:11" s="48" customFormat="1">
       <c r="A34" s="48" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B34" s="48" t="s">
         <v>4</v>
@@ -4562,7 +4562,7 @@
     </row>
     <row r="35" spans="1:11" s="48" customFormat="1">
       <c r="A35" s="48" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B35" s="48" t="s">
         <v>4</v>
@@ -4573,7 +4573,7 @@
     </row>
     <row r="36" spans="1:11" s="48" customFormat="1">
       <c r="A36" s="48" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B36" s="48" t="s">
         <v>4</v>
@@ -4584,7 +4584,7 @@
     </row>
     <row r="37" spans="1:11" s="48" customFormat="1">
       <c r="A37" s="48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B37" s="48" t="s">
         <v>4</v>
@@ -4595,7 +4595,7 @@
     </row>
     <row r="38" spans="1:11" s="48" customFormat="1">
       <c r="A38" s="48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B38" s="48" t="s">
         <v>4</v>
@@ -4606,7 +4606,7 @@
     </row>
     <row r="39" spans="1:11" s="48" customFormat="1">
       <c r="A39" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B39" s="48" t="s">
         <v>4</v>
@@ -4617,7 +4617,7 @@
     </row>
     <row r="40" spans="1:11" s="48" customFormat="1">
       <c r="A40" s="48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B40" s="48" t="s">
         <v>4</v>
@@ -4628,7 +4628,7 @@
     </row>
     <row r="41" spans="1:11" s="48" customFormat="1">
       <c r="A41" s="48" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B41" s="48" t="s">
         <v>4</v>
@@ -4639,7 +4639,7 @@
     </row>
     <row r="42" spans="1:11" s="48" customFormat="1">
       <c r="A42" s="48" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B42" s="48" t="s">
         <v>4</v>
@@ -4650,7 +4650,7 @@
     </row>
     <row r="43" spans="1:11" s="48" customFormat="1">
       <c r="A43" s="48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B43" s="48" t="s">
         <v>4</v>
@@ -4661,7 +4661,7 @@
     </row>
     <row r="44" spans="1:11" s="48" customFormat="1">
       <c r="A44" s="48" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B44" s="48" t="s">
         <v>4</v>
@@ -4672,7 +4672,7 @@
     </row>
     <row r="45" spans="1:11" s="48" customFormat="1">
       <c r="A45" s="48" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B45" s="48" t="s">
         <v>4</v>
@@ -4683,7 +4683,7 @@
     </row>
     <row r="46" spans="1:11" s="48" customFormat="1">
       <c r="A46" s="48" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B46" s="48" t="s">
         <v>4</v>
@@ -4694,7 +4694,7 @@
     </row>
     <row r="47" spans="1:11" s="48" customFormat="1">
       <c r="A47" s="48" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B47" s="48" t="s">
         <v>4</v>
@@ -4705,7 +4705,7 @@
     </row>
     <row r="48" spans="1:11" s="48" customFormat="1">
       <c r="A48" s="48" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B48" s="48" t="s">
         <v>4</v>
@@ -4727,7 +4727,7 @@
     </row>
     <row r="50" spans="1:11" s="48" customFormat="1">
       <c r="A50" s="48" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B50" s="48" t="s">
         <v>125</v>
@@ -4741,7 +4741,7 @@
     </row>
     <row r="51" spans="1:11" s="48" customFormat="1">
       <c r="A51" s="48" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B51" s="48" t="s">
         <v>19</v>
@@ -4752,7 +4752,7 @@
     </row>
     <row r="52" spans="1:11" s="48" customFormat="1">
       <c r="A52" s="48" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B52" s="48" t="s">
         <v>125</v>
@@ -4766,7 +4766,7 @@
     </row>
     <row r="53" spans="1:11" s="48" customFormat="1">
       <c r="A53" s="48" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B53" s="48" t="s">
         <v>125</v>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="54" spans="1:11" s="48" customFormat="1">
       <c r="A54" s="48" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B54" s="48" t="s">
         <v>125</v>
@@ -4786,7 +4786,7 @@
         <v>87</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K54" s="48" t="s">
         <v>27</v>
@@ -4794,7 +4794,7 @@
     </row>
     <row r="55" spans="1:11" s="48" customFormat="1">
       <c r="A55" s="48" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B55" s="48" t="s">
         <v>19</v>
@@ -4805,7 +4805,7 @@
     </row>
     <row r="56" spans="1:11" s="48" customFormat="1">
       <c r="A56" s="48" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B56" s="48" t="s">
         <v>125</v>
@@ -4819,7 +4819,7 @@
     </row>
     <row r="57" spans="1:11" s="48" customFormat="1">
       <c r="A57" s="48" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B57" s="48" t="s">
         <v>125</v>
@@ -4833,7 +4833,7 @@
     </row>
     <row r="58" spans="1:11" s="48" customFormat="1">
       <c r="A58" s="48" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B58" s="48" t="s">
         <v>125</v>
@@ -4844,7 +4844,7 @@
     </row>
     <row r="59" spans="1:11" s="48" customFormat="1">
       <c r="A59" s="48" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B59" s="48" t="s">
         <v>125</v>
@@ -4855,13 +4855,13 @@
     </row>
     <row r="60" spans="1:11" s="48" customFormat="1">
       <c r="A60" s="48" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B60" s="48" t="s">
         <v>169</v>
       </c>
       <c r="C60" s="48" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K60" s="48" t="s">
         <v>27</v>
@@ -4869,35 +4869,35 @@
     </row>
     <row r="61" spans="1:11" s="48" customFormat="1">
       <c r="A61" s="48" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B61" s="48" t="s">
         <v>169</v>
       </c>
       <c r="C61" s="48" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="48" customFormat="1">
       <c r="A62" s="48" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B62" s="48" t="s">
         <v>169</v>
       </c>
       <c r="C62" s="48" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="63" spans="1:11" s="48" customFormat="1">
       <c r="A63" s="48" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B63" s="48" t="s">
         <v>169</v>
       </c>
       <c r="C63" s="48" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K63" s="48" t="s">
         <v>27</v>
@@ -4905,110 +4905,110 @@
     </row>
     <row r="64" spans="1:11" s="48" customFormat="1">
       <c r="A64" s="48" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B64" s="48" t="s">
         <v>169</v>
       </c>
       <c r="C64" s="48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="65" spans="1:11" s="48" customFormat="1">
       <c r="A65" s="48" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B65" s="48" t="s">
         <v>169</v>
       </c>
       <c r="C65" s="48" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="66" spans="1:11" s="48" customFormat="1">
       <c r="A66" s="48" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B66" s="48" t="s">
         <v>169</v>
       </c>
       <c r="C66" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="48" customFormat="1">
       <c r="A67" s="48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B67" s="48" t="s">
         <v>110</v>
       </c>
       <c r="C67" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="D67" s="48" t="s">
         <v>236</v>
-      </c>
-      <c r="D67" s="48" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="68" spans="1:11" s="48" customFormat="1">
       <c r="A68" s="48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B68" s="48" t="s">
         <v>110</v>
       </c>
       <c r="C68" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="D68" s="48" t="s">
         <v>236</v>
-      </c>
-      <c r="D68" s="48" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="48" customFormat="1">
       <c r="A69" s="48" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B69" s="48" t="s">
         <v>110</v>
       </c>
       <c r="C69" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="D69" s="48" t="s">
         <v>236</v>
-      </c>
-      <c r="D69" s="48" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="48" customFormat="1">
       <c r="A70" s="48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B70" s="48" t="s">
         <v>110</v>
       </c>
       <c r="C70" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="D70" s="48" t="s">
         <v>236</v>
-      </c>
-      <c r="D70" s="48" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="71" spans="1:11" s="48" customFormat="1">
       <c r="A71" s="48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B71" s="48" t="s">
         <v>110</v>
       </c>
       <c r="C71" s="48" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D71" s="48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="72" spans="1:11" s="48" customFormat="1">
       <c r="A72" s="48" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B72" s="48" t="s">
         <v>15</v>
@@ -5019,16 +5019,16 @@
     </row>
     <row r="73" spans="1:11" s="48" customFormat="1">
       <c r="A73" s="48" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B73" s="48" t="s">
         <v>110</v>
       </c>
       <c r="C73" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="D73" s="48" t="s">
         <v>236</v>
-      </c>
-      <c r="D73" s="48" t="s">
-        <v>237</v>
       </c>
       <c r="K73" s="48" t="s">
         <v>27</v>
@@ -5036,105 +5036,105 @@
     </row>
     <row r="74" spans="1:11" s="48" customFormat="1">
       <c r="A74" s="48" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B74" s="48" t="s">
         <v>110</v>
       </c>
       <c r="C74" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="D74" s="48" t="s">
         <v>236</v>
-      </c>
-      <c r="D74" s="48" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="75" spans="1:11" s="48" customFormat="1">
       <c r="A75" s="48" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B75" s="48" t="s">
         <v>110</v>
       </c>
       <c r="C75" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="D75" s="48" t="s">
         <v>236</v>
-      </c>
-      <c r="D75" s="48" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="48" customFormat="1">
       <c r="A76" s="48" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B76" s="48" t="s">
         <v>110</v>
       </c>
       <c r="C76" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="D76" s="48" t="s">
         <v>236</v>
-      </c>
-      <c r="D76" s="48" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="48" customFormat="1">
       <c r="A77" s="48" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B77" s="48" t="s">
         <v>110</v>
       </c>
       <c r="C77" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="D77" s="48" t="s">
         <v>236</v>
-      </c>
-      <c r="D77" s="48" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="48" customFormat="1">
       <c r="A78" s="48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B78" s="48" t="s">
         <v>110</v>
       </c>
       <c r="C78" s="48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="48" customFormat="1">
       <c r="A79" s="48" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B79" s="48" t="s">
         <v>110</v>
       </c>
       <c r="C79" s="48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="80" spans="1:11" s="48" customFormat="1">
       <c r="A80" s="48" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B80" s="48" t="s">
         <v>110</v>
       </c>
       <c r="C80" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="D80" s="48" t="s">
         <v>236</v>
-      </c>
-      <c r="D80" s="48" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="81" spans="1:11" s="48" customFormat="1">
       <c r="A81" s="48" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B81" s="48" t="s">
         <v>135</v>
       </c>
       <c r="C81" s="48" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D81" s="48" t="s">
         <v>83</v>
@@ -5145,24 +5145,24 @@
     </row>
     <row r="82" spans="1:11" s="48" customFormat="1">
       <c r="A82" s="48" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B82" s="48" t="s">
         <v>128</v>
       </c>
       <c r="C82" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D82" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E82" s="48" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="83" spans="1:11" s="48" customFormat="1">
       <c r="A83" s="49" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B83" s="48" t="s">
         <v>135</v>
@@ -5174,27 +5174,27 @@
         <v>83</v>
       </c>
       <c r="K83" s="48" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="84" spans="1:11" s="48" customFormat="1">
       <c r="A84" s="48" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B84" s="48" t="s">
         <v>135</v>
       </c>
       <c r="C84" s="48" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D84" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="E84" s="48" t="s">
         <v>291</v>
       </c>
-      <c r="E84" s="48" t="s">
-        <v>292</v>
-      </c>
       <c r="F84" s="48" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G84" s="48" t="s">
         <v>152</v>
@@ -5202,7 +5202,7 @@
     </row>
     <row r="85" spans="1:11" s="48" customFormat="1">
       <c r="A85" s="48" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B85" s="48" t="s">
         <v>128</v>
@@ -5222,13 +5222,13 @@
     </row>
     <row r="86" spans="1:11" s="48" customFormat="1">
       <c r="A86" s="48" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B86" s="48" t="s">
         <v>135</v>
       </c>
       <c r="C86" s="48" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D86" s="48" t="s">
         <v>147</v>
@@ -5237,18 +5237,18 @@
         <v>146</v>
       </c>
       <c r="F86" s="48" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G86" s="48" t="s">
         <v>152</v>
       </c>
       <c r="K86" s="48" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="87" spans="1:11" s="48" customFormat="1">
       <c r="A87" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B87" s="48" t="s">
         <v>135</v>
@@ -5266,12 +5266,12 @@
         <v>152</v>
       </c>
       <c r="K87" s="48" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="88" spans="1:11" s="48" customFormat="1">
       <c r="A88" s="49" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B88" s="48" t="s">
         <v>135</v>
@@ -5289,12 +5289,12 @@
         <v>152</v>
       </c>
       <c r="K88" s="48" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="89" spans="1:11" s="47" customFormat="1">
       <c r="A89" s="47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B89" s="47" t="s">
         <v>122</v>
@@ -5311,7 +5311,7 @@
     </row>
     <row r="90" spans="1:11" s="48" customFormat="1">
       <c r="A90" s="48" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B90" s="48" t="s">
         <v>94</v>
@@ -5325,12 +5325,12 @@
         <v>131</v>
       </c>
       <c r="C91" s="48" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="92" spans="1:11" s="48" customFormat="1">
       <c r="A92" s="48" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B92" s="48" t="s">
         <v>131</v>
@@ -5344,7 +5344,7 @@
     </row>
     <row r="93" spans="1:11" s="48" customFormat="1">
       <c r="A93" s="49" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B93" s="48" t="s">
         <v>131</v>
@@ -5353,29 +5353,29 @@
         <v>130</v>
       </c>
       <c r="K93" s="48" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="94" spans="1:11" s="48" customFormat="1">
       <c r="A94" s="48" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B94" s="48" t="s">
         <v>140</v>
       </c>
       <c r="C94" s="48" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:11" s="48" customFormat="1">
       <c r="A95" s="48" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B95" s="48" t="s">
         <v>140</v>
       </c>
       <c r="C95" s="48" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="96" spans="1:11" s="50" customFormat="1">
@@ -5386,32 +5386,32 @@
         <v>140</v>
       </c>
       <c r="C96" s="50" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="48" customFormat="1">
       <c r="A97" s="48" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B97" s="48" t="s">
         <v>140</v>
       </c>
       <c r="C97" s="48" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="48" customFormat="1">
       <c r="A98" s="48" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B98" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C98" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D98" s="48" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E98" s="48" t="s">
         <v>61</v>
@@ -5419,272 +5419,272 @@
     </row>
     <row r="99" spans="1:5" s="48" customFormat="1">
       <c r="A99" s="48" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B99" s="48" t="s">
         <v>42</v>
       </c>
       <c r="C99" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="48" customFormat="1">
       <c r="A100" s="48" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B100" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C100" s="48" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="48" customFormat="1">
       <c r="A101" s="48" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B101" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C101" s="48" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C102" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C103" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C104" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C105" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C106" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C107" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C108" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B109" t="s">
         <v>140</v>
       </c>
       <c r="C109" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B110" t="s">
         <v>140</v>
       </c>
       <c r="C110" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B111" t="s">
         <v>140</v>
       </c>
       <c r="C111" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B112" t="s">
         <v>140</v>
       </c>
       <c r="C112" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B113" t="s">
         <v>140</v>
       </c>
       <c r="C113" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B114" t="s">
         <v>140</v>
       </c>
       <c r="C114" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B115" t="s">
         <v>140</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B116" t="s">
         <v>140</v>
       </c>
       <c r="C116" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B117" t="s">
         <v>141</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B118" t="s">
         <v>141</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B119" t="s">
         <v>141</v>
       </c>
       <c r="C119" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B120" t="s">
         <v>141</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B121" t="s">
         <v>141</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B122" t="s">
         <v>141</v>
       </c>
       <c r="C122" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B123" t="s">
         <v>141</v>
       </c>
       <c r="C123" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B124" t="s">
         <v>141</v>
       </c>
       <c r="C124" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B125" t="s">
         <v>141</v>
@@ -5695,194 +5695,194 @@
     </row>
     <row r="126" spans="1:3" s="48" customFormat="1">
       <c r="A126" s="48" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B126" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C126" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="127" spans="1:3" s="48" customFormat="1">
       <c r="A127" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B127" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C127" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="128" spans="1:3" s="48" customFormat="1">
       <c r="A128" s="48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B128" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C128" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="129" spans="1:3" s="48" customFormat="1">
       <c r="A129" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B129" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C129" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="130" spans="1:3" s="48" customFormat="1">
       <c r="A130" s="48" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B130" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C130" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="131" spans="1:3" s="48" customFormat="1">
       <c r="A131" s="48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B131" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C131" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="132" spans="1:3" s="48" customFormat="1">
       <c r="A132" s="48" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B132" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C132" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="133" spans="1:3" s="48" customFormat="1">
       <c r="A133" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B133" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C133" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="134" spans="1:3" s="48" customFormat="1">
       <c r="A134" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B134" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C134" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="135" spans="1:3" s="48" customFormat="1">
       <c r="A135" s="48" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B135" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C135" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="136" spans="1:3" s="48" customFormat="1">
       <c r="A136" s="48" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B136" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C136" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="137" spans="1:3" s="48" customFormat="1">
       <c r="A137" s="48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B137" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C137" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="138" spans="1:3" s="48" customFormat="1">
       <c r="A138" s="48" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B138" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C138" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="139" spans="1:3" s="48" customFormat="1">
       <c r="A139" s="48" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B139" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C139" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="140" spans="1:3" s="48" customFormat="1">
       <c r="A140" s="48" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B140" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C140" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="141" spans="1:3" s="48" customFormat="1">
       <c r="A141" s="48" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B141" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C141" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="142" spans="1:3" s="48" customFormat="1">
       <c r="A142" s="48" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B142" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C142" s="48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="48" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B143" s="48" t="s">
         <v>129</v>
@@ -5890,7 +5890,7 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="48" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B144" s="48" t="s">
         <v>177</v>
@@ -5919,7 +5919,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5929,20 +5929,20 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B8" t="s">
         <v>376</v>
-      </c>
-      <c r="B8" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
`Zv` with two inputs now allows the first to be `logical`
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Dropbox\MATL\spec\functionTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F333A510-8FD6-4E05-A269-A23CC30724DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3DD30F-B4E4-4F23-9C16-B4C927D13290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2358,8 +2358,8 @@
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12" customHeight="1"/>
@@ -3057,10 +3057,10 @@
       <c r="D44" s="40" t="s">
         <v>242</v>
       </c>
-      <c r="E44" s="46"/>
-      <c r="F44" s="52" t="s">
+      <c r="E44" s="52" t="s">
         <v>548</v>
       </c>
+      <c r="F44" s="46"/>
     </row>
     <row r="45" spans="2:6" ht="12" customHeight="1">
       <c r="B45" s="27" t="s">

</xml_diff>

<commit_message>
Corrected Matlab function name
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Dropbox\MATL\spec\functionTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995E3B91-BDFC-4B0F-A024-F31FDD730C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41374E0-C4EB-49A7-94F2-3AA31F519EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1626,9 +1626,6 @@
     <t>std / cov / skewness / kurtosis</t>
   </si>
   <si>
-    <t>fft, nfft</t>
-  </si>
-  <si>
     <t>matrix power, or sum of matrix powers</t>
   </si>
   <si>
@@ -1690,6 +1687,9 @@
   </si>
   <si>
     <t>symbolic-specific functions</t>
+  </si>
+  <si>
+    <t>fft, fftn</t>
   </si>
 </sst>
 </file>
@@ -2361,8 +2361,8 @@
   </sheetPr>
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F98" sqref="B3:F98"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12" customHeight="1"/>
@@ -2496,10 +2496,10 @@
         <v>187</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F8" s="43" t="s">
         <v>253</v>
@@ -2547,7 +2547,7 @@
         <v>381</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E11" s="28" t="s">
         <v>451</v>
@@ -2561,16 +2561,16 @@
         <v>106</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D12" s="37" t="s">
         <v>481</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12" customHeight="1">
@@ -2578,16 +2578,16 @@
         <v>107</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D13" s="37" t="s">
         <v>482</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12" customHeight="1">
@@ -2682,7 +2682,7 @@
         <v>224</v>
       </c>
       <c r="E19" s="52" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F19" s="28" t="s">
         <v>225</v>
@@ -3030,7 +3030,7 @@
         <v>513</v>
       </c>
       <c r="F42" s="52" t="s">
-        <v>534</v>
+        <v>555</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="12" customHeight="1">
@@ -3061,7 +3061,7 @@
         <v>242</v>
       </c>
       <c r="E44" s="52" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F44" s="46"/>
     </row>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="E46" s="46"/>
       <c r="F46" s="52" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="12" customHeight="1">
@@ -3186,7 +3186,7 @@
         <v>392</v>
       </c>
       <c r="F52" s="52" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="12" customHeight="1">
@@ -3237,7 +3237,7 @@
         <v>193</v>
       </c>
       <c r="F55" s="52" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="12" customHeight="1">
@@ -3353,7 +3353,7 @@
         <v>230</v>
       </c>
       <c r="E64" s="52" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F64" s="52" t="s">
         <v>521</v>
@@ -3383,7 +3383,7 @@
         <v>44</v>
       </c>
       <c r="E66" s="52" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F66" s="28" t="s">
         <v>512</v>
@@ -3490,10 +3490,10 @@
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="52" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F73" s="52" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="74" spans="1:7" customFormat="1" ht="12" customHeight="1">
@@ -3508,7 +3508,7 @@
         <v>150</v>
       </c>
       <c r="E74" s="52" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F74" s="29"/>
       <c r="G74" s="1"/>
@@ -3708,7 +3708,7 @@
         <v>79</v>
       </c>
       <c r="F86" s="52" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="87" spans="2:6" ht="12" customHeight="1">
@@ -3817,7 +3817,7 @@
         <v>111</v>
       </c>
       <c r="C94" s="52" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D94" s="28" t="s">
         <v>501</v>

</xml_diff>

<commit_message>
Added `ZE`: `ifftn` and `ifft`
</commit_message>
<xml_diff>
--- a/spec/functionTable/MATL.xlsx
+++ b/spec/functionTable/MATL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Dropbox\MATL\spec\functionTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41374E0-C4EB-49A7-94F2-3AA31F519EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1456A48-DA49-4273-A842-7CA41FDD0686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="557">
   <si>
     <t>Normal function</t>
   </si>
@@ -1690,6 +1690,9 @@
   </si>
   <si>
     <t>fft, fftn</t>
+  </si>
+  <si>
+    <t>ifft, ifftn</t>
   </si>
 </sst>
 </file>
@@ -2362,7 +2365,7 @@
   <dimension ref="A1:L302"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12" customHeight="1"/>
@@ -3016,7 +3019,9 @@
         <v>484</v>
       </c>
       <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
+      <c r="F41" s="52" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="42" spans="2:6" ht="12" customHeight="1">
       <c r="B42" s="27" t="s">

</xml_diff>